<commit_message>
Add one more matched term
</commit_message>
<xml_diff>
--- a/doc/mapping results/termsMapping.xlsx
+++ b/doc/mapping results/termsMapping.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr date1904="1"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="-15" windowWidth="12615" windowHeight="11760" tabRatio="548" activeTab="1"/>
+    <workbookView xWindow="-15" yWindow="-15" windowWidth="12615" windowHeight="11760" tabRatio="548" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="terms2ignore" sheetId="2" r:id="rId1"/>
@@ -14,12 +14,12 @@
     <sheet name="Summary of Subset" sheetId="6" r:id="rId5"/>
     <sheet name="Summary of Mapping" sheetId="7" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5192" uniqueCount="3291">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5192" uniqueCount="3292">
   <si>
     <t>MO URI</t>
   </si>
@@ -9897,6 +9897,9 @@
   </si>
   <si>
     <t>high molecular weight DNA extract</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/CL_0002351</t>
   </si>
 </sst>
 </file>
@@ -10084,12 +10087,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -10104,10 +10101,16 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="超链接" xfId="1" builtinId="8"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -11784,7 +11787,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H660"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+    <sheetView topLeftCell="D1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A377" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="F388" sqref="F388"/>
     </sheetView>
@@ -19466,7 +19469,7 @@
       <c r="C388" s="11" t="s">
         <v>393</v>
       </c>
-      <c r="D388" s="27" t="s">
+      <c r="D388" s="25" t="s">
         <v>692</v>
       </c>
       <c r="E388" t="s">
@@ -24649,8 +24652,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H197"/>
   <sheetViews>
-    <sheetView topLeftCell="C41" workbookViewId="0">
-      <selection activeCell="D51" sqref="D51"/>
+    <sheetView tabSelected="1" topLeftCell="C127" workbookViewId="0">
+      <selection activeCell="D104" sqref="D104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -24658,7 +24661,7 @@
     <col min="2" max="2" width="16.75" customWidth="1"/>
     <col min="3" max="3" width="24.75" customWidth="1"/>
     <col min="4" max="4" width="49.25" customWidth="1"/>
-    <col min="5" max="5" width="21.625" customWidth="1"/>
+    <col min="5" max="5" width="35.875" customWidth="1"/>
     <col min="6" max="6" width="18.875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -25337,6 +25340,9 @@
       <c r="D50" t="s">
         <v>404</v>
       </c>
+      <c r="E50" s="1" t="s">
+        <v>3291</v>
+      </c>
       <c r="G50" t="s">
         <v>405</v>
       </c>
@@ -27232,8 +27238,10 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="F197" r:id="rId1"/>
+    <hyperlink ref="E50" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="0" r:id="rId3"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
@@ -27714,7 +27722,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I44"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
@@ -27754,7 +27762,7 @@
       <c r="A2" s="18" t="s">
         <v>3193</v>
       </c>
-      <c r="B2" s="20">
+      <c r="B2" s="26">
         <v>198</v>
       </c>
       <c r="C2" s="18">
@@ -27772,7 +27780,7 @@
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="18"/>
-      <c r="B3" s="20"/>
+      <c r="B3" s="26"/>
       <c r="C3" s="18">
         <v>450</v>
       </c>
@@ -27793,7 +27801,7 @@
       <c r="A4" s="18" t="s">
         <v>3196</v>
       </c>
-      <c r="B4" s="20">
+      <c r="B4" s="26">
         <v>46</v>
       </c>
       <c r="C4" s="18">
@@ -27811,7 +27819,7 @@
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="18"/>
-      <c r="B5" s="20"/>
+      <c r="B5" s="26"/>
       <c r="C5" s="18">
         <v>309</v>
       </c>
@@ -27924,7 +27932,7 @@
       <c r="A10" s="18" t="s">
         <v>3214</v>
       </c>
-      <c r="B10" s="20">
+      <c r="B10" s="26">
         <v>33</v>
       </c>
       <c r="C10" s="18">
@@ -27942,7 +27950,7 @@
     </row>
     <row r="11" spans="1:8">
       <c r="A11" s="18"/>
-      <c r="B11" s="20"/>
+      <c r="B11" s="26"/>
       <c r="C11" s="18">
         <v>70</v>
       </c>
@@ -27963,7 +27971,7 @@
       <c r="A12" s="19" t="s">
         <v>3253</v>
       </c>
-      <c r="B12" s="21">
+      <c r="B12" s="27">
         <v>11</v>
       </c>
       <c r="C12" s="19">
@@ -27984,7 +27992,7 @@
     </row>
     <row r="13" spans="1:8">
       <c r="A13" s="18"/>
-      <c r="B13" s="21"/>
+      <c r="B13" s="27"/>
       <c r="C13" s="19">
         <v>333</v>
       </c>
@@ -28005,7 +28013,7 @@
       <c r="A14" s="19" t="s">
         <v>3205</v>
       </c>
-      <c r="B14" s="21">
+      <c r="B14" s="27">
         <v>141</v>
       </c>
       <c r="C14" s="19">
@@ -28026,7 +28034,7 @@
     </row>
     <row r="15" spans="1:8">
       <c r="A15" s="18"/>
-      <c r="B15" s="21"/>
+      <c r="B15" s="27"/>
       <c r="C15" s="18">
         <v>1206</v>
       </c>
@@ -28050,13 +28058,13 @@
       <c r="B16">
         <v>14</v>
       </c>
-      <c r="C16" s="22">
+      <c r="C16" s="20">
         <v>62</v>
       </c>
-      <c r="D16" s="22">
+      <c r="D16" s="20">
         <v>0</v>
       </c>
-      <c r="E16" s="22">
+      <c r="E16" s="20">
         <v>99</v>
       </c>
       <c r="F16" s="18" t="s">
@@ -28064,28 +28072,28 @@
       </c>
     </row>
     <row r="23" spans="1:9" ht="31.5">
-      <c r="A23" s="23" t="s">
+      <c r="A23" s="21" t="s">
         <v>3199</v>
       </c>
-      <c r="B23" s="23" t="s">
+      <c r="B23" s="21" t="s">
         <v>3200</v>
       </c>
-      <c r="C23" s="24" t="s">
+      <c r="C23" s="22" t="s">
         <v>3259</v>
       </c>
-      <c r="D23" s="24" t="s">
+      <c r="D23" s="22" t="s">
         <v>3260</v>
       </c>
-      <c r="E23" s="24" t="s">
+      <c r="E23" s="22" t="s">
         <v>3261</v>
       </c>
-      <c r="F23" s="24" t="s">
+      <c r="F23" s="22" t="s">
         <v>3262</v>
       </c>
-      <c r="G23" s="24" t="s">
+      <c r="G23" s="22" t="s">
         <v>3263</v>
       </c>
-      <c r="H23" s="24" t="s">
+      <c r="H23" s="22" t="s">
         <v>3264</v>
       </c>
     </row>
@@ -28093,7 +28101,7 @@
       <c r="A24" t="s">
         <v>3193</v>
       </c>
-      <c r="B24" s="25" t="s">
+      <c r="B24" s="23" t="s">
         <v>3273</v>
       </c>
       <c r="C24">
@@ -28119,7 +28127,7 @@
       <c r="A25" t="s">
         <v>3212</v>
       </c>
-      <c r="B25" s="25" t="s">
+      <c r="B25" s="23" t="s">
         <v>3272</v>
       </c>
       <c r="D25">
@@ -28145,7 +28153,7 @@
       <c r="A26" t="s">
         <v>3205</v>
       </c>
-      <c r="B26" s="25" t="s">
+      <c r="B26" s="23" t="s">
         <v>3206</v>
       </c>
       <c r="C26">
@@ -28171,7 +28179,7 @@
       <c r="A27" t="s">
         <v>3214</v>
       </c>
-      <c r="B27" s="25" t="s">
+      <c r="B27" s="23" t="s">
         <v>3274</v>
       </c>
       <c r="C27">
@@ -28194,7 +28202,7 @@
       <c r="A28" t="s">
         <v>3208</v>
       </c>
-      <c r="B28" s="25" t="s">
+      <c r="B28" s="23" t="s">
         <v>3209</v>
       </c>
       <c r="C28">
@@ -28220,7 +28228,7 @@
       <c r="A29" t="s">
         <v>3218</v>
       </c>
-      <c r="B29" s="25" t="s">
+      <c r="B29" s="23" t="s">
         <v>3275</v>
       </c>
       <c r="C29">
@@ -28243,7 +28251,7 @@
       <c r="A30" t="s">
         <v>3222</v>
       </c>
-      <c r="B30" s="25" t="s">
+      <c r="B30" s="23" t="s">
         <v>3223</v>
       </c>
       <c r="D30">
@@ -28266,7 +28274,7 @@
       <c r="A31" t="s">
         <v>3224</v>
       </c>
-      <c r="B31" s="25" t="s">
+      <c r="B31" s="23" t="s">
         <v>3276</v>
       </c>
       <c r="C31">
@@ -28283,7 +28291,7 @@
       <c r="A32" t="s">
         <v>3239</v>
       </c>
-      <c r="B32" s="25"/>
+      <c r="B32" s="23"/>
       <c r="D32">
         <v>0</v>
       </c>
@@ -28298,25 +28306,25 @@
       </c>
     </row>
     <row r="33" spans="1:2">
-      <c r="B33" s="25"/>
+      <c r="B33" s="23"/>
     </row>
     <row r="34" spans="1:2">
-      <c r="B34" s="25"/>
+      <c r="B34" s="23"/>
     </row>
     <row r="35" spans="1:2">
-      <c r="B35" s="25"/>
+      <c r="B35" s="23"/>
     </row>
     <row r="36" spans="1:2">
-      <c r="B36" s="25"/>
+      <c r="B36" s="23"/>
     </row>
     <row r="37" spans="1:2">
-      <c r="B37" s="25"/>
+      <c r="B37" s="23"/>
     </row>
     <row r="39" spans="1:2">
       <c r="A39" t="s">
         <v>3286</v>
       </c>
-      <c r="B39" s="26" t="s">
+      <c r="B39" s="24" t="s">
         <v>3287</v>
       </c>
     </row>
@@ -28375,10 +28383,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E55"/>
+  <dimension ref="A1:E54"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E9"/>
+      <selection activeCell="A10" sqref="A10:XFD10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -28530,40 +28538,43 @@
     </row>
     <row r="10" spans="1:5">
       <c r="A10" t="s">
-        <v>3227</v>
+        <v>3228</v>
       </c>
       <c r="B10" s="13"/>
       <c r="C10">
         <v>2</v>
       </c>
+      <c r="D10" t="s">
+        <v>3229</v>
+      </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" t="s">
-        <v>3228</v>
+        <v>3230</v>
       </c>
       <c r="B11" s="13"/>
       <c r="C11">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D11" t="s">
-        <v>3229</v>
+        <v>750</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" t="s">
-        <v>3230</v>
+        <v>3231</v>
       </c>
       <c r="B12" s="13"/>
       <c r="C12">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D12" t="s">
-        <v>750</v>
+        <v>3216</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" t="s">
-        <v>3231</v>
+        <v>3232</v>
       </c>
       <c r="B13" s="13"/>
       <c r="C13">
@@ -28575,64 +28586,64 @@
     </row>
     <row r="14" spans="1:5">
       <c r="A14" t="s">
-        <v>3232</v>
+        <v>3233</v>
       </c>
       <c r="B14" s="13"/>
       <c r="C14">
-        <v>2</v>
-      </c>
-      <c r="D14" t="s">
-        <v>3216</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" t="s">
-        <v>3233</v>
+        <v>3234</v>
       </c>
       <c r="B15" s="13"/>
       <c r="C15">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="D15" t="s">
+        <v>3235</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" t="s">
-        <v>3234</v>
+        <v>3236</v>
       </c>
       <c r="B16" s="13"/>
       <c r="C16">
         <v>1</v>
       </c>
       <c r="D16" t="s">
-        <v>3235</v>
+        <v>3216</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" t="s">
-        <v>3236</v>
+        <v>3237</v>
       </c>
       <c r="B17" s="13"/>
       <c r="C17">
         <v>1</v>
       </c>
       <c r="D17" t="s">
-        <v>3216</v>
+        <v>3238</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" t="s">
-        <v>3237</v>
+        <v>3239</v>
       </c>
       <c r="B18" s="13"/>
       <c r="C18">
         <v>1</v>
       </c>
       <c r="D18" t="s">
-        <v>3238</v>
+        <v>3216</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" t="s">
-        <v>3239</v>
+        <v>3240</v>
       </c>
       <c r="B19" s="13"/>
       <c r="C19">
@@ -28644,203 +28655,202 @@
     </row>
     <row r="20" spans="1:4">
       <c r="A20" t="s">
-        <v>3240</v>
+        <v>3241</v>
       </c>
       <c r="B20" s="13"/>
       <c r="C20">
         <v>1</v>
       </c>
       <c r="D20" t="s">
-        <v>3216</v>
+        <v>3242</v>
       </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" t="s">
-        <v>3241</v>
+        <v>3243</v>
       </c>
       <c r="B21" s="13"/>
       <c r="C21">
         <v>1</v>
       </c>
       <c r="D21" t="s">
-        <v>3242</v>
+        <v>2170</v>
       </c>
     </row>
     <row r="22" spans="1:4">
       <c r="A22" t="s">
-        <v>3243</v>
+        <v>3244</v>
       </c>
       <c r="B22" s="13"/>
       <c r="C22">
         <v>1</v>
       </c>
       <c r="D22" t="s">
-        <v>2170</v>
+        <v>1908</v>
       </c>
     </row>
     <row r="23" spans="1:4">
-      <c r="A23" t="s">
-        <v>3244</v>
-      </c>
-      <c r="B23" s="13"/>
       <c r="C23">
-        <v>1</v>
-      </c>
-      <c r="D23" t="s">
-        <v>1908</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4">
-      <c r="C24">
-        <f>SUM(C2:C23)</f>
-        <v>497</v>
+        <f>SUM(C2:C22)</f>
+        <v>494</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26" t="s">
+        <v>3245</v>
+      </c>
+      <c r="C26">
+        <v>63</v>
+      </c>
+      <c r="D26" t="s">
+        <v>3246</v>
       </c>
     </row>
     <row r="27" spans="1:4">
       <c r="A27" t="s">
-        <v>3245</v>
+        <v>3247</v>
       </c>
       <c r="C27">
-        <v>63</v>
+        <v>2</v>
       </c>
       <c r="D27" t="s">
-        <v>3246</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4">
-      <c r="A28" t="s">
-        <v>3247</v>
-      </c>
-      <c r="C28">
-        <v>2</v>
-      </c>
-      <c r="D28" t="s">
         <v>3248</v>
       </c>
     </row>
+    <row r="32" spans="1:4">
+      <c r="A32" s="14" t="s">
+        <v>3199</v>
+      </c>
+      <c r="B32" s="14" t="s">
+        <v>3201</v>
+      </c>
+      <c r="C32" s="14" t="s">
+        <v>818</v>
+      </c>
+    </row>
     <row r="33" spans="1:3">
-      <c r="A33" s="14" t="s">
-        <v>3199</v>
-      </c>
-      <c r="B33" s="14" t="s">
-        <v>3201</v>
-      </c>
-      <c r="C33" s="14" t="s">
-        <v>818</v>
-      </c>
+      <c r="A33" s="15" t="s">
+        <v>3193</v>
+      </c>
+      <c r="B33" s="15">
+        <v>199</v>
+      </c>
+      <c r="C33" s="15"/>
     </row>
     <row r="34" spans="1:3">
-      <c r="A34" s="15" t="s">
-        <v>3193</v>
-      </c>
-      <c r="B34" s="15">
-        <v>199</v>
-      </c>
-      <c r="C34" s="15"/>
+      <c r="A34" s="16" t="s">
+        <v>3205</v>
+      </c>
+      <c r="B34" s="16">
+        <v>126</v>
+      </c>
+      <c r="C34" s="16"/>
     </row>
     <row r="35" spans="1:3">
       <c r="A35" s="16" t="s">
-        <v>3205</v>
+        <v>3208</v>
       </c>
       <c r="B35" s="16">
-        <v>126</v>
-      </c>
-      <c r="C35" s="16"/>
+        <v>66</v>
+      </c>
+      <c r="C35" s="16" t="s">
+        <v>3210</v>
+      </c>
     </row>
     <row r="36" spans="1:3">
       <c r="A36" s="16" t="s">
-        <v>3208</v>
+        <v>3212</v>
       </c>
       <c r="B36" s="16">
-        <v>66</v>
-      </c>
-      <c r="C36" s="16" t="s">
-        <v>3210</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="C36" s="16"/>
     </row>
     <row r="37" spans="1:3">
       <c r="A37" s="16" t="s">
-        <v>3212</v>
+        <v>3214</v>
       </c>
       <c r="B37" s="16">
-        <v>45</v>
-      </c>
-      <c r="C37" s="16"/>
+        <v>19</v>
+      </c>
+      <c r="C37" s="16" t="s">
+        <v>3216</v>
+      </c>
     </row>
     <row r="38" spans="1:3">
       <c r="A38" s="16" t="s">
-        <v>3214</v>
+        <v>3218</v>
       </c>
       <c r="B38" s="16">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="C38" s="16" t="s">
-        <v>3216</v>
+        <v>3220</v>
       </c>
     </row>
     <row r="39" spans="1:3">
       <c r="A39" s="16" t="s">
-        <v>3218</v>
+        <v>3222</v>
       </c>
       <c r="B39" s="16">
-        <v>12</v>
-      </c>
-      <c r="C39" s="16" t="s">
-        <v>3220</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="C39" s="16"/>
     </row>
     <row r="40" spans="1:3">
       <c r="A40" s="16" t="s">
-        <v>3222</v>
+        <v>3224</v>
       </c>
       <c r="B40" s="16">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="C40" s="16"/>
     </row>
     <row r="41" spans="1:3">
       <c r="A41" s="16" t="s">
-        <v>3224</v>
+        <v>3227</v>
       </c>
       <c r="B41" s="16">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C41" s="16"/>
     </row>
     <row r="42" spans="1:3">
       <c r="A42" s="16" t="s">
-        <v>3227</v>
+        <v>3228</v>
       </c>
       <c r="B42" s="16">
         <v>2</v>
       </c>
-      <c r="C42" s="16"/>
+      <c r="C42" s="16" t="s">
+        <v>3229</v>
+      </c>
     </row>
     <row r="43" spans="1:3">
       <c r="A43" s="16" t="s">
-        <v>3228</v>
+        <v>3230</v>
       </c>
       <c r="B43" s="16">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C43" s="16" t="s">
-        <v>3229</v>
+        <v>750</v>
       </c>
     </row>
     <row r="44" spans="1:3">
       <c r="A44" s="16" t="s">
-        <v>3230</v>
+        <v>3231</v>
       </c>
       <c r="B44" s="16">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C44" s="16" t="s">
-        <v>750</v>
+        <v>3216</v>
       </c>
     </row>
     <row r="45" spans="1:3">
       <c r="A45" s="16" t="s">
-        <v>3231</v>
+        <v>3232</v>
       </c>
       <c r="B45" s="16">
         <v>2</v>
@@ -28851,60 +28861,60 @@
     </row>
     <row r="46" spans="1:3">
       <c r="A46" s="16" t="s">
-        <v>3232</v>
+        <v>3233</v>
       </c>
       <c r="B46" s="16">
         <v>2</v>
       </c>
-      <c r="C46" s="16" t="s">
-        <v>3216</v>
-      </c>
+      <c r="C46" s="16"/>
     </row>
     <row r="47" spans="1:3">
       <c r="A47" s="16" t="s">
-        <v>3233</v>
+        <v>3234</v>
       </c>
       <c r="B47" s="16">
-        <v>2</v>
-      </c>
-      <c r="C47" s="16"/>
+        <v>1</v>
+      </c>
+      <c r="C47" s="16" t="s">
+        <v>3235</v>
+      </c>
     </row>
     <row r="48" spans="1:3">
       <c r="A48" s="16" t="s">
-        <v>3234</v>
+        <v>3236</v>
       </c>
       <c r="B48" s="16">
         <v>1</v>
       </c>
       <c r="C48" s="16" t="s">
-        <v>3235</v>
+        <v>3216</v>
       </c>
     </row>
     <row r="49" spans="1:3">
       <c r="A49" s="16" t="s">
-        <v>3236</v>
+        <v>3237</v>
       </c>
       <c r="B49" s="16">
         <v>1</v>
       </c>
       <c r="C49" s="16" t="s">
-        <v>3216</v>
+        <v>3238</v>
       </c>
     </row>
     <row r="50" spans="1:3">
       <c r="A50" s="16" t="s">
-        <v>3237</v>
+        <v>3239</v>
       </c>
       <c r="B50" s="16">
         <v>1</v>
       </c>
       <c r="C50" s="16" t="s">
-        <v>3238</v>
+        <v>3216</v>
       </c>
     </row>
     <row r="51" spans="1:3">
       <c r="A51" s="16" t="s">
-        <v>3239</v>
+        <v>3240</v>
       </c>
       <c r="B51" s="16">
         <v>1</v>
@@ -28915,45 +28925,34 @@
     </row>
     <row r="52" spans="1:3">
       <c r="A52" s="16" t="s">
-        <v>3240</v>
+        <v>3241</v>
       </c>
       <c r="B52" s="16">
         <v>1</v>
       </c>
       <c r="C52" s="16" t="s">
-        <v>3216</v>
+        <v>3242</v>
       </c>
     </row>
     <row r="53" spans="1:3">
       <c r="A53" s="16" t="s">
-        <v>3241</v>
+        <v>3243</v>
       </c>
       <c r="B53" s="16">
         <v>1</v>
       </c>
       <c r="C53" s="16" t="s">
-        <v>3242</v>
+        <v>2170</v>
       </c>
     </row>
     <row r="54" spans="1:3">
-      <c r="A54" s="16" t="s">
-        <v>3243</v>
-      </c>
-      <c r="B54" s="16">
+      <c r="A54" s="17" t="s">
+        <v>3244</v>
+      </c>
+      <c r="B54" s="17">
         <v>1</v>
       </c>
-      <c r="C54" s="16" t="s">
-        <v>2170</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3">
-      <c r="A55" s="17" t="s">
-        <v>3244</v>
-      </c>
-      <c r="B55" s="17">
-        <v>1</v>
-      </c>
-      <c r="C55" s="17" t="s">
+      <c r="C54" s="17" t="s">
         <v>1908</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update summary table for the ICBO paper
</commit_message>
<xml_diff>
--- a/doc/mapping results/termsMapping.xlsx
+++ b/doc/mapping results/termsMapping.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5244" uniqueCount="3305">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5256" uniqueCount="3317">
   <si>
     <t>MO URI</t>
   </si>
@@ -9940,6 +9940,42 @@
   </si>
   <si>
     <t>Pre Graz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  12/20/2012 </t>
+  </si>
+  <si>
+    <t>column 7</t>
+  </si>
+  <si>
+    <t>Version if not available provide release date</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>2013-01-08</t>
+  </si>
+  <si>
+    <t>2012-10-03</t>
+  </si>
+  <si>
+    <t>3.1</t>
+  </si>
+  <si>
+    <t>1.512</t>
+  </si>
+  <si>
+    <t>2013-01-25</t>
+  </si>
+  <si>
+    <t>2013-01-24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">31.0. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  01/05/2013</t>
   </si>
 </sst>
 </file>
@@ -10104,7 +10140,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -10145,6 +10181,10 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -27854,10 +27894,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I71"/>
+  <dimension ref="A1:I72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="G57" sqref="G57"/>
+    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="H65" sqref="H65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -28235,9 +28275,6 @@
       <c r="A24" t="s">
         <v>3193</v>
       </c>
-      <c r="B24" s="23" t="s">
-        <v>3273</v>
-      </c>
       <c r="C24" s="12">
         <v>2042</v>
       </c>
@@ -28261,9 +28298,6 @@
       <c r="A25" t="s">
         <v>3212</v>
       </c>
-      <c r="B25" s="23" t="s">
-        <v>3272</v>
-      </c>
       <c r="C25" s="12">
         <v>2120</v>
       </c>
@@ -28290,9 +28324,6 @@
       <c r="A26" t="s">
         <v>3205</v>
       </c>
-      <c r="B26" s="23" t="s">
-        <v>3206</v>
-      </c>
       <c r="C26">
         <v>8188</v>
       </c>
@@ -28316,9 +28347,6 @@
       <c r="A27" t="s">
         <v>3214</v>
       </c>
-      <c r="B27" s="23" t="s">
-        <v>3274</v>
-      </c>
       <c r="C27">
         <v>1455</v>
       </c>
@@ -28339,9 +28367,6 @@
       <c r="A28" t="s">
         <v>3208</v>
       </c>
-      <c r="B28" s="23" t="s">
-        <v>3209</v>
-      </c>
       <c r="C28">
         <v>361</v>
       </c>
@@ -28365,9 +28390,6 @@
       <c r="A29" t="s">
         <v>3218</v>
       </c>
-      <c r="B29" s="23" t="s">
-        <v>3275</v>
-      </c>
       <c r="C29">
         <v>38551</v>
       </c>
@@ -28388,9 +28410,6 @@
       <c r="A30" t="s">
         <v>3222</v>
       </c>
-      <c r="B30" s="23" t="s">
-        <v>3223</v>
-      </c>
       <c r="C30" s="12">
         <v>35436</v>
       </c>
@@ -28414,9 +28433,6 @@
       <c r="A31" t="s">
         <v>3224</v>
       </c>
-      <c r="B31" s="23" t="s">
-        <v>3276</v>
-      </c>
       <c r="C31">
         <v>82</v>
       </c>
@@ -28472,8 +28488,8 @@
       <c r="A40" t="s">
         <v>3281</v>
       </c>
-      <c r="B40" t="s">
-        <v>3277</v>
+      <c r="B40" s="24" t="s">
+        <v>3307</v>
       </c>
     </row>
     <row r="41" spans="1:8">
@@ -28481,7 +28497,7 @@
         <v>3282</v>
       </c>
       <c r="B41" t="s">
-        <v>3278</v>
+        <v>3277</v>
       </c>
     </row>
     <row r="42" spans="1:8">
@@ -28489,7 +28505,7 @@
         <v>3283</v>
       </c>
       <c r="B42" t="s">
-        <v>3288</v>
+        <v>3278</v>
       </c>
     </row>
     <row r="43" spans="1:8">
@@ -28497,7 +28513,7 @@
         <v>3284</v>
       </c>
       <c r="B43" t="s">
-        <v>3279</v>
+        <v>3288</v>
       </c>
     </row>
     <row r="44" spans="1:8">
@@ -28505,113 +28521,146 @@
         <v>3285</v>
       </c>
       <c r="B44" t="s">
+        <v>3279</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8">
+      <c r="A45" t="s">
+        <v>3306</v>
+      </c>
+      <c r="B45" t="s">
         <v>3280</v>
       </c>
     </row>
-    <row r="47" spans="1:8" ht="31.5">
-      <c r="A47" s="21" t="s">
+    <row r="48" spans="1:8" ht="31.5">
+      <c r="A48" s="21" t="s">
         <v>3199</v>
       </c>
-      <c r="B47" s="21" t="s">
+      <c r="B48" s="21" t="s">
         <v>3200</v>
       </c>
-      <c r="C47" s="22" t="s">
+      <c r="C48" s="22" t="s">
         <v>3259</v>
       </c>
-      <c r="D47" s="22" t="s">
+      <c r="D48" s="22" t="s">
         <v>3260</v>
       </c>
-      <c r="E47" s="22" t="s">
+      <c r="E48" s="22" t="s">
         <v>3261</v>
       </c>
-      <c r="F47" s="22" t="s">
+      <c r="F48" s="22" t="s">
         <v>3262</v>
       </c>
-      <c r="G47" s="22" t="s">
+      <c r="G48" s="22" t="s">
         <v>3263</v>
       </c>
-      <c r="H47" s="22" t="s">
+      <c r="H48" s="22" t="s">
         <v>3264</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8">
-      <c r="A48" t="s">
-        <v>3299</v>
-      </c>
-      <c r="B48" t="s">
-        <v>3304</v>
-      </c>
-      <c r="D48">
-        <v>2</v>
       </c>
     </row>
     <row r="49" spans="1:4">
       <c r="A49" t="s">
-        <v>3300</v>
+        <v>3299</v>
+      </c>
+      <c r="B49" t="s">
+        <v>3304</v>
       </c>
       <c r="D49">
         <v>2</v>
       </c>
     </row>
     <row r="50" spans="1:4">
-      <c r="A50" t="s">
-        <v>3301</v>
+      <c r="A50" s="11" t="s">
+        <v>3300</v>
+      </c>
+      <c r="B50" t="s">
+        <v>3305</v>
       </c>
       <c r="D50">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="51" spans="1:4">
       <c r="A51" t="s">
-        <v>3258</v>
+        <v>3301</v>
+      </c>
+      <c r="B51" s="29" t="s">
+        <v>3308</v>
+      </c>
+      <c r="C51">
+        <v>48</v>
       </c>
       <c r="D51">
-        <v>12</v>
+        <v>1</v>
       </c>
     </row>
     <row r="52" spans="1:4">
       <c r="A52" t="s">
-        <v>3196</v>
+        <v>3258</v>
+      </c>
+      <c r="B52" s="23" t="s">
+        <v>3275</v>
       </c>
       <c r="D52">
-        <v>46</v>
+        <v>12</v>
       </c>
     </row>
     <row r="53" spans="1:4">
       <c r="A53" t="s">
-        <v>3253</v>
+        <v>3196</v>
+      </c>
+      <c r="B53" s="23" t="s">
+        <v>3272</v>
+      </c>
+      <c r="C53">
+        <v>2120</v>
       </c>
       <c r="D53">
-        <v>11</v>
+        <v>46</v>
       </c>
     </row>
     <row r="54" spans="1:4">
       <c r="A54" t="s">
-        <v>3302</v>
+        <v>3253</v>
+      </c>
+      <c r="B54" s="23" t="s">
+        <v>3223</v>
+      </c>
+      <c r="C54">
+        <v>35436</v>
       </c>
       <c r="D54">
-        <v>1</v>
+        <v>11</v>
       </c>
     </row>
     <row r="55" spans="1:4">
       <c r="A55" t="s">
+        <v>3302</v>
+      </c>
+      <c r="B55" s="23" t="s">
+        <v>3309</v>
+      </c>
+      <c r="D55">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4">
+      <c r="A56" s="11" t="s">
         <v>3247</v>
       </c>
-      <c r="D55">
+      <c r="B56" s="23" t="s">
+        <v>3310</v>
+      </c>
+      <c r="D56">
         <v>2</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4">
-      <c r="A56" t="s">
-        <v>3230</v>
-      </c>
-      <c r="D56">
-        <v>1</v>
       </c>
     </row>
     <row r="57" spans="1:4">
       <c r="A57" t="s">
-        <v>3237</v>
+        <v>3230</v>
+      </c>
+      <c r="B57" s="23" t="s">
+        <v>3311</v>
       </c>
       <c r="D57">
         <v>1</v>
@@ -28619,15 +28668,21 @@
     </row>
     <row r="58" spans="1:4">
       <c r="A58" t="s">
-        <v>3231</v>
+        <v>3237</v>
+      </c>
+      <c r="B58" s="23" t="s">
+        <v>3312</v>
       </c>
       <c r="D58">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="59" spans="1:4">
       <c r="A59" t="s">
-        <v>3232</v>
+        <v>3231</v>
+      </c>
+      <c r="B59" s="23" t="s">
+        <v>3313</v>
       </c>
       <c r="D59">
         <v>2</v>
@@ -28635,47 +28690,69 @@
     </row>
     <row r="60" spans="1:4">
       <c r="A60" t="s">
-        <v>3239</v>
-      </c>
+        <v>3232</v>
+      </c>
+      <c r="B60" s="23"/>
       <c r="D60">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="61" spans="1:4">
       <c r="A61" t="s">
-        <v>3193</v>
+        <v>3239</v>
+      </c>
+      <c r="B61" s="23" t="s">
+        <v>3314</v>
+      </c>
+      <c r="C61">
+        <v>981148</v>
       </c>
       <c r="D61">
-        <v>200</v>
+        <v>1</v>
       </c>
     </row>
     <row r="62" spans="1:4">
       <c r="A62" t="s">
-        <v>3224</v>
+        <v>3193</v>
+      </c>
+      <c r="B62" s="23" t="s">
+        <v>3273</v>
+      </c>
+      <c r="C62">
+        <v>2042</v>
       </c>
       <c r="D62">
-        <v>3</v>
+        <v>200</v>
       </c>
     </row>
     <row r="63" spans="1:4">
       <c r="A63" t="s">
-        <v>3214</v>
+        <v>3224</v>
+      </c>
+      <c r="B63" s="23" t="s">
+        <v>3276</v>
       </c>
       <c r="D63">
-        <v>19</v>
+        <v>3</v>
       </c>
     </row>
     <row r="64" spans="1:4">
       <c r="A64" t="s">
-        <v>3249</v>
+        <v>3214</v>
+      </c>
+      <c r="B64" s="23" t="s">
+        <v>3274</v>
       </c>
       <c r="D64">
-        <v>1</v>
+        <v>19</v>
       </c>
     </row>
     <row r="65" spans="1:4">
       <c r="A65" t="s">
-        <v>3241</v>
+        <v>3249</v>
+      </c>
+      <c r="B65" s="23" t="s">
+        <v>3315</v>
       </c>
       <c r="D65">
         <v>1</v>
@@ -28683,7 +28760,10 @@
     </row>
     <row r="66" spans="1:4">
       <c r="A66" t="s">
-        <v>3233</v>
+        <v>3241</v>
+      </c>
+      <c r="B66">
+        <v>4.5999999999999996</v>
       </c>
       <c r="D66">
         <v>1</v>
@@ -28691,41 +28771,67 @@
     </row>
     <row r="67" spans="1:4">
       <c r="A67" t="s">
-        <v>3205</v>
+        <v>3233</v>
+      </c>
+      <c r="B67" s="28">
+        <v>39752</v>
       </c>
       <c r="D67">
-        <v>126</v>
+        <v>1</v>
       </c>
     </row>
     <row r="68" spans="1:4">
       <c r="A68" t="s">
-        <v>3208</v>
+        <v>3205</v>
+      </c>
+      <c r="B68" s="23" t="s">
+        <v>3206</v>
       </c>
       <c r="D68">
-        <v>67</v>
+        <v>126</v>
       </c>
     </row>
     <row r="69" spans="1:4">
       <c r="A69" t="s">
-        <v>3243</v>
+        <v>3208</v>
+      </c>
+      <c r="B69" s="23" t="s">
+        <v>3209</v>
       </c>
       <c r="D69">
-        <v>1</v>
+        <v>67</v>
       </c>
     </row>
     <row r="70" spans="1:4">
       <c r="A70" t="s">
+        <v>3243</v>
+      </c>
+      <c r="B70" s="23" t="s">
+        <v>3316</v>
+      </c>
+      <c r="D70">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4">
+      <c r="A71" s="11" t="s">
         <v>3303</v>
       </c>
-      <c r="D70">
+      <c r="B71">
+        <v>2.31</v>
+      </c>
+      <c r="D71">
         <v>63</v>
       </c>
     </row>
-    <row r="71" spans="1:4">
-      <c r="A71" t="s">
+    <row r="72" spans="1:4">
+      <c r="A72" t="s">
         <v>3244</v>
       </c>
-      <c r="D71">
+      <c r="B72">
+        <v>0.5</v>
+      </c>
+      <c r="D72">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add more mapping and provide definitions for new terms
</commit_message>
<xml_diff>
--- a/doc/mapping results/termsMapping.xlsx
+++ b/doc/mapping results/termsMapping.xlsx
@@ -1,26 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr date1904="1"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="-15" windowWidth="12615" windowHeight="11760" tabRatio="693" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="-15" yWindow="-15" windowWidth="12615" windowHeight="11760" tabRatio="852"/>
   </bookViews>
   <sheets>
-    <sheet name="terms2ignore" sheetId="2" r:id="rId1"/>
-    <sheet name="mappedTerms" sheetId="3" r:id="rId2"/>
-    <sheet name="terms2submit" sheetId="4" r:id="rId3"/>
-    <sheet name="termsInBCGO" sheetId="8" r:id="rId4"/>
-    <sheet name="StrainOrLine_Emily" sheetId="5" r:id="rId5"/>
-    <sheet name="Summary of Subset" sheetId="6" r:id="rId6"/>
-    <sheet name="Summary of Mapping" sheetId="7" r:id="rId7"/>
+    <sheet name="terms2add" sheetId="9" r:id="rId1"/>
+    <sheet name="terms2add-cell type" sheetId="10" r:id="rId2"/>
+    <sheet name="terms2ignore" sheetId="2" r:id="rId3"/>
+    <sheet name="mappedTerms" sheetId="3" r:id="rId4"/>
+    <sheet name="terms2submit" sheetId="4" r:id="rId5"/>
+    <sheet name="termsInBCGO" sheetId="8" r:id="rId6"/>
+    <sheet name="StrainOrLine_Emily" sheetId="5" r:id="rId7"/>
+    <sheet name="Summary of Subset" sheetId="6" r:id="rId8"/>
+    <sheet name="Summary of Mapping" sheetId="7" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5284" uniqueCount="3324">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6109" uniqueCount="3421">
   <si>
     <t>MO URI</t>
   </si>
@@ -9998,6 +10000,305 @@
   </si>
   <si>
     <t>http://purl.obolibrary.org/obo/CL_0000163</t>
+  </si>
+  <si>
+    <t>Axioms</t>
+  </si>
+  <si>
+    <t>Parent Class</t>
+  </si>
+  <si>
+    <t>specify the method and type of reportor on array</t>
+  </si>
+  <si>
+    <t>planned process/material? Like microarray feature, part of microarray</t>
+  </si>
+  <si>
+    <t>method feature spotting, input doble stranded DNA, output ds DNA microarray feature</t>
+  </si>
+  <si>
+    <t>method feature spotting, input ss_oligo, output spotted ss oligo feature, (ChEBI:oligonucleotide)</t>
+  </si>
+  <si>
+    <t>feature in situ method, input ChEBI:oligonucleotide</t>
+  </si>
+  <si>
+    <t>Label</t>
+  </si>
+  <si>
+    <t>microarray feature</t>
+  </si>
+  <si>
+    <t>in situ oligo microarray feature</t>
+  </si>
+  <si>
+    <t>spotted ds DNA microarray feature</t>
+  </si>
+  <si>
+    <t>spotted ss oligo microarray feature</t>
+  </si>
+  <si>
+    <t>contact representative role</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/OBI_0001687</t>
+  </si>
+  <si>
+    <t>A role inhering in a person who represents an institution, organization, or service provider and realized when communication is directed at them about the entity they represent.</t>
+  </si>
+  <si>
+    <t>only apply to human not organization.</t>
+  </si>
+  <si>
+    <t>(has_specified_input some 
+    ('material entity'
+     and ('has quality' only (not (frozen)))))
+ and (has_specified_output some 
+    ('material entity'
+     and ('has quality' some frozen)))</t>
+  </si>
+  <si>
+    <t>a planned process to create an output material with a decreased concentration of a material of interest that is part of the input material</t>
+  </si>
+  <si>
+    <t>has_specified_output some 
+    ('material entity'
+     and ('has quality' some PATO:'decreased concentration' or PATO:diluted))</t>
+  </si>
+  <si>
+    <t>OBI:concentrate, has objective 'separation into different composition objective'. For dilute, can we say 'add material objective'
+What major difference between diluted(http://purl.obolibrary.org/obo/PATO_0001161) and decreased concentration (http://purl.obolibrary.org/obo/PATO_0001163) in PATO. Cannot understand why it is subclass of concentrated. Can I think diluted is the subclass of decreased concentration?</t>
+  </si>
+  <si>
+    <t>obi has freezing storage. Could add freezing, and set freezing storage has part freezing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">process or planned process, can we think quality changes as material transformation? </t>
+  </si>
+  <si>
+    <t>Do we need this term without any subclasses (glass, nylon, etc.) included? If we need, how about coating material, and add coating role</t>
+  </si>
+  <si>
+    <t>temperature setting specification</t>
+  </si>
+  <si>
+    <t>plan specification</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A plan specification that the temperature is specified. </t>
+  </si>
+  <si>
+    <t>is about some temperature value</t>
+  </si>
+  <si>
+    <t>physical object quality</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/PATO_0001241</t>
+  </si>
+  <si>
+    <t>is it data analysis objective? Do we need the specific study design type for it? Is transcription profiling design enough?</t>
+  </si>
+  <si>
+    <t>technology</t>
+  </si>
+  <si>
+    <t>transcription profiling</t>
+  </si>
+  <si>
+    <t>objective</t>
+  </si>
+  <si>
+    <t>software optimal</t>
+  </si>
+  <si>
+    <t>biological objective (organismal, cellular, molecular level)</t>
+  </si>
+  <si>
+    <t>Do we want to include data analysis objective?</t>
+  </si>
+  <si>
+    <t>do we want to cover experimental factor in OBI?</t>
+  </si>
+  <si>
+    <t>experimental factor specification</t>
+  </si>
+  <si>
+    <t>subClassOf independent variable specification?</t>
+  </si>
+  <si>
+    <t>should we use more specific terms, like height, mass …</t>
+  </si>
+  <si>
+    <t>Information concerning the envinonrment a material entity has been exposed to, such as an organism from a lake.</t>
+  </si>
+  <si>
+    <t>information content entity</t>
+  </si>
+  <si>
+    <t>environmental history</t>
+  </si>
+  <si>
+    <t>OBI/OGMS</t>
+  </si>
+  <si>
+    <t>observation record</t>
+  </si>
+  <si>
+    <t xml:space="preserve">data item </t>
+  </si>
+  <si>
+    <t>A data item that records examination of material entity with unaided eyes.</t>
+  </si>
+  <si>
+    <t>specimen/processed specimen</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/OBI_0000953</t>
+  </si>
+  <si>
+    <t>OMRS (Ontology of Medically Related Social Entities)</t>
+  </si>
+  <si>
+    <t>family role</t>
+  </si>
+  <si>
+    <t>available in Role ontology (http://bioportal.bioontology.org/ontologies/1538), do we also need its subclasses, like mother, father, son, aunt, uncle, etc.</t>
+  </si>
+  <si>
+    <t>SO:region?</t>
+  </si>
+  <si>
+    <t>molecular</t>
+  </si>
+  <si>
+    <t>generic dependent continuant</t>
+  </si>
+  <si>
+    <t>Categorical terms with no any subclasses or instances were used in annotation, should be ignored.</t>
+  </si>
+  <si>
+    <t>transcription factor SOX-17</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/PR_000015424</t>
+  </si>
+  <si>
+    <t>produce some transcript translate_to</t>
+  </si>
+  <si>
+    <t>protein ID</t>
+  </si>
+  <si>
+    <t>is_part_of</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/UBERON_0003924</t>
+  </si>
+  <si>
+    <t>ventral pancreatic bud</t>
+  </si>
+  <si>
+    <t>BCGO</t>
+  </si>
+  <si>
+    <t>ventral pancreatic bud Sox17 expressing cell</t>
+  </si>
+  <si>
+    <t>Parent</t>
+  </si>
+  <si>
+    <t>native cell</t>
+  </si>
+  <si>
+    <t>definition</t>
+  </si>
+  <si>
+    <t>definition in GBCO</t>
+  </si>
+  <si>
+    <t>tumor-associated calcium signal transducer 1</t>
+  </si>
+  <si>
+    <t>A native cell that is expressing Sox17 and EpCAM which is part of embryonic mid gut containing ventral pancreatic buds.</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/PR_000001559</t>
+  </si>
+  <si>
+    <t>A native cell  that is part of mature islet and is expressing insulin</t>
+  </si>
+  <si>
+    <t>insulin</t>
+  </si>
+  <si>
+    <t>existence_starts_at some developmenta stage</t>
+  </si>
+  <si>
+    <t>islet mature stage (need to add a new term)</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/PR_000009054</t>
+  </si>
+  <si>
+    <t>pancreatic bud ngn3 expressing cell</t>
+  </si>
+  <si>
+    <t>insulin-expressing mature pancreatic beta cell</t>
+  </si>
+  <si>
+    <t>relation to type B pancreatic cell, does it only exist in mature islet, can we better define matured beta cell.</t>
+  </si>
+  <si>
+    <t>http://purl.oblibrary.org/obo/bcgo/BCGO_0000012</t>
+  </si>
+  <si>
+    <t>native cell/type B pancreatic cell</t>
+  </si>
+  <si>
+    <t>a native cell that is part of pancreatic bud and is expressing ngn3</t>
+  </si>
+  <si>
+    <t>BCGO URI</t>
+  </si>
+  <si>
+    <t>BCGO / CL</t>
+  </si>
+  <si>
+    <t>develop_into some posterior foregut</t>
+  </si>
+  <si>
+    <t>An embryonic stem cell that will develop into posterior foregut</t>
+  </si>
+  <si>
+    <t>need to add posterior foregut</t>
+  </si>
+  <si>
+    <t>hepatic stem cell</t>
+  </si>
+  <si>
+    <t>postnatal day 60</t>
+  </si>
+  <si>
+    <t>http://purl.oblibrary.org/obo/bcgo/BCGO_0000015</t>
+  </si>
+  <si>
+    <t>molecular label</t>
+  </si>
+  <si>
+    <t>=molecular entity and has_role molecular label role</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/UO_0000179</t>
+  </si>
+  <si>
+    <t>unit per liter</t>
+  </si>
+  <si>
+    <t>Should be in IAO</t>
+  </si>
+  <si>
+    <t>don't think it is developmental stage, more like time datum, differentiation stage</t>
   </si>
 </sst>
 </file>
@@ -10162,7 +10463,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -10244,16 +10545,20 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1" shrinkToFit="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="超链接" xfId="1" builtinId="8"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -10650,13 +10955,2959 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G92"/>
+  <dimension ref="A1:L179"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C77" sqref="C77"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="4" ySplit="1" topLeftCell="I53" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="E1" sqref="E1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="J73" sqref="J73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
+  <cols>
+    <col min="2" max="2" width="16.75" customWidth="1"/>
+    <col min="3" max="3" width="28.375" customWidth="1"/>
+    <col min="4" max="5" width="56" customWidth="1"/>
+    <col min="6" max="6" width="14.125" customWidth="1"/>
+    <col min="7" max="7" width="19.875" customWidth="1"/>
+    <col min="8" max="8" width="26.125" customWidth="1"/>
+    <col min="9" max="9" width="13.25" customWidth="1"/>
+    <col min="10" max="10" width="83.625" customWidth="1"/>
+    <col min="11" max="11" width="50.125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" s="3" customFormat="1" ht="18.75">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>3331</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>3199</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>3325</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>3324</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>818</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
+      <c r="A2" t="s">
+        <v>483</v>
+      </c>
+      <c r="C2" t="s">
+        <v>81</v>
+      </c>
+      <c r="D2" t="s">
+        <v>165</v>
+      </c>
+      <c r="E2" t="s">
+        <v>3332</v>
+      </c>
+      <c r="F2" t="s">
+        <v>3193</v>
+      </c>
+      <c r="G2" t="s">
+        <v>3327</v>
+      </c>
+      <c r="J2" t="s">
+        <v>3326</v>
+      </c>
+      <c r="K2" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
+      <c r="A3" t="s">
+        <v>434</v>
+      </c>
+      <c r="C3" t="s">
+        <v>165</v>
+      </c>
+      <c r="D3" t="s">
+        <v>435</v>
+      </c>
+      <c r="E3" t="s">
+        <v>3333</v>
+      </c>
+      <c r="F3" t="s">
+        <v>3193</v>
+      </c>
+      <c r="J3" t="s">
+        <v>3330</v>
+      </c>
+      <c r="K3" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
+      <c r="A4" t="s">
+        <v>164</v>
+      </c>
+      <c r="C4" t="s">
+        <v>165</v>
+      </c>
+      <c r="D4" t="s">
+        <v>166</v>
+      </c>
+      <c r="E4" t="s">
+        <v>3334</v>
+      </c>
+      <c r="F4" t="s">
+        <v>3193</v>
+      </c>
+      <c r="J4" t="s">
+        <v>3328</v>
+      </c>
+      <c r="K4" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
+      <c r="A5" t="s">
+        <v>805</v>
+      </c>
+      <c r="C5" t="s">
+        <v>165</v>
+      </c>
+      <c r="D5" t="s">
+        <v>806</v>
+      </c>
+      <c r="E5" t="s">
+        <v>3335</v>
+      </c>
+      <c r="F5" t="s">
+        <v>3193</v>
+      </c>
+      <c r="J5" t="s">
+        <v>3329</v>
+      </c>
+      <c r="K5" t="s">
+        <v>807</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="141.75">
+      <c r="B7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" t="s">
+        <v>524</v>
+      </c>
+      <c r="D7" t="s">
+        <v>532</v>
+      </c>
+      <c r="E7" t="s">
+        <v>532</v>
+      </c>
+      <c r="F7" t="s">
+        <v>3193</v>
+      </c>
+      <c r="G7" s="41" t="s">
+        <v>3345</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>3340</v>
+      </c>
+      <c r="J7" t="s">
+        <v>3344</v>
+      </c>
+      <c r="K7" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="94.5">
+      <c r="A8" t="s">
+        <v>523</v>
+      </c>
+      <c r="C8" t="s">
+        <v>524</v>
+      </c>
+      <c r="D8" t="s">
+        <v>525</v>
+      </c>
+      <c r="E8" t="s">
+        <v>525</v>
+      </c>
+      <c r="F8" t="s">
+        <v>3193</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>3342</v>
+      </c>
+      <c r="I8" t="s">
+        <v>3341</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>3343</v>
+      </c>
+      <c r="K8" t="s">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
+      <c r="A9" t="s">
+        <v>581</v>
+      </c>
+      <c r="C9" t="s">
+        <v>524</v>
+      </c>
+      <c r="D9" t="s">
+        <v>582</v>
+      </c>
+      <c r="E9" t="s">
+        <v>3347</v>
+      </c>
+      <c r="F9" t="s">
+        <v>3193</v>
+      </c>
+      <c r="G9" t="s">
+        <v>3348</v>
+      </c>
+      <c r="H9" t="s">
+        <v>3350</v>
+      </c>
+      <c r="I9" t="s">
+        <v>3349</v>
+      </c>
+      <c r="K9" t="s">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
+      <c r="A11" t="s">
+        <v>764</v>
+      </c>
+      <c r="C11" t="s">
+        <v>432</v>
+      </c>
+      <c r="D11" t="s">
+        <v>765</v>
+      </c>
+      <c r="G11" t="s">
+        <v>2069</v>
+      </c>
+      <c r="J11" t="s">
+        <v>3353</v>
+      </c>
+      <c r="K11" t="s">
+        <v>766</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11">
+      <c r="A12" t="s">
+        <v>158</v>
+      </c>
+      <c r="C12" t="s">
+        <v>70</v>
+      </c>
+      <c r="D12" t="s">
+        <v>159</v>
+      </c>
+      <c r="G12" t="s">
+        <v>2069</v>
+      </c>
+      <c r="K12" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11">
+      <c r="A14" t="s">
+        <v>641</v>
+      </c>
+      <c r="C14" t="s">
+        <v>183</v>
+      </c>
+      <c r="D14" t="s">
+        <v>642</v>
+      </c>
+      <c r="E14" t="s">
+        <v>3351</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>3352</v>
+      </c>
+      <c r="K14" t="s">
+        <v>643</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11">
+      <c r="A15" t="s">
+        <v>348</v>
+      </c>
+      <c r="C15" t="s">
+        <v>210</v>
+      </c>
+      <c r="D15" t="s">
+        <v>275</v>
+      </c>
+      <c r="E15" t="s">
+        <v>3351</v>
+      </c>
+      <c r="J15" t="s">
+        <v>3363</v>
+      </c>
+      <c r="K15" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11">
+      <c r="A16" t="s">
+        <v>209</v>
+      </c>
+      <c r="C16" t="s">
+        <v>210</v>
+      </c>
+      <c r="D16" t="s">
+        <v>211</v>
+      </c>
+      <c r="E16" t="s">
+        <v>3366</v>
+      </c>
+      <c r="F16" t="s">
+        <v>3367</v>
+      </c>
+      <c r="G16" t="s">
+        <v>3365</v>
+      </c>
+      <c r="I16" t="s">
+        <v>3364</v>
+      </c>
+      <c r="K16" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11">
+      <c r="A17" t="s">
+        <v>465</v>
+      </c>
+      <c r="C17" t="s">
+        <v>210</v>
+      </c>
+      <c r="D17" t="s">
+        <v>198</v>
+      </c>
+      <c r="E17" t="s">
+        <v>3368</v>
+      </c>
+      <c r="F17" t="s">
+        <v>3193</v>
+      </c>
+      <c r="G17" t="s">
+        <v>3369</v>
+      </c>
+      <c r="I17" t="s">
+        <v>3370</v>
+      </c>
+      <c r="K17" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11">
+      <c r="A18" t="s">
+        <v>502</v>
+      </c>
+      <c r="C18" t="s">
+        <v>44</v>
+      </c>
+      <c r="D18" t="s">
+        <v>503</v>
+      </c>
+      <c r="E18" t="s">
+        <v>885</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>884</v>
+      </c>
+      <c r="K18" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11">
+      <c r="A19" t="s">
+        <v>401</v>
+      </c>
+      <c r="C19" t="s">
+        <v>44</v>
+      </c>
+      <c r="D19" t="s">
+        <v>402</v>
+      </c>
+      <c r="E19" t="s">
+        <v>3371</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>3372</v>
+      </c>
+      <c r="K19" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11">
+      <c r="A20" t="s">
+        <v>77</v>
+      </c>
+      <c r="C20" t="s">
+        <v>78</v>
+      </c>
+      <c r="D20" t="s">
+        <v>79</v>
+      </c>
+      <c r="E20" t="s">
+        <v>3415</v>
+      </c>
+      <c r="F20" t="s">
+        <v>3193</v>
+      </c>
+      <c r="G20" t="s">
+        <v>954</v>
+      </c>
+      <c r="H20" s="44" t="s">
+        <v>3416</v>
+      </c>
+      <c r="K20" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11">
+      <c r="B22" t="s">
+        <v>17</v>
+      </c>
+      <c r="C22" t="s">
+        <v>91</v>
+      </c>
+      <c r="D22" t="s">
+        <v>786</v>
+      </c>
+      <c r="K22" t="s">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11">
+      <c r="B23" t="s">
+        <v>17</v>
+      </c>
+      <c r="C23" t="s">
+        <v>91</v>
+      </c>
+      <c r="D23" t="s">
+        <v>787</v>
+      </c>
+      <c r="K23" t="s">
+        <v>788</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11">
+      <c r="B24" t="s">
+        <v>17</v>
+      </c>
+      <c r="C24" t="s">
+        <v>91</v>
+      </c>
+      <c r="D24" t="s">
+        <v>570</v>
+      </c>
+      <c r="K24" t="s">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11">
+      <c r="B25" t="s">
+        <v>17</v>
+      </c>
+      <c r="C25" t="s">
+        <v>91</v>
+      </c>
+      <c r="D25" t="s">
+        <v>598</v>
+      </c>
+      <c r="K25" t="s">
+        <v>599</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11">
+      <c r="B26" t="s">
+        <v>17</v>
+      </c>
+      <c r="C26" t="s">
+        <v>91</v>
+      </c>
+      <c r="D26" t="s">
+        <v>799</v>
+      </c>
+      <c r="K26" t="s">
+        <v>788</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11">
+      <c r="B27" t="s">
+        <v>17</v>
+      </c>
+      <c r="C27" t="s">
+        <v>91</v>
+      </c>
+      <c r="D27" t="s">
+        <v>675</v>
+      </c>
+      <c r="K27" t="s">
+        <v>599</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11">
+      <c r="B28" t="s">
+        <v>17</v>
+      </c>
+      <c r="C28" t="s">
+        <v>91</v>
+      </c>
+      <c r="D28" t="s">
+        <v>423</v>
+      </c>
+      <c r="K28" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11">
+      <c r="B29" t="s">
+        <v>17</v>
+      </c>
+      <c r="C29" t="s">
+        <v>91</v>
+      </c>
+      <c r="D29" t="s">
+        <v>425</v>
+      </c>
+      <c r="K29" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11">
+      <c r="B30" t="s">
+        <v>17</v>
+      </c>
+      <c r="C30" t="s">
+        <v>91</v>
+      </c>
+      <c r="D30" t="s">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11">
+      <c r="B31" t="s">
+        <v>17</v>
+      </c>
+      <c r="C31" t="s">
+        <v>91</v>
+      </c>
+      <c r="D31" t="s">
+        <v>542</v>
+      </c>
+      <c r="K31" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11">
+      <c r="B32" t="s">
+        <v>17</v>
+      </c>
+      <c r="C32" t="s">
+        <v>91</v>
+      </c>
+      <c r="D32" t="s">
+        <v>123</v>
+      </c>
+      <c r="K32" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11">
+      <c r="B33" t="s">
+        <v>17</v>
+      </c>
+      <c r="C33" t="s">
+        <v>91</v>
+      </c>
+      <c r="D33" t="s">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11">
+      <c r="B34" t="s">
+        <v>17</v>
+      </c>
+      <c r="C34" t="s">
+        <v>91</v>
+      </c>
+      <c r="D34" t="s">
+        <v>481</v>
+      </c>
+      <c r="K34" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11">
+      <c r="B35" t="s">
+        <v>17</v>
+      </c>
+      <c r="C35" t="s">
+        <v>91</v>
+      </c>
+      <c r="D35" t="s">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11">
+      <c r="A36" t="s">
+        <v>516</v>
+      </c>
+      <c r="C36" t="s">
+        <v>91</v>
+      </c>
+      <c r="D36" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11">
+      <c r="C37" t="s">
+        <v>91</v>
+      </c>
+      <c r="D37" t="s">
+        <v>576</v>
+      </c>
+      <c r="K37" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11">
+      <c r="C38" t="s">
+        <v>91</v>
+      </c>
+      <c r="D38" t="s">
+        <v>505</v>
+      </c>
+      <c r="K38" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11">
+      <c r="B40" t="s">
+        <v>17</v>
+      </c>
+      <c r="C40" t="s">
+        <v>25</v>
+      </c>
+      <c r="D40" t="s">
+        <v>407</v>
+      </c>
+      <c r="K40" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11">
+      <c r="B41" t="s">
+        <v>17</v>
+      </c>
+      <c r="C41" t="s">
+        <v>25</v>
+      </c>
+      <c r="D41" t="s">
+        <v>779</v>
+      </c>
+      <c r="K41" t="s">
+        <v>780</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11">
+      <c r="A42" t="s">
+        <v>40</v>
+      </c>
+      <c r="C42" t="s">
+        <v>25</v>
+      </c>
+      <c r="D42" t="s">
+        <v>41</v>
+      </c>
+      <c r="K42" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11">
+      <c r="A43" t="s">
+        <v>303</v>
+      </c>
+      <c r="C43" t="s">
+        <v>25</v>
+      </c>
+      <c r="D43" t="s">
+        <v>304</v>
+      </c>
+      <c r="K43" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11">
+      <c r="A44" t="s">
+        <v>488</v>
+      </c>
+      <c r="C44" t="s">
+        <v>25</v>
+      </c>
+      <c r="D44" t="s">
+        <v>489</v>
+      </c>
+      <c r="F44" t="s">
+        <v>1837</v>
+      </c>
+      <c r="H44" s="1" t="s">
+        <v>1838</v>
+      </c>
+      <c r="I44" s="1"/>
+      <c r="J44" s="1"/>
+      <c r="K44" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11">
+      <c r="A45" t="s">
+        <v>114</v>
+      </c>
+      <c r="C45" t="s">
+        <v>25</v>
+      </c>
+      <c r="D45" t="s">
+        <v>115</v>
+      </c>
+      <c r="F45" t="s">
+        <v>1945</v>
+      </c>
+      <c r="H45" s="1" t="s">
+        <v>1946</v>
+      </c>
+      <c r="I45" s="1"/>
+      <c r="J45" s="1"/>
+      <c r="K45" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11">
+      <c r="A46" t="s">
+        <v>332</v>
+      </c>
+      <c r="C46" t="s">
+        <v>25</v>
+      </c>
+      <c r="D46" t="s">
+        <v>333</v>
+      </c>
+      <c r="K46" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11">
+      <c r="A49" t="s">
+        <v>3419</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11">
+      <c r="A50" t="s">
+        <v>672</v>
+      </c>
+      <c r="C50" t="s">
+        <v>8</v>
+      </c>
+      <c r="D50" t="s">
+        <v>673</v>
+      </c>
+      <c r="K50" t="s">
+        <v>674</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11">
+      <c r="A51" t="s">
+        <v>63</v>
+      </c>
+      <c r="C51" t="s">
+        <v>8</v>
+      </c>
+      <c r="D51" t="s">
+        <v>64</v>
+      </c>
+      <c r="K51" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11">
+      <c r="A52" t="s">
+        <v>783</v>
+      </c>
+      <c r="C52" t="s">
+        <v>8</v>
+      </c>
+      <c r="D52" t="s">
+        <v>784</v>
+      </c>
+      <c r="K52" t="s">
+        <v>785</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11">
+      <c r="A53" t="s">
+        <v>593</v>
+      </c>
+      <c r="C53" t="s">
+        <v>8</v>
+      </c>
+      <c r="D53" t="s">
+        <v>594</v>
+      </c>
+      <c r="K53" t="s">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11">
+      <c r="A54" t="s">
+        <v>342</v>
+      </c>
+      <c r="C54" t="s">
+        <v>8</v>
+      </c>
+      <c r="D54" t="s">
+        <v>343</v>
+      </c>
+      <c r="K54" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11">
+      <c r="A55" t="s">
+        <v>151</v>
+      </c>
+      <c r="C55" t="s">
+        <v>8</v>
+      </c>
+      <c r="D55" t="s">
+        <v>152</v>
+      </c>
+      <c r="K55" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11">
+      <c r="A56" t="s">
+        <v>647</v>
+      </c>
+      <c r="C56" t="s">
+        <v>8</v>
+      </c>
+      <c r="D56" t="s">
+        <v>648</v>
+      </c>
+      <c r="K56" t="s">
+        <v>649</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11">
+      <c r="A57" t="s">
+        <v>776</v>
+      </c>
+      <c r="C57" t="s">
+        <v>8</v>
+      </c>
+      <c r="D57" t="s">
+        <v>777</v>
+      </c>
+      <c r="K57" t="s">
+        <v>778</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11">
+      <c r="A58" t="s">
+        <v>676</v>
+      </c>
+      <c r="C58" t="s">
+        <v>8</v>
+      </c>
+      <c r="D58" t="s">
+        <v>677</v>
+      </c>
+      <c r="K58" t="s">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11">
+      <c r="A59" t="s">
+        <v>244</v>
+      </c>
+      <c r="C59" t="s">
+        <v>8</v>
+      </c>
+      <c r="D59" t="s">
+        <v>245</v>
+      </c>
+      <c r="K59" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11">
+      <c r="A60" t="s">
+        <v>277</v>
+      </c>
+      <c r="C60" t="s">
+        <v>8</v>
+      </c>
+      <c r="D60" t="s">
+        <v>278</v>
+      </c>
+      <c r="K60" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11">
+      <c r="A61" t="s">
+        <v>120</v>
+      </c>
+      <c r="C61" t="s">
+        <v>8</v>
+      </c>
+      <c r="D61" t="s">
+        <v>121</v>
+      </c>
+      <c r="K61" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11">
+      <c r="A62" t="s">
+        <v>234</v>
+      </c>
+      <c r="C62" t="s">
+        <v>8</v>
+      </c>
+      <c r="D62" t="s">
+        <v>235</v>
+      </c>
+      <c r="K62" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11">
+      <c r="B64" t="s">
+        <v>17</v>
+      </c>
+      <c r="C64" t="s">
+        <v>15</v>
+      </c>
+      <c r="D64" t="s">
+        <v>813</v>
+      </c>
+      <c r="E64" t="s">
+        <v>3413</v>
+      </c>
+      <c r="F64" s="1" t="s">
+        <v>3414</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11">
+      <c r="C66" t="s">
+        <v>15</v>
+      </c>
+      <c r="D66" t="s">
+        <v>47</v>
+      </c>
+      <c r="J66" t="s">
+        <v>3420</v>
+      </c>
+      <c r="K66" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11">
+      <c r="C67" t="s">
+        <v>15</v>
+      </c>
+      <c r="D67" t="s">
+        <v>655</v>
+      </c>
+      <c r="K67" t="s">
+        <v>656</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11">
+      <c r="A69" t="s">
+        <v>520</v>
+      </c>
+      <c r="C69" t="s">
+        <v>211</v>
+      </c>
+      <c r="D69" t="s">
+        <v>521</v>
+      </c>
+      <c r="K69" t="s">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="70" spans="1:11">
+      <c r="A70" t="s">
+        <v>633</v>
+      </c>
+      <c r="C70" t="s">
+        <v>192</v>
+      </c>
+      <c r="D70" t="s">
+        <v>182</v>
+      </c>
+      <c r="K70" t="s">
+        <v>634</v>
+      </c>
+    </row>
+    <row r="71" spans="1:11">
+      <c r="A71" t="s">
+        <v>225</v>
+      </c>
+      <c r="C71" t="s">
+        <v>192</v>
+      </c>
+      <c r="D71" t="s">
+        <v>226</v>
+      </c>
+      <c r="K71" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11">
+      <c r="A72" t="s">
+        <v>191</v>
+      </c>
+      <c r="C72" t="s">
+        <v>192</v>
+      </c>
+      <c r="D72" t="s">
+        <v>193</v>
+      </c>
+      <c r="K72" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11">
+      <c r="A73" t="s">
+        <v>553</v>
+      </c>
+      <c r="B73" t="s">
+        <v>554</v>
+      </c>
+      <c r="C73" t="s">
+        <v>186</v>
+      </c>
+      <c r="D73" t="s">
+        <v>555</v>
+      </c>
+      <c r="K73" t="s">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="74" spans="1:11">
+      <c r="A74" t="s">
+        <v>309</v>
+      </c>
+      <c r="C74" t="s">
+        <v>186</v>
+      </c>
+      <c r="D74" t="s">
+        <v>310</v>
+      </c>
+      <c r="K74" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="75" spans="1:11">
+      <c r="A75" t="s">
+        <v>185</v>
+      </c>
+      <c r="C75" t="s">
+        <v>186</v>
+      </c>
+      <c r="D75" t="s">
+        <v>187</v>
+      </c>
+      <c r="K75" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="76" spans="1:11">
+      <c r="A76" t="s">
+        <v>440</v>
+      </c>
+      <c r="C76" t="s">
+        <v>186</v>
+      </c>
+      <c r="D76" t="s">
+        <v>441</v>
+      </c>
+      <c r="K76" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="77" spans="1:11">
+      <c r="A77" t="s">
+        <v>431</v>
+      </c>
+      <c r="C77" t="s">
+        <v>69</v>
+      </c>
+      <c r="D77" t="s">
+        <v>432</v>
+      </c>
+      <c r="K77" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="78" spans="1:11">
+      <c r="A78" t="s">
+        <v>68</v>
+      </c>
+      <c r="C78" t="s">
+        <v>69</v>
+      </c>
+      <c r="D78" t="s">
+        <v>70</v>
+      </c>
+      <c r="K78" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="79" spans="1:11">
+      <c r="A79" t="s">
+        <v>110</v>
+      </c>
+      <c r="C79" t="s">
+        <v>69</v>
+      </c>
+      <c r="D79" t="s">
+        <v>111</v>
+      </c>
+      <c r="K79" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="80" spans="1:11">
+      <c r="A80" t="s">
+        <v>146</v>
+      </c>
+      <c r="C80" t="s">
+        <v>69</v>
+      </c>
+      <c r="D80" t="s">
+        <v>57</v>
+      </c>
+      <c r="K80" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="81" spans="1:11">
+      <c r="A81" t="s">
+        <v>446</v>
+      </c>
+      <c r="C81" t="s">
+        <v>69</v>
+      </c>
+      <c r="D81" t="s">
+        <v>447</v>
+      </c>
+      <c r="K81" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="82" spans="1:11">
+      <c r="A82" t="s">
+        <v>507</v>
+      </c>
+      <c r="C82" t="s">
+        <v>508</v>
+      </c>
+      <c r="D82" t="s">
+        <v>192</v>
+      </c>
+      <c r="K82" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="83" spans="1:11">
+      <c r="A83" t="s">
+        <v>669</v>
+      </c>
+      <c r="C83" t="s">
+        <v>508</v>
+      </c>
+      <c r="D83" t="s">
+        <v>670</v>
+      </c>
+      <c r="K83" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="84" spans="1:11">
+      <c r="A84" t="s">
+        <v>558</v>
+      </c>
+      <c r="C84" t="s">
+        <v>508</v>
+      </c>
+      <c r="D84" t="s">
+        <v>559</v>
+      </c>
+      <c r="K84" t="s">
+        <v>560</v>
+      </c>
+    </row>
+    <row r="85" spans="1:11">
+      <c r="A85" t="s">
+        <v>657</v>
+      </c>
+      <c r="C85" t="s">
+        <v>508</v>
+      </c>
+      <c r="D85" t="s">
+        <v>658</v>
+      </c>
+      <c r="K85" t="s">
+        <v>659</v>
+      </c>
+    </row>
+    <row r="86" spans="1:11">
+      <c r="B86" t="s">
+        <v>17</v>
+      </c>
+      <c r="C86" t="s">
+        <v>395</v>
+      </c>
+      <c r="D86" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="87" spans="1:11">
+      <c r="B87" t="s">
+        <v>17</v>
+      </c>
+      <c r="C87" t="s">
+        <v>395</v>
+      </c>
+      <c r="D87" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="88" spans="1:11">
+      <c r="B88" t="s">
+        <v>17</v>
+      </c>
+      <c r="C88" t="s">
+        <v>494</v>
+      </c>
+      <c r="D88" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="89" spans="1:11">
+      <c r="B89" t="s">
+        <v>17</v>
+      </c>
+      <c r="C89" t="s">
+        <v>494</v>
+      </c>
+      <c r="D89" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="90" spans="1:11">
+      <c r="B90" t="s">
+        <v>17</v>
+      </c>
+      <c r="C90" t="s">
+        <v>494</v>
+      </c>
+      <c r="D90" t="s">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="91" spans="1:11">
+      <c r="B91" t="s">
+        <v>17</v>
+      </c>
+      <c r="C91" t="s">
+        <v>494</v>
+      </c>
+      <c r="D91" t="s">
+        <v>740</v>
+      </c>
+    </row>
+    <row r="92" spans="1:11">
+      <c r="A92" t="s">
+        <v>377</v>
+      </c>
+      <c r="C92" t="s">
+        <v>346</v>
+      </c>
+      <c r="D92" t="s">
+        <v>378</v>
+      </c>
+      <c r="K92" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="93" spans="1:11">
+      <c r="B93" t="s">
+        <v>17</v>
+      </c>
+      <c r="C93" t="s">
+        <v>60</v>
+      </c>
+      <c r="D93" t="s">
+        <v>242</v>
+      </c>
+      <c r="K93" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="94" spans="1:11">
+      <c r="B94" t="s">
+        <v>17</v>
+      </c>
+      <c r="C94" t="s">
+        <v>60</v>
+      </c>
+      <c r="D94" t="s">
+        <v>288</v>
+      </c>
+      <c r="K94" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="95" spans="1:11">
+      <c r="B95" t="s">
+        <v>17</v>
+      </c>
+      <c r="C95" t="s">
+        <v>60</v>
+      </c>
+      <c r="D95" t="s">
+        <v>61</v>
+      </c>
+      <c r="K95" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="96" spans="1:11">
+      <c r="A96" t="s">
+        <v>148</v>
+      </c>
+      <c r="C96" t="s">
+        <v>60</v>
+      </c>
+      <c r="D96" t="s">
+        <v>149</v>
+      </c>
+      <c r="K96" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="97" spans="1:11">
+      <c r="B97" t="s">
+        <v>17</v>
+      </c>
+      <c r="C97" t="s">
+        <v>196</v>
+      </c>
+      <c r="D97" t="s">
+        <v>751</v>
+      </c>
+    </row>
+    <row r="98" spans="1:11">
+      <c r="A98" t="s">
+        <v>719</v>
+      </c>
+      <c r="C98" t="s">
+        <v>196</v>
+      </c>
+      <c r="D98" t="s">
+        <v>720</v>
+      </c>
+      <c r="K98" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="99" spans="1:11">
+      <c r="B99" t="s">
+        <v>17</v>
+      </c>
+      <c r="C99" t="s">
+        <v>198</v>
+      </c>
+      <c r="D99" t="s">
+        <v>199</v>
+      </c>
+      <c r="K99" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="100" spans="1:11">
+      <c r="B100" t="s">
+        <v>17</v>
+      </c>
+      <c r="C100" t="s">
+        <v>32</v>
+      </c>
+      <c r="D100" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="101" spans="1:11">
+      <c r="A101" t="s">
+        <v>811</v>
+      </c>
+      <c r="C101" t="s">
+        <v>32</v>
+      </c>
+      <c r="D101" t="s">
+        <v>812</v>
+      </c>
+    </row>
+    <row r="102" spans="1:11">
+      <c r="A102" t="s">
+        <v>218</v>
+      </c>
+      <c r="C102" t="s">
+        <v>32</v>
+      </c>
+      <c r="D102" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="103" spans="1:11">
+      <c r="A103" t="s">
+        <v>132</v>
+      </c>
+      <c r="C103" t="s">
+        <v>32</v>
+      </c>
+      <c r="D103" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="104" spans="1:11">
+      <c r="C104" t="s">
+        <v>32</v>
+      </c>
+      <c r="D104" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="105" spans="1:11">
+      <c r="A105" t="s">
+        <v>536</v>
+      </c>
+      <c r="C105" t="s">
+        <v>32</v>
+      </c>
+      <c r="D105" t="s">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="106" spans="1:11">
+      <c r="C106" t="s">
+        <v>32</v>
+      </c>
+      <c r="D106" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="107" spans="1:11">
+      <c r="C107" t="s">
+        <v>32</v>
+      </c>
+      <c r="D107" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="108" spans="1:11">
+      <c r="C108" t="s">
+        <v>32</v>
+      </c>
+      <c r="D108" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="109" spans="1:11">
+      <c r="C109" t="s">
+        <v>32</v>
+      </c>
+      <c r="D109" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="110" spans="1:11">
+      <c r="C110" t="s">
+        <v>32</v>
+      </c>
+      <c r="D110" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="111" spans="1:11">
+      <c r="C111" t="s">
+        <v>32</v>
+      </c>
+      <c r="D111" t="s">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="112" spans="1:11">
+      <c r="A112" t="s">
+        <v>254</v>
+      </c>
+      <c r="C112" t="s">
+        <v>32</v>
+      </c>
+      <c r="D112" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="113" spans="1:11">
+      <c r="A113" t="s">
+        <v>796</v>
+      </c>
+      <c r="C113" t="s">
+        <v>32</v>
+      </c>
+      <c r="D113" t="s">
+        <v>797</v>
+      </c>
+    </row>
+    <row r="114" spans="1:11">
+      <c r="A114" t="s">
+        <v>264</v>
+      </c>
+      <c r="C114" t="s">
+        <v>265</v>
+      </c>
+      <c r="D114" t="s">
+        <v>266</v>
+      </c>
+      <c r="K114" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="115" spans="1:11">
+      <c r="A115" t="s">
+        <v>23</v>
+      </c>
+      <c r="C115" t="s">
+        <v>24</v>
+      </c>
+      <c r="D115" t="s">
+        <v>25</v>
+      </c>
+      <c r="K115" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="116" spans="1:11">
+      <c r="A116" t="s">
+        <v>189</v>
+      </c>
+      <c r="C116" t="s">
+        <v>24</v>
+      </c>
+      <c r="D116" t="s">
+        <v>186</v>
+      </c>
+      <c r="K116" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="117" spans="1:11">
+      <c r="A117" t="s">
+        <v>144</v>
+      </c>
+      <c r="C117" t="s">
+        <v>24</v>
+      </c>
+      <c r="D117" t="s">
+        <v>60</v>
+      </c>
+      <c r="K117" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="118" spans="1:11">
+      <c r="A118" t="s">
+        <v>630</v>
+      </c>
+      <c r="C118" t="s">
+        <v>108</v>
+      </c>
+      <c r="D118" t="s">
+        <v>631</v>
+      </c>
+      <c r="K118" t="s">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="119" spans="1:11">
+      <c r="A119" t="s">
+        <v>205</v>
+      </c>
+      <c r="C119" t="s">
+        <v>108</v>
+      </c>
+      <c r="D119" t="s">
+        <v>206</v>
+      </c>
+      <c r="K119" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="120" spans="1:11">
+      <c r="A120" t="s">
+        <v>362</v>
+      </c>
+      <c r="C120" t="s">
+        <v>108</v>
+      </c>
+      <c r="D120" t="s">
+        <v>363</v>
+      </c>
+      <c r="K120" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="121" spans="1:11">
+      <c r="B121" t="s">
+        <v>17</v>
+      </c>
+      <c r="C121" t="s">
+        <v>12</v>
+      </c>
+      <c r="D121" t="s">
+        <v>350</v>
+      </c>
+      <c r="K121" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="122" spans="1:11">
+      <c r="B122" t="s">
+        <v>17</v>
+      </c>
+      <c r="C122" t="s">
+        <v>12</v>
+      </c>
+      <c r="D122" t="s">
+        <v>388</v>
+      </c>
+      <c r="K122" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="123" spans="1:11">
+      <c r="B123" t="s">
+        <v>17</v>
+      </c>
+      <c r="C123" t="s">
+        <v>12</v>
+      </c>
+      <c r="D123" t="s">
+        <v>762</v>
+      </c>
+      <c r="K123" t="s">
+        <v>763</v>
+      </c>
+    </row>
+    <row r="124" spans="1:11">
+      <c r="B124" t="s">
+        <v>17</v>
+      </c>
+      <c r="C124" t="s">
+        <v>12</v>
+      </c>
+      <c r="D124" t="s">
+        <v>476</v>
+      </c>
+      <c r="K124" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="125" spans="1:11">
+      <c r="A125" t="s">
+        <v>644</v>
+      </c>
+      <c r="B125" t="s">
+        <v>17</v>
+      </c>
+      <c r="C125" t="s">
+        <v>12</v>
+      </c>
+      <c r="D125" t="s">
+        <v>645</v>
+      </c>
+    </row>
+    <row r="126" spans="1:11">
+      <c r="A126" t="s">
+        <v>268</v>
+      </c>
+      <c r="B126" t="s">
+        <v>17</v>
+      </c>
+      <c r="C126" t="s">
+        <v>12</v>
+      </c>
+      <c r="D126" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="127" spans="1:11">
+      <c r="A127" t="s">
+        <v>268</v>
+      </c>
+      <c r="B127" t="s">
+        <v>17</v>
+      </c>
+      <c r="C127" t="s">
+        <v>12</v>
+      </c>
+      <c r="D127" t="s">
+        <v>590</v>
+      </c>
+    </row>
+    <row r="128" spans="1:11">
+      <c r="B128" t="s">
+        <v>17</v>
+      </c>
+      <c r="C128" t="s">
+        <v>12</v>
+      </c>
+      <c r="D128" t="s">
+        <v>357</v>
+      </c>
+      <c r="K128" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="129" spans="1:11">
+      <c r="B129" t="s">
+        <v>17</v>
+      </c>
+      <c r="C129" t="s">
+        <v>12</v>
+      </c>
+      <c r="D129" t="s">
+        <v>390</v>
+      </c>
+      <c r="K129" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="130" spans="1:11">
+      <c r="B130" t="s">
+        <v>17</v>
+      </c>
+      <c r="C130" t="s">
+        <v>12</v>
+      </c>
+      <c r="D130" t="s">
+        <v>679</v>
+      </c>
+      <c r="K130" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="131" spans="1:11">
+      <c r="B131" t="s">
+        <v>17</v>
+      </c>
+      <c r="C131" t="s">
+        <v>12</v>
+      </c>
+      <c r="D131" t="s">
+        <v>646</v>
+      </c>
+      <c r="K131" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="132" spans="1:11">
+      <c r="B132" t="s">
+        <v>17</v>
+      </c>
+      <c r="C132" t="s">
+        <v>12</v>
+      </c>
+      <c r="D132" t="s">
+        <v>306</v>
+      </c>
+      <c r="K132" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="133" spans="1:11">
+      <c r="B133" t="s">
+        <v>17</v>
+      </c>
+      <c r="C133" t="s">
+        <v>12</v>
+      </c>
+      <c r="D133" t="s">
+        <v>381</v>
+      </c>
+      <c r="K133" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="134" spans="1:11">
+      <c r="B134" t="s">
+        <v>17</v>
+      </c>
+      <c r="C134" t="s">
+        <v>12</v>
+      </c>
+      <c r="D134" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="135" spans="1:11">
+      <c r="B135" t="s">
+        <v>17</v>
+      </c>
+      <c r="C135" t="s">
+        <v>12</v>
+      </c>
+      <c r="D135" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="136" spans="1:11">
+      <c r="B136" t="s">
+        <v>17</v>
+      </c>
+      <c r="C136" t="s">
+        <v>12</v>
+      </c>
+      <c r="D136" t="s">
+        <v>538</v>
+      </c>
+      <c r="K136" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="137" spans="1:11">
+      <c r="B137" t="s">
+        <v>17</v>
+      </c>
+      <c r="C137" t="s">
+        <v>12</v>
+      </c>
+      <c r="D137" t="s">
+        <v>461</v>
+      </c>
+      <c r="K137" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="138" spans="1:11">
+      <c r="B138" t="s">
+        <v>17</v>
+      </c>
+      <c r="C138" t="s">
+        <v>12</v>
+      </c>
+      <c r="D138" t="s">
+        <v>247</v>
+      </c>
+      <c r="K138" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="139" spans="1:11">
+      <c r="A139" t="s">
+        <v>49</v>
+      </c>
+      <c r="C139" t="s">
+        <v>12</v>
+      </c>
+      <c r="D139" t="s">
+        <v>50</v>
+      </c>
+      <c r="K139" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="140" spans="1:11">
+      <c r="A140" t="s">
+        <v>567</v>
+      </c>
+      <c r="C140" t="s">
+        <v>12</v>
+      </c>
+      <c r="D140" t="s">
+        <v>568</v>
+      </c>
+      <c r="K140" t="s">
+        <v>569</v>
+      </c>
+    </row>
+    <row r="141" spans="1:11">
+      <c r="A141" t="s">
+        <v>717</v>
+      </c>
+      <c r="C141" t="s">
+        <v>12</v>
+      </c>
+      <c r="D141" t="s">
+        <v>718</v>
+      </c>
+    </row>
+    <row r="142" spans="1:11">
+      <c r="A142" t="s">
+        <v>755</v>
+      </c>
+      <c r="C142" t="s">
+        <v>12</v>
+      </c>
+      <c r="D142" t="s">
+        <v>756</v>
+      </c>
+      <c r="K142" t="s">
+        <v>757</v>
+      </c>
+    </row>
+    <row r="143" spans="1:11">
+      <c r="A143" t="s">
+        <v>11</v>
+      </c>
+      <c r="C143" t="s">
+        <v>12</v>
+      </c>
+      <c r="D143" t="s">
+        <v>13</v>
+      </c>
+      <c r="K143" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="144" spans="1:11">
+      <c r="A144" t="s">
+        <v>547</v>
+      </c>
+      <c r="C144" t="s">
+        <v>12</v>
+      </c>
+      <c r="D144" t="s">
+        <v>548</v>
+      </c>
+      <c r="K144" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="145" spans="1:12">
+      <c r="C145" t="s">
+        <v>12</v>
+      </c>
+      <c r="D145" t="s">
+        <v>636</v>
+      </c>
+      <c r="K145" t="s">
+        <v>636</v>
+      </c>
+    </row>
+    <row r="146" spans="1:12">
+      <c r="A146" t="s">
+        <v>82</v>
+      </c>
+      <c r="C146" t="s">
+        <v>12</v>
+      </c>
+      <c r="D146" t="s">
+        <v>83</v>
+      </c>
+      <c r="K146" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="147" spans="1:12">
+      <c r="C147" t="s">
+        <v>12</v>
+      </c>
+      <c r="D147" t="s">
+        <v>319</v>
+      </c>
+      <c r="K147" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="148" spans="1:12">
+      <c r="A148" t="s">
+        <v>705</v>
+      </c>
+      <c r="C148" t="s">
+        <v>12</v>
+      </c>
+      <c r="D148" t="s">
+        <v>706</v>
+      </c>
+      <c r="K148" t="s">
+        <v>707</v>
+      </c>
+    </row>
+    <row r="149" spans="1:12">
+      <c r="B149" t="s">
+        <v>17</v>
+      </c>
+      <c r="C149" t="s">
+        <v>165</v>
+      </c>
+      <c r="D149" t="s">
+        <v>529</v>
+      </c>
+      <c r="K149" t="s">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="153" spans="1:12">
+      <c r="A153" t="s">
+        <v>7</v>
+      </c>
+      <c r="C153" t="s">
+        <v>8</v>
+      </c>
+      <c r="D153" t="s">
+        <v>9</v>
+      </c>
+      <c r="F153" t="s">
+        <v>9</v>
+      </c>
+      <c r="H153" t="s">
+        <v>859</v>
+      </c>
+      <c r="K153" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="154" spans="1:12">
+      <c r="B154" t="s">
+        <v>17</v>
+      </c>
+      <c r="C154" t="s">
+        <v>60</v>
+      </c>
+      <c r="D154" t="s">
+        <v>386</v>
+      </c>
+      <c r="F154" t="s">
+        <v>891</v>
+      </c>
+      <c r="H154" s="1" t="s">
+        <v>889</v>
+      </c>
+      <c r="I154" s="1"/>
+      <c r="J154" s="1"/>
+      <c r="K154" t="s">
+        <v>387</v>
+      </c>
+      <c r="L154" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="159" spans="1:12">
+      <c r="A159" t="s">
+        <v>2069</v>
+      </c>
+      <c r="B159" t="s">
+        <v>3354</v>
+      </c>
+      <c r="C159" t="s">
+        <v>3291</v>
+      </c>
+    </row>
+    <row r="160" spans="1:12">
+      <c r="B160" t="s">
+        <v>1218</v>
+      </c>
+      <c r="C160" t="s">
+        <v>3355</v>
+      </c>
+    </row>
+    <row r="161" spans="1:11">
+      <c r="B161" t="s">
+        <v>3356</v>
+      </c>
+      <c r="C161" t="s">
+        <v>3357</v>
+      </c>
+    </row>
+    <row r="162" spans="1:11">
+      <c r="C162" t="s">
+        <v>3358</v>
+      </c>
+    </row>
+    <row r="163" spans="1:11">
+      <c r="B163" t="s">
+        <v>3359</v>
+      </c>
+    </row>
+    <row r="165" spans="1:11">
+      <c r="A165" t="s">
+        <v>3360</v>
+      </c>
+    </row>
+    <row r="166" spans="1:11">
+      <c r="B166" t="s">
+        <v>3361</v>
+      </c>
+    </row>
+    <row r="167" spans="1:11">
+      <c r="C167" t="s">
+        <v>3362</v>
+      </c>
+    </row>
+    <row r="171" spans="1:11">
+      <c r="A171" t="s">
+        <v>3379</v>
+      </c>
+    </row>
+    <row r="172" spans="1:11">
+      <c r="A172" t="s">
+        <v>285</v>
+      </c>
+      <c r="C172" t="s">
+        <v>100</v>
+      </c>
+      <c r="D172" t="s">
+        <v>94</v>
+      </c>
+      <c r="J172" t="s">
+        <v>3346</v>
+      </c>
+      <c r="K172" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="173" spans="1:11">
+      <c r="A173" t="s">
+        <v>771</v>
+      </c>
+      <c r="C173" t="s">
+        <v>664</v>
+      </c>
+      <c r="D173" t="s">
+        <v>772</v>
+      </c>
+      <c r="E173" t="s">
+        <v>3336</v>
+      </c>
+      <c r="F173" s="1" t="s">
+        <v>3337</v>
+      </c>
+      <c r="I173" t="s">
+        <v>3338</v>
+      </c>
+      <c r="J173" t="s">
+        <v>3339</v>
+      </c>
+      <c r="K173" t="s">
+        <v>773</v>
+      </c>
+    </row>
+    <row r="174" spans="1:11">
+      <c r="A174" t="s">
+        <v>43</v>
+      </c>
+      <c r="C174" t="s">
+        <v>44</v>
+      </c>
+      <c r="D174" t="s">
+        <v>45</v>
+      </c>
+      <c r="E174" t="s">
+        <v>3374</v>
+      </c>
+      <c r="F174" t="s">
+        <v>3373</v>
+      </c>
+      <c r="J174" t="s">
+        <v>3375</v>
+      </c>
+      <c r="K174" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="175" spans="1:11">
+      <c r="A175" t="s">
+        <v>258</v>
+      </c>
+      <c r="C175" t="s">
+        <v>259</v>
+      </c>
+      <c r="D175" t="s">
+        <v>260</v>
+      </c>
+      <c r="K175" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="176" spans="1:11">
+      <c r="A176" t="s">
+        <v>316</v>
+      </c>
+      <c r="C176" t="s">
+        <v>259</v>
+      </c>
+      <c r="D176" t="s">
+        <v>317</v>
+      </c>
+      <c r="K176" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="177" spans="1:11">
+      <c r="A177" t="s">
+        <v>392</v>
+      </c>
+      <c r="C177" t="s">
+        <v>260</v>
+      </c>
+      <c r="D177" t="s">
+        <v>393</v>
+      </c>
+      <c r="G177" t="s">
+        <v>3378</v>
+      </c>
+      <c r="J177" t="s">
+        <v>3376</v>
+      </c>
+      <c r="K177" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="178" spans="1:11">
+      <c r="A178" t="s">
+        <v>468</v>
+      </c>
+      <c r="C178" t="s">
+        <v>260</v>
+      </c>
+      <c r="D178" t="s">
+        <v>469</v>
+      </c>
+      <c r="G178" t="s">
+        <v>954</v>
+      </c>
+      <c r="J178" t="s">
+        <v>3377</v>
+      </c>
+      <c r="K178" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="179" spans="1:11">
+      <c r="A179" t="s">
+        <v>611</v>
+      </c>
+      <c r="C179" t="s">
+        <v>155</v>
+      </c>
+      <c r="D179" t="s">
+        <v>612</v>
+      </c>
+      <c r="K179" t="s">
+        <v>613</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="H154" r:id="rId1"/>
+    <hyperlink ref="H44" r:id="rId2"/>
+    <hyperlink ref="H45" r:id="rId3"/>
+    <hyperlink ref="F173" r:id="rId4"/>
+    <hyperlink ref="F14" r:id="rId5"/>
+    <hyperlink ref="F18" r:id="rId6"/>
+    <hyperlink ref="F19" r:id="rId7"/>
+    <hyperlink ref="F64" r:id="rId8"/>
+  </hyperlinks>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" r:id="rId9"/>
+  <headerFooter alignWithMargins="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:M50"/>
+  <sheetViews>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75"/>
+  <cols>
+    <col min="1" max="1" width="40" customWidth="1"/>
+    <col min="2" max="3" width="12.375" customWidth="1"/>
+    <col min="4" max="4" width="40.875" customWidth="1"/>
+    <col min="5" max="5" width="22.75" customWidth="1"/>
+    <col min="6" max="6" width="38.125" customWidth="1"/>
+    <col min="7" max="7" width="39.375" customWidth="1"/>
+    <col min="8" max="8" width="22.625" customWidth="1"/>
+    <col min="9" max="9" width="43.75" customWidth="1"/>
+    <col min="10" max="10" width="34.5" customWidth="1"/>
+    <col min="11" max="11" width="19" customWidth="1"/>
+    <col min="12" max="12" width="40.875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13">
+      <c r="B1" t="s">
+        <v>3199</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3407</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3331</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3389</v>
+      </c>
+      <c r="F1" t="s">
+        <v>3382</v>
+      </c>
+      <c r="G1" t="s">
+        <v>3383</v>
+      </c>
+      <c r="H1" t="s">
+        <v>3384</v>
+      </c>
+      <c r="J1" t="s">
+        <v>3398</v>
+      </c>
+      <c r="K1" t="s">
+        <v>3391</v>
+      </c>
+      <c r="L1" t="s">
+        <v>3392</v>
+      </c>
+      <c r="M1" t="s">
+        <v>818</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13">
+      <c r="A2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3387</v>
+      </c>
+      <c r="D2" t="s">
+        <v>3388</v>
+      </c>
+      <c r="E2" t="s">
+        <v>3390</v>
+      </c>
+      <c r="F2" t="s">
+        <v>3380</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>3381</v>
+      </c>
+      <c r="H2" t="s">
+        <v>3386</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>3385</v>
+      </c>
+      <c r="J2" s="1"/>
+      <c r="K2" t="s">
+        <v>3394</v>
+      </c>
+      <c r="L2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13">
+      <c r="F3" t="s">
+        <v>3393</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>3395</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13">
+      <c r="A4" t="s">
+        <v>66</v>
+      </c>
+      <c r="B4" t="s">
+        <v>3387</v>
+      </c>
+      <c r="D4" t="s">
+        <v>3402</v>
+      </c>
+      <c r="E4" t="s">
+        <v>3405</v>
+      </c>
+      <c r="F4" t="s">
+        <v>3397</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>3400</v>
+      </c>
+      <c r="H4" t="s">
+        <v>2290</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>2291</v>
+      </c>
+      <c r="J4" t="s">
+        <v>3399</v>
+      </c>
+      <c r="K4" t="s">
+        <v>3396</v>
+      </c>
+      <c r="L4" t="s">
+        <v>67</v>
+      </c>
+      <c r="M4" t="s">
+        <v>3403</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13">
+      <c r="A5" t="s">
+        <v>72</v>
+      </c>
+      <c r="B5" t="s">
+        <v>3387</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>3404</v>
+      </c>
+      <c r="D5" t="s">
+        <v>3401</v>
+      </c>
+      <c r="E5" t="s">
+        <v>3390</v>
+      </c>
+      <c r="K5" t="s">
+        <v>3406</v>
+      </c>
+      <c r="L5" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13">
+      <c r="A6" t="s">
+        <v>76</v>
+      </c>
+      <c r="B6" t="s">
+        <v>3408</v>
+      </c>
+      <c r="E6" t="s">
+        <v>1119</v>
+      </c>
+      <c r="J6" t="s">
+        <v>3409</v>
+      </c>
+      <c r="L6" t="s">
+        <v>3410</v>
+      </c>
+      <c r="M6" t="s">
+        <v>3411</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13">
+      <c r="A7" t="s">
+        <v>98</v>
+      </c>
+      <c r="M7" t="s">
+        <v>3412</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11">
+      <c r="B17" t="s">
+        <v>17</v>
+      </c>
+      <c r="C17" t="s">
+        <v>18</v>
+      </c>
+      <c r="D17" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11">
+      <c r="B18" t="s">
+        <v>17</v>
+      </c>
+      <c r="C18" t="s">
+        <v>18</v>
+      </c>
+      <c r="D18" t="s">
+        <v>216</v>
+      </c>
+      <c r="K18" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11">
+      <c r="B19" t="s">
+        <v>17</v>
+      </c>
+      <c r="C19" t="s">
+        <v>18</v>
+      </c>
+      <c r="D19" t="s">
+        <v>256</v>
+      </c>
+      <c r="K19" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11">
+      <c r="B20" t="s">
+        <v>17</v>
+      </c>
+      <c r="C20" t="s">
+        <v>18</v>
+      </c>
+      <c r="D20" t="s">
+        <v>283</v>
+      </c>
+      <c r="K20" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11">
+      <c r="B21" t="s">
+        <v>17</v>
+      </c>
+      <c r="C21" t="s">
+        <v>18</v>
+      </c>
+      <c r="D21" t="s">
+        <v>326</v>
+      </c>
+      <c r="K21" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11">
+      <c r="B22" t="s">
+        <v>17</v>
+      </c>
+      <c r="C22" t="s">
+        <v>18</v>
+      </c>
+      <c r="D22" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11">
+      <c r="B23" t="s">
+        <v>17</v>
+      </c>
+      <c r="C23" t="s">
+        <v>18</v>
+      </c>
+      <c r="D23" t="s">
+        <v>372</v>
+      </c>
+      <c r="K23" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11">
+      <c r="B24" t="s">
+        <v>17</v>
+      </c>
+      <c r="C24" t="s">
+        <v>18</v>
+      </c>
+      <c r="D24" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11">
+      <c r="B25" t="s">
+        <v>17</v>
+      </c>
+      <c r="C25" t="s">
+        <v>18</v>
+      </c>
+      <c r="D25" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11">
+      <c r="B26" t="s">
+        <v>17</v>
+      </c>
+      <c r="C26" t="s">
+        <v>18</v>
+      </c>
+      <c r="D26" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11">
+      <c r="B27" t="s">
+        <v>17</v>
+      </c>
+      <c r="C27" t="s">
+        <v>18</v>
+      </c>
+      <c r="D27" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11">
+      <c r="B28" t="s">
+        <v>17</v>
+      </c>
+      <c r="C28" t="s">
+        <v>18</v>
+      </c>
+      <c r="D28" t="s">
+        <v>540</v>
+      </c>
+      <c r="K28" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11">
+      <c r="B29" t="s">
+        <v>17</v>
+      </c>
+      <c r="C29" t="s">
+        <v>18</v>
+      </c>
+      <c r="D29" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11">
+      <c r="B30" t="s">
+        <v>17</v>
+      </c>
+      <c r="C30" t="s">
+        <v>18</v>
+      </c>
+      <c r="D30" t="s">
+        <v>591</v>
+      </c>
+      <c r="K30" t="s">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11">
+      <c r="B31" t="s">
+        <v>17</v>
+      </c>
+      <c r="C31" t="s">
+        <v>18</v>
+      </c>
+      <c r="D31" t="s">
+        <v>596</v>
+      </c>
+      <c r="K31" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11">
+      <c r="A32" t="s">
+        <v>628</v>
+      </c>
+      <c r="B32" t="s">
+        <v>17</v>
+      </c>
+      <c r="C32" t="s">
+        <v>18</v>
+      </c>
+      <c r="D32" t="s">
+        <v>629</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11">
+      <c r="B33" t="s">
+        <v>17</v>
+      </c>
+      <c r="C33" t="s">
+        <v>18</v>
+      </c>
+      <c r="D33" t="s">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11">
+      <c r="B34" t="s">
+        <v>17</v>
+      </c>
+      <c r="C34" t="s">
+        <v>18</v>
+      </c>
+      <c r="D34" t="s">
+        <v>702</v>
+      </c>
+      <c r="K34" t="s">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11">
+      <c r="B35" t="s">
+        <v>17</v>
+      </c>
+      <c r="C35" t="s">
+        <v>18</v>
+      </c>
+      <c r="D35" t="s">
+        <v>715</v>
+      </c>
+      <c r="K35" t="s">
+        <v>716</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11">
+      <c r="B36" t="s">
+        <v>17</v>
+      </c>
+      <c r="C36" t="s">
+        <v>18</v>
+      </c>
+      <c r="D36" t="s">
+        <v>725</v>
+      </c>
+      <c r="K36" t="s">
+        <v>726</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11">
+      <c r="B37" t="s">
+        <v>17</v>
+      </c>
+      <c r="C37" t="s">
+        <v>18</v>
+      </c>
+      <c r="D37" t="s">
+        <v>795</v>
+      </c>
+      <c r="F37" t="s">
+        <v>3322</v>
+      </c>
+      <c r="H37" s="1" t="s">
+        <v>3323</v>
+      </c>
+      <c r="I37" s="1"/>
+      <c r="J37" s="1"/>
+    </row>
+    <row r="38" spans="1:11">
+      <c r="B38" t="s">
+        <v>17</v>
+      </c>
+      <c r="C38" t="s">
+        <v>18</v>
+      </c>
+      <c r="D38" t="s">
+        <v>798</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11">
+      <c r="B39" t="s">
+        <v>17</v>
+      </c>
+      <c r="C39" t="s">
+        <v>18</v>
+      </c>
+      <c r="D39" t="s">
+        <v>21</v>
+      </c>
+      <c r="F39" t="s">
+        <v>3321</v>
+      </c>
+      <c r="H39" t="s">
+        <v>3320</v>
+      </c>
+      <c r="K39" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11">
+      <c r="B40" t="s">
+        <v>17</v>
+      </c>
+      <c r="C40" t="s">
+        <v>18</v>
+      </c>
+      <c r="D40" t="s">
+        <v>220</v>
+      </c>
+      <c r="K40" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11">
+      <c r="B41" t="s">
+        <v>17</v>
+      </c>
+      <c r="C41" t="s">
+        <v>18</v>
+      </c>
+      <c r="D41" t="s">
+        <v>340</v>
+      </c>
+      <c r="K41" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11">
+      <c r="C42" t="s">
+        <v>18</v>
+      </c>
+      <c r="D42" t="s">
+        <v>312</v>
+      </c>
+      <c r="K42" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11">
+      <c r="C43" t="s">
+        <v>18</v>
+      </c>
+      <c r="D43" t="s">
+        <v>774</v>
+      </c>
+      <c r="K43" t="s">
+        <v>775</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11">
+      <c r="A44" t="s">
+        <v>550</v>
+      </c>
+      <c r="C44" t="s">
+        <v>18</v>
+      </c>
+      <c r="D44" t="s">
+        <v>551</v>
+      </c>
+      <c r="K44" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11">
+      <c r="C45" t="s">
+        <v>18</v>
+      </c>
+      <c r="D45" t="s">
+        <v>228</v>
+      </c>
+      <c r="K45" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11">
+      <c r="A46" t="s">
+        <v>335</v>
+      </c>
+      <c r="C46" t="s">
+        <v>18</v>
+      </c>
+      <c r="D46" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11">
+      <c r="A47" t="s">
+        <v>800</v>
+      </c>
+      <c r="C47" t="s">
+        <v>18</v>
+      </c>
+      <c r="D47" t="s">
+        <v>801</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11">
+      <c r="A48" t="s">
+        <v>74</v>
+      </c>
+      <c r="C48" t="s">
+        <v>18</v>
+      </c>
+      <c r="D48" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4">
+      <c r="A49" t="s">
+        <v>686</v>
+      </c>
+      <c r="C49" t="s">
+        <v>18</v>
+      </c>
+      <c r="D49" t="s">
+        <v>687</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4">
+      <c r="A50" t="s">
+        <v>686</v>
+      </c>
+      <c r="C50" t="s">
+        <v>18</v>
+      </c>
+      <c r="D50" t="s">
+        <v>704</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="G2" r:id="rId1"/>
+    <hyperlink ref="I2" r:id="rId2"/>
+    <hyperlink ref="G3" r:id="rId3"/>
+    <hyperlink ref="I4" r:id="rId4"/>
+    <hyperlink ref="G4" r:id="rId5"/>
+    <hyperlink ref="C5" r:id="rId6"/>
+    <hyperlink ref="H37" r:id="rId7"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:G92"/>
+  <sheetViews>
+    <sheetView topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="C76" sqref="C76"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
+  <cols>
+    <col min="3" max="3" width="31.5" customWidth="1"/>
+    <col min="4" max="4" width="27.25" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" t="s">
@@ -11926,13 +15177,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H665"/>
+  <dimension ref="A1:K672"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A648" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D24" sqref="D24"/>
+      <selection pane="bottomLeft" activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -24676,7 +27927,7 @@
         <v>654</v>
       </c>
     </row>
-    <row r="657" spans="1:8">
+    <row r="657" spans="1:11">
       <c r="B657" t="s">
         <v>17</v>
       </c>
@@ -24693,7 +27944,7 @@
         <v>3151</v>
       </c>
     </row>
-    <row r="658" spans="1:8">
+    <row r="658" spans="1:11">
       <c r="B658" t="s">
         <v>17</v>
       </c>
@@ -24710,7 +27961,7 @@
         <v>844</v>
       </c>
     </row>
-    <row r="659" spans="1:8">
+    <row r="659" spans="1:11">
       <c r="A659" t="s">
         <v>230</v>
       </c>
@@ -24730,7 +27981,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="660" spans="1:8">
+    <row r="660" spans="1:11">
       <c r="A660" t="s">
         <v>3152</v>
       </c>
@@ -24747,7 +27998,7 @@
         <v>3155</v>
       </c>
     </row>
-    <row r="661" spans="1:8">
+    <row r="661" spans="1:11">
       <c r="A661" t="s">
         <v>3156</v>
       </c>
@@ -24764,7 +28015,7 @@
         <v>3159</v>
       </c>
     </row>
-    <row r="662" spans="1:8">
+    <row r="662" spans="1:11">
       <c r="A662" t="s">
         <v>3160</v>
       </c>
@@ -24781,7 +28032,7 @@
         <v>3163</v>
       </c>
     </row>
-    <row r="663" spans="1:8">
+    <row r="663" spans="1:11">
       <c r="A663" t="s">
         <v>3164</v>
       </c>
@@ -24798,7 +28049,7 @@
         <v>3167</v>
       </c>
     </row>
-    <row r="664" spans="1:8">
+    <row r="664" spans="1:11">
       <c r="A664" t="s">
         <v>3168</v>
       </c>
@@ -24815,7 +28066,7 @@
         <v>3171</v>
       </c>
     </row>
-    <row r="665" spans="1:8">
+    <row r="665" spans="1:11">
       <c r="A665" t="s">
         <v>449</v>
       </c>
@@ -24833,6 +28084,26 @@
       </c>
       <c r="H665" t="s">
         <v>451</v>
+      </c>
+    </row>
+    <row r="672" spans="1:11">
+      <c r="A672" t="s">
+        <v>624</v>
+      </c>
+      <c r="C672" t="s">
+        <v>625</v>
+      </c>
+      <c r="D672" t="s">
+        <v>626</v>
+      </c>
+      <c r="E672" t="s">
+        <v>3418</v>
+      </c>
+      <c r="F672" s="1" t="s">
+        <v>3417</v>
+      </c>
+      <c r="K672" t="s">
+        <v>627</v>
       </c>
     </row>
   </sheetData>
@@ -24901,20 +28172,21 @@
     <hyperlink ref="F579" r:id="rId59"/>
     <hyperlink ref="F585" r:id="rId60"/>
     <hyperlink ref="F70" r:id="rId61"/>
+    <hyperlink ref="F672" r:id="rId62"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId62"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId63"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H188"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A39" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D40" sqref="D40"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D42" sqref="D42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -27439,7 +30711,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H4"/>
   <sheetViews>
@@ -27510,7 +30782,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E32"/>
   <sheetViews>
@@ -27982,12 +31254,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I73"/>
   <sheetViews>
-    <sheetView topLeftCell="A59" workbookViewId="0">
-      <selection activeCell="B76" sqref="B76"/>
+    <sheetView topLeftCell="A47" workbookViewId="0">
+      <selection activeCell="L49" sqref="L49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -28026,7 +31298,7 @@
       <c r="A2" s="18" t="s">
         <v>3193</v>
       </c>
-      <c r="B2" s="41">
+      <c r="B2" s="42">
         <v>198</v>
       </c>
       <c r="C2" s="18">
@@ -28044,7 +31316,7 @@
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="18"/>
-      <c r="B3" s="41"/>
+      <c r="B3" s="42"/>
       <c r="C3" s="18">
         <v>450</v>
       </c>
@@ -28065,7 +31337,7 @@
       <c r="A4" s="18" t="s">
         <v>3196</v>
       </c>
-      <c r="B4" s="41">
+      <c r="B4" s="42">
         <v>46</v>
       </c>
       <c r="C4" s="18">
@@ -28083,7 +31355,7 @@
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="18"/>
-      <c r="B5" s="41"/>
+      <c r="B5" s="42"/>
       <c r="C5" s="18">
         <v>309</v>
       </c>
@@ -28196,7 +31468,7 @@
       <c r="A10" s="18" t="s">
         <v>3214</v>
       </c>
-      <c r="B10" s="41">
+      <c r="B10" s="42">
         <v>33</v>
       </c>
       <c r="C10" s="18">
@@ -28214,7 +31486,7 @@
     </row>
     <row r="11" spans="1:8">
       <c r="A11" s="18"/>
-      <c r="B11" s="41"/>
+      <c r="B11" s="42"/>
       <c r="C11" s="18">
         <v>70</v>
       </c>
@@ -28235,7 +31507,7 @@
       <c r="A12" s="19" t="s">
         <v>3253</v>
       </c>
-      <c r="B12" s="42">
+      <c r="B12" s="43">
         <v>11</v>
       </c>
       <c r="C12" s="19">
@@ -28256,7 +31528,7 @@
     </row>
     <row r="13" spans="1:8">
       <c r="A13" s="18"/>
-      <c r="B13" s="42"/>
+      <c r="B13" s="43"/>
       <c r="C13" s="19">
         <v>333</v>
       </c>
@@ -28277,7 +31549,7 @@
       <c r="A14" s="19" t="s">
         <v>3205</v>
       </c>
-      <c r="B14" s="42">
+      <c r="B14" s="43">
         <v>141</v>
       </c>
       <c r="C14" s="19">
@@ -28298,7 +31570,7 @@
     </row>
     <row r="15" spans="1:8">
       <c r="A15" s="18"/>
-      <c r="B15" s="42"/>
+      <c r="B15" s="43"/>
       <c r="C15" s="18">
         <v>1206</v>
       </c>
@@ -29185,7 +32457,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E54"/>
   <sheetViews>

</xml_diff>

<commit_message>
worked on unmapped terms
</commit_message>
<xml_diff>
--- a/doc/mapping results/termsMapping.xlsx
+++ b/doc/mapping results/termsMapping.xlsx
@@ -4,16 +4,16 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr date1904="1"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="-15" windowWidth="12615" windowHeight="11760" tabRatio="852" activeTab="1"/>
+    <workbookView xWindow="-15" yWindow="-15" windowWidth="12615" windowHeight="11760" tabRatio="852"/>
   </bookViews>
   <sheets>
     <sheet name="terms2add" sheetId="9" r:id="rId1"/>
     <sheet name="terms2add-cell type" sheetId="10" r:id="rId2"/>
     <sheet name="terms2add-cell line" sheetId="11" r:id="rId3"/>
-    <sheet name="terms2ignore" sheetId="2" r:id="rId4"/>
-    <sheet name="mappedTerms" sheetId="3" r:id="rId5"/>
-    <sheet name="terms2submit" sheetId="4" r:id="rId6"/>
-    <sheet name="termsInBCGO" sheetId="8" r:id="rId7"/>
+    <sheet name="termsAdded-BCGO" sheetId="8" r:id="rId4"/>
+    <sheet name="terms2ignore" sheetId="2" r:id="rId5"/>
+    <sheet name="mappedTerms" sheetId="3" r:id="rId6"/>
+    <sheet name="terms2submit" sheetId="4" r:id="rId7"/>
     <sheet name="StrainOrLine_Emily" sheetId="5" r:id="rId8"/>
     <sheet name="Summary of Subset" sheetId="6" r:id="rId9"/>
     <sheet name="Summary of Mapping" sheetId="7" r:id="rId10"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6210" uniqueCount="3468">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6273" uniqueCount="3517">
   <si>
     <t>MO URI</t>
   </si>
@@ -10074,9 +10074,6 @@
     <t>obi has freezing storage. Could add freezing, and set freezing storage has part freezing</t>
   </si>
   <si>
-    <t xml:space="preserve">process or planned process, can we think quality changes as material transformation? </t>
-  </si>
-  <si>
     <t>Do we need this term without any subclasses (glass, nylon, etc.) included? If we need, how about coating material, and add coating role</t>
   </si>
   <si>
@@ -10098,9 +10095,6 @@
     <t>http://purl.obolibrary.org/obo/PATO_0001241</t>
   </si>
   <si>
-    <t>is it data analysis objective? Do we need the specific study design type for it? Is transcription profiling design enough?</t>
-  </si>
-  <si>
     <t>technology</t>
   </si>
   <si>
@@ -10146,9 +10140,6 @@
     <t>observation record</t>
   </si>
   <si>
-    <t xml:space="preserve">data item </t>
-  </si>
-  <si>
     <t>A data item that records examination of material entity with unaided eyes.</t>
   </si>
   <si>
@@ -10248,9 +10239,6 @@
     <t>hepatic stem cell</t>
   </si>
   <si>
-    <t>postnatal day 60</t>
-  </si>
-  <si>
     <t>http://purl.oblibrary.org/obo/bcgo/BCGO_0000015</t>
   </si>
   <si>
@@ -10266,12 +10254,6 @@
     <t>unit per liter</t>
   </si>
   <si>
-    <t>Should be in IAO</t>
-  </si>
-  <si>
-    <t>don't think it is developmental stage, more like time datum, differentiation stage</t>
-  </si>
-  <si>
     <t>endothelial cell</t>
   </si>
   <si>
@@ -10441,13 +10423,183 @@
   </si>
   <si>
     <t xml:space="preserve">Do we want to add a shortcut relation in BCGO to replace "produces some transcript and translate_to"? How will we call it, has_transcript_translate_to? </t>
+  </si>
+  <si>
+    <t>is it biological identification objective? Do we need the specific study design type for it? Is transcription profiling design enough?</t>
+  </si>
+  <si>
+    <t>data item / measurement datum</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/REO_0000280</t>
+  </si>
+  <si>
+    <t>Not really used now</t>
+  </si>
+  <si>
+    <t>freezing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">process or planned process, since no objective associated, prefer to define as a subclass of process.
+Can we think quality changes as material transformation? </t>
+  </si>
+  <si>
+    <t>lowess scale group transformation</t>
+  </si>
+  <si>
+    <t>achieves_planned_objective some 'scaling objective'
+'is immediately preceded by' some 'lowess group transformation'</t>
+  </si>
+  <si>
+    <t>Definition in Ontology</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A data transformation consisting in the application of a scale adjustment following a lowess group transformation, to render the group variances similar. </t>
+  </si>
+  <si>
+    <t>spline normalization</t>
+  </si>
+  <si>
+    <t>achieves_planned_objective some 'scaling objective'
+achieves_planned_objective some 'normalization objective'</t>
+  </si>
+  <si>
+    <t>A data transformation re-scales paired-assay data from one data set relative to the other, based on a spline fit of the values in the one set to those in the other, where the latter utilizes either all values in the data set, or an appropriate subset of these (e.g. special control Features on a microarray, or 2DE spots containing constitutively expressed proteins).</t>
+  </si>
+  <si>
+    <t>protocol realized in data transformation, do we need this term? Or just use 'data transformation'.</t>
+  </si>
+  <si>
+    <t>filtering transformation ?</t>
+  </si>
+  <si>
+    <t>define the input of a data transformation?</t>
+  </si>
+  <si>
+    <t>A data transformation applies to part of a dataset.</t>
+  </si>
+  <si>
+    <t>A data transformation applies to part of multiple compatible datasets.</t>
+  </si>
+  <si>
+    <t>Data transformation</t>
+  </si>
+  <si>
+    <t>Submit to IAO tracker? Won't be used in query in near future</t>
+  </si>
+  <si>
+    <t>not quite sure in MO it wants to define a filtering transformation, or a data item (threshold value) used for filtering. Do we want to add data filtering objective, filter value, or threshold value/data?</t>
+  </si>
+  <si>
+    <t>Ontology Term</t>
+  </si>
+  <si>
+    <t>embryonic day 10.5</t>
+  </si>
+  <si>
+    <t>embryonic day 8.5</t>
+  </si>
+  <si>
+    <t>embryonic day 9.5</t>
+  </si>
+  <si>
+    <t>http://purl.oblibrary.org/obo/bcgo/BCGO_0000009</t>
+  </si>
+  <si>
+    <t>http://purl.oblibrary.org/obo/bcgo/BCGO_0000007</t>
+  </si>
+  <si>
+    <t>http://purl.oblibrary.org/obo/bcgo/BCGO_0000008</t>
+  </si>
+  <si>
+    <t>mouse postnatal day 60</t>
+  </si>
+  <si>
+    <t>don't think it is developmental stage, add a class relates to GO:stem cell differentiation (
+http://purl.obolibrary.org/obo/GO_0048863), might need to add D'Amour differentiation protocol or a planned process, add cell differentiation stage?</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/OBI_0001619</t>
+  </si>
+  <si>
+    <t>specimen collection time measurement datum</t>
+  </si>
+  <si>
+    <t>Not quite sure. Specimen collection not always means sampling process</t>
+  </si>
+  <si>
+    <t>fractionation</t>
+  </si>
+  <si>
+    <t>dilution</t>
+  </si>
+  <si>
+    <t>achieves_planned_objective some 'separation into different composition objective'</t>
+  </si>
+  <si>
+    <t>Adapted from MO defintion: A planned process that separates a material into one or more fractions e.g. differential centrifugation or FACS when used for cell sorting (see purify).</t>
+  </si>
+  <si>
+    <t>Don't think MO definition fits what fractionation mean. MO defintion seems like material component separation, might be a defined classes. The definition from wikipedia: a separation process in which a certain quantity of a mixture (solid, liquid, solute, suspension or isotope) is divided up in a number of smaller quantities (fractions) in which the composition varies according to a gradient. eg. as by distillation or crystallization.</t>
+  </si>
+  <si>
+    <t>a planned process that depriving an organism of food or nutrients</t>
+  </si>
+  <si>
+    <t>has_specified_input some organism
+has_specified_output some organism</t>
+  </si>
+  <si>
+    <t>incubation</t>
+  </si>
+  <si>
+    <t>A planned process of placing a material entity under specified conditions e.g. time, temperature, humidity for the purposes of obtaining a different product.</t>
+  </si>
+  <si>
+    <t>does it always generate a different product? How about cell culture?</t>
+  </si>
+  <si>
+    <t>=planned process and has_participant some incubator</t>
+  </si>
+  <si>
+    <t>looks so general, not quite sure how to add the term, the label does not fit its definition.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Study design </t>
+  </si>
+  <si>
+    <t>Process, planned process, quality, etc.</t>
+  </si>
+  <si>
+    <t>study design by technique</t>
+  </si>
+  <si>
+    <t>study design by molecular feature identification</t>
+  </si>
+  <si>
+    <t>has overlapping with other types, like BioMolecularAnnotation, BiologicalProperty</t>
+  </si>
+  <si>
+    <t>study design by organism feature identification</t>
+  </si>
+  <si>
+    <t>study design by cellular feature identification</t>
+  </si>
+  <si>
+    <t>Need to define some study design for organizational purpose, should be defined using N&amp;S.</t>
+  </si>
+  <si>
+    <t>study design by sequence feature identification</t>
+  </si>
+  <si>
+    <t>study design by organism population feature identification</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="11">
+  <fonts count="13">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -10521,6 +10673,18 @@
     </font>
     <font>
       <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF7030A0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -10605,7 +10769,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -10697,6 +10861,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -11099,22 +11267,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L179"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E62" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="4" ySplit="1" topLeftCell="E50" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A69" sqref="A69"/>
+      <selection pane="bottomRight" activeCell="E70" sqref="E70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
+    <col min="1" max="1" width="79.375" customWidth="1"/>
     <col min="2" max="2" width="16.75" customWidth="1"/>
     <col min="3" max="3" width="28.375" customWidth="1"/>
-    <col min="4" max="5" width="56" customWidth="1"/>
-    <col min="6" max="6" width="14.125" customWidth="1"/>
+    <col min="4" max="4" width="36.75" customWidth="1"/>
+    <col min="5" max="5" width="35" customWidth="1"/>
+    <col min="6" max="6" width="40.875" customWidth="1"/>
     <col min="7" max="7" width="19.875" customWidth="1"/>
     <col min="8" max="8" width="26.125" customWidth="1"/>
-    <col min="9" max="9" width="13.25" customWidth="1"/>
+    <col min="9" max="9" width="50.5" customWidth="1"/>
     <col min="10" max="10" width="83.625" customWidth="1"/>
     <col min="11" max="11" width="50.125" customWidth="1"/>
   </cols>
@@ -11145,7 +11315,7 @@
         <v>3324</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>6</v>
+        <v>3470</v>
       </c>
       <c r="J1" s="3" t="s">
         <v>818</v>
@@ -11154,1185 +11324,1110 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
-      <c r="A2" t="s">
-        <v>483</v>
-      </c>
-      <c r="C2" t="s">
-        <v>81</v>
-      </c>
-      <c r="D2" t="s">
-        <v>165</v>
-      </c>
-      <c r="E2" t="s">
-        <v>3332</v>
-      </c>
-      <c r="F2" t="s">
-        <v>3193</v>
-      </c>
-      <c r="G2" t="s">
-        <v>3327</v>
-      </c>
-      <c r="J2" t="s">
-        <v>3326</v>
-      </c>
-      <c r="K2" t="s">
-        <v>484</v>
+    <row r="2" spans="1:11" ht="18.75">
+      <c r="A2" s="46" t="s">
+        <v>3465</v>
       </c>
     </row>
     <row r="3" spans="1:11">
       <c r="A3" t="s">
-        <v>434</v>
+        <v>483</v>
       </c>
       <c r="C3" t="s">
+        <v>81</v>
+      </c>
+      <c r="D3" t="s">
         <v>165</v>
       </c>
-      <c r="D3" t="s">
-        <v>435</v>
-      </c>
       <c r="E3" t="s">
-        <v>3333</v>
+        <v>3332</v>
       </c>
       <c r="F3" t="s">
         <v>3193</v>
       </c>
+      <c r="G3" t="s">
+        <v>3327</v>
+      </c>
       <c r="J3" t="s">
-        <v>3330</v>
+        <v>3326</v>
       </c>
       <c r="K3" t="s">
-        <v>436</v>
+        <v>484</v>
       </c>
     </row>
     <row r="4" spans="1:11">
       <c r="A4" t="s">
-        <v>164</v>
+        <v>434</v>
       </c>
       <c r="C4" t="s">
         <v>165</v>
       </c>
       <c r="D4" t="s">
-        <v>166</v>
+        <v>435</v>
       </c>
       <c r="E4" t="s">
-        <v>3334</v>
+        <v>3333</v>
       </c>
       <c r="F4" t="s">
         <v>3193</v>
       </c>
       <c r="J4" t="s">
-        <v>3328</v>
+        <v>3330</v>
       </c>
       <c r="K4" t="s">
-        <v>167</v>
+        <v>436</v>
       </c>
     </row>
     <row r="5" spans="1:11">
       <c r="A5" t="s">
-        <v>805</v>
+        <v>164</v>
       </c>
       <c r="C5" t="s">
         <v>165</v>
       </c>
       <c r="D5" t="s">
-        <v>806</v>
+        <v>166</v>
       </c>
       <c r="E5" t="s">
-        <v>3335</v>
+        <v>3334</v>
       </c>
       <c r="F5" t="s">
         <v>3193</v>
       </c>
       <c r="J5" t="s">
+        <v>3328</v>
+      </c>
+      <c r="K5" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
+      <c r="A6" t="s">
+        <v>805</v>
+      </c>
+      <c r="C6" t="s">
+        <v>165</v>
+      </c>
+      <c r="D6" t="s">
+        <v>806</v>
+      </c>
+      <c r="E6" t="s">
+        <v>3335</v>
+      </c>
+      <c r="F6" t="s">
+        <v>3193</v>
+      </c>
+      <c r="J6" t="s">
         <v>3329</v>
       </c>
-      <c r="K5" t="s">
+      <c r="K6" t="s">
         <v>807</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="141.75">
-      <c r="B7" t="s">
+    <row r="8" spans="1:11" ht="18.75">
+      <c r="A8" s="46" t="s">
+        <v>3508</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="141.75">
+      <c r="B9" t="s">
         <v>17</v>
-      </c>
-      <c r="C7" t="s">
-        <v>524</v>
-      </c>
-      <c r="D7" t="s">
-        <v>532</v>
-      </c>
-      <c r="E7" t="s">
-        <v>532</v>
-      </c>
-      <c r="F7" t="s">
-        <v>3193</v>
-      </c>
-      <c r="G7" s="41" t="s">
-        <v>3345</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>3340</v>
-      </c>
-      <c r="J7" t="s">
-        <v>3344</v>
-      </c>
-      <c r="K7" t="s">
-        <v>533</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" ht="94.5">
-      <c r="A8" t="s">
-        <v>523</v>
-      </c>
-      <c r="C8" t="s">
-        <v>524</v>
-      </c>
-      <c r="D8" t="s">
-        <v>525</v>
-      </c>
-      <c r="E8" t="s">
-        <v>525</v>
-      </c>
-      <c r="F8" t="s">
-        <v>3193</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>3342</v>
-      </c>
-      <c r="I8" t="s">
-        <v>3341</v>
-      </c>
-      <c r="J8" s="2" t="s">
-        <v>3343</v>
-      </c>
-      <c r="K8" t="s">
-        <v>526</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11">
-      <c r="A9" t="s">
-        <v>581</v>
       </c>
       <c r="C9" t="s">
         <v>524</v>
       </c>
       <c r="D9" t="s">
-        <v>582</v>
+        <v>532</v>
       </c>
       <c r="E9" t="s">
-        <v>3347</v>
+        <v>3466</v>
       </c>
       <c r="F9" t="s">
         <v>3193</v>
       </c>
-      <c r="G9" t="s">
-        <v>3348</v>
-      </c>
-      <c r="H9" t="s">
-        <v>3350</v>
-      </c>
-      <c r="I9" t="s">
-        <v>3349</v>
+      <c r="G9" s="41" t="s">
+        <v>3467</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>3340</v>
+      </c>
+      <c r="J9" t="s">
+        <v>3344</v>
       </c>
       <c r="K9" t="s">
-        <v>583</v>
+        <v>533</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="94.5">
+      <c r="A10" t="s">
+        <v>523</v>
+      </c>
+      <c r="C10" t="s">
+        <v>524</v>
+      </c>
+      <c r="D10" t="s">
+        <v>525</v>
+      </c>
+      <c r="E10" t="s">
+        <v>3496</v>
+      </c>
+      <c r="F10" t="s">
+        <v>3193</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>3342</v>
+      </c>
+      <c r="I10" t="s">
+        <v>3341</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>3343</v>
+      </c>
+      <c r="K10" t="s">
+        <v>526</v>
       </c>
     </row>
     <row r="11" spans="1:11">
       <c r="A11" t="s">
-        <v>764</v>
+        <v>581</v>
       </c>
       <c r="C11" t="s">
-        <v>432</v>
+        <v>524</v>
       </c>
       <c r="D11" t="s">
-        <v>765</v>
+        <v>582</v>
+      </c>
+      <c r="E11" t="s">
+        <v>3346</v>
+      </c>
+      <c r="F11" t="s">
+        <v>3193</v>
       </c>
       <c r="G11" t="s">
-        <v>2069</v>
-      </c>
-      <c r="J11" t="s">
-        <v>3353</v>
+        <v>3347</v>
+      </c>
+      <c r="H11" t="s">
+        <v>3349</v>
+      </c>
+      <c r="I11" t="s">
+        <v>3348</v>
       </c>
       <c r="K11" t="s">
-        <v>766</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="79.5" customHeight="1">
       <c r="A12" t="s">
-        <v>158</v>
+        <v>553</v>
       </c>
       <c r="C12" t="s">
-        <v>70</v>
+        <v>186</v>
       </c>
       <c r="D12" t="s">
-        <v>159</v>
+        <v>555</v>
+      </c>
+      <c r="E12" t="s">
+        <v>3495</v>
+      </c>
+      <c r="F12" t="s">
+        <v>3193</v>
       </c>
       <c r="G12" t="s">
-        <v>2069</v>
+        <v>1190</v>
+      </c>
+      <c r="H12" s="45" t="s">
+        <v>3497</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>3498</v>
+      </c>
+      <c r="J12" s="2" t="s">
+        <v>3499</v>
       </c>
       <c r="K12" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11">
+      <c r="A13" t="s">
+        <v>309</v>
+      </c>
+      <c r="C13" t="s">
+        <v>186</v>
+      </c>
+      <c r="D13" t="s">
+        <v>310</v>
+      </c>
+      <c r="J13" t="s">
+        <v>3506</v>
+      </c>
+      <c r="K13" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="47.25">
       <c r="A14" t="s">
-        <v>641</v>
+        <v>185</v>
       </c>
       <c r="C14" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="D14" t="s">
-        <v>642</v>
+        <v>187</v>
       </c>
       <c r="E14" t="s">
-        <v>3351</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>3352</v>
+        <v>3502</v>
+      </c>
+      <c r="F14" t="s">
+        <v>3193</v>
+      </c>
+      <c r="G14" t="s">
+        <v>1190</v>
+      </c>
+      <c r="H14" s="42" t="s">
+        <v>3505</v>
+      </c>
+      <c r="I14" s="2" t="s">
+        <v>3503</v>
+      </c>
+      <c r="J14" s="2" t="s">
+        <v>3504</v>
       </c>
       <c r="K14" t="s">
-        <v>643</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="63">
       <c r="A15" t="s">
-        <v>348</v>
+        <v>440</v>
       </c>
       <c r="C15" t="s">
-        <v>210</v>
+        <v>186</v>
       </c>
       <c r="D15" t="s">
-        <v>275</v>
+        <v>441</v>
       </c>
       <c r="E15" t="s">
-        <v>3351</v>
-      </c>
-      <c r="J15" t="s">
-        <v>3363</v>
+        <v>441</v>
+      </c>
+      <c r="F15" t="s">
+        <v>3193</v>
+      </c>
+      <c r="G15" t="s">
+        <v>1190</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>3501</v>
+      </c>
+      <c r="I15" t="s">
+        <v>3500</v>
       </c>
       <c r="K15" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11">
-      <c r="A16" t="s">
-        <v>209</v>
-      </c>
-      <c r="C16" t="s">
-        <v>210</v>
-      </c>
-      <c r="D16" t="s">
-        <v>211</v>
-      </c>
-      <c r="E16" t="s">
-        <v>3366</v>
-      </c>
-      <c r="F16" t="s">
-        <v>3367</v>
-      </c>
-      <c r="G16" t="s">
-        <v>3365</v>
-      </c>
-      <c r="I16" t="s">
-        <v>3364</v>
-      </c>
-      <c r="K16" t="s">
-        <v>212</v>
+        <v>442</v>
       </c>
     </row>
     <row r="17" spans="1:11">
       <c r="A17" t="s">
-        <v>465</v>
+        <v>641</v>
       </c>
       <c r="C17" t="s">
-        <v>210</v>
+        <v>183</v>
       </c>
       <c r="D17" t="s">
-        <v>198</v>
+        <v>642</v>
       </c>
       <c r="E17" t="s">
-        <v>3368</v>
-      </c>
-      <c r="F17" t="s">
-        <v>3193</v>
-      </c>
-      <c r="G17" t="s">
-        <v>3369</v>
-      </c>
-      <c r="I17" t="s">
-        <v>3370</v>
+        <v>3350</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>3351</v>
       </c>
       <c r="K17" t="s">
-        <v>466</v>
+        <v>643</v>
       </c>
     </row>
     <row r="18" spans="1:11">
       <c r="A18" t="s">
-        <v>502</v>
+        <v>348</v>
       </c>
       <c r="C18" t="s">
-        <v>44</v>
+        <v>210</v>
       </c>
       <c r="D18" t="s">
-        <v>503</v>
+        <v>275</v>
       </c>
       <c r="E18" t="s">
-        <v>885</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>884</v>
+        <v>3350</v>
+      </c>
+      <c r="J18" t="s">
+        <v>3361</v>
       </c>
       <c r="K18" t="s">
-        <v>504</v>
+        <v>349</v>
       </c>
     </row>
     <row r="19" spans="1:11">
       <c r="A19" t="s">
-        <v>401</v>
+        <v>209</v>
       </c>
       <c r="C19" t="s">
-        <v>44</v>
+        <v>210</v>
       </c>
       <c r="D19" t="s">
-        <v>402</v>
+        <v>211</v>
       </c>
       <c r="E19" t="s">
-        <v>3371</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>3372</v>
+        <v>3364</v>
+      </c>
+      <c r="F19" t="s">
+        <v>3365</v>
+      </c>
+      <c r="G19" t="s">
+        <v>3363</v>
+      </c>
+      <c r="I19" t="s">
+        <v>3362</v>
       </c>
       <c r="K19" t="s">
-        <v>403</v>
+        <v>212</v>
       </c>
     </row>
     <row r="20" spans="1:11">
       <c r="A20" t="s">
-        <v>77</v>
+        <v>465</v>
       </c>
       <c r="C20" t="s">
-        <v>78</v>
+        <v>210</v>
       </c>
       <c r="D20" t="s">
-        <v>79</v>
+        <v>198</v>
       </c>
       <c r="E20" t="s">
-        <v>3405</v>
+        <v>3366</v>
       </c>
       <c r="F20" t="s">
         <v>3193</v>
       </c>
       <c r="G20" t="s">
+        <v>3463</v>
+      </c>
+      <c r="I20" t="s">
+        <v>3367</v>
+      </c>
+      <c r="K20" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11">
+      <c r="A21" t="s">
+        <v>502</v>
+      </c>
+      <c r="C21" t="s">
+        <v>44</v>
+      </c>
+      <c r="D21" t="s">
+        <v>503</v>
+      </c>
+      <c r="E21" t="s">
+        <v>885</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>884</v>
+      </c>
+      <c r="K21" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11">
+      <c r="A22" t="s">
+        <v>401</v>
+      </c>
+      <c r="C22" t="s">
+        <v>44</v>
+      </c>
+      <c r="D22" t="s">
+        <v>402</v>
+      </c>
+      <c r="E22" t="s">
+        <v>3368</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>3369</v>
+      </c>
+      <c r="K22" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11">
+      <c r="A23" t="s">
+        <v>77</v>
+      </c>
+      <c r="C23" t="s">
+        <v>78</v>
+      </c>
+      <c r="D23" t="s">
+        <v>79</v>
+      </c>
+      <c r="E23" t="s">
+        <v>3401</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>3464</v>
+      </c>
+      <c r="G23" t="s">
         <v>954</v>
       </c>
-      <c r="H20" s="42" t="s">
-        <v>3406</v>
-      </c>
-      <c r="K20" t="s">
+      <c r="H23" s="42" t="s">
+        <v>3402</v>
+      </c>
+      <c r="K23" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="22" spans="1:11">
-      <c r="B22" t="s">
-        <v>17</v>
-      </c>
-      <c r="C22" t="s">
-        <v>91</v>
-      </c>
-      <c r="D22" t="s">
-        <v>786</v>
-      </c>
-      <c r="K22" t="s">
-        <v>571</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11">
-      <c r="B23" t="s">
-        <v>17</v>
-      </c>
-      <c r="C23" t="s">
-        <v>91</v>
-      </c>
-      <c r="D23" t="s">
-        <v>787</v>
-      </c>
-      <c r="K23" t="s">
-        <v>788</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11">
-      <c r="B24" t="s">
-        <v>17</v>
-      </c>
+    <row r="24" spans="1:11" ht="47.25">
       <c r="C24" t="s">
-        <v>91</v>
+        <v>15</v>
       </c>
       <c r="D24" t="s">
-        <v>570</v>
+        <v>47</v>
+      </c>
+      <c r="J24" s="2" t="s">
+        <v>3491</v>
       </c>
       <c r="K24" t="s">
-        <v>571</v>
+        <v>48</v>
       </c>
     </row>
     <row r="25" spans="1:11">
-      <c r="B25" t="s">
-        <v>17</v>
-      </c>
       <c r="C25" t="s">
-        <v>91</v>
+        <v>15</v>
       </c>
       <c r="D25" t="s">
-        <v>598</v>
+        <v>655</v>
       </c>
       <c r="K25" t="s">
-        <v>599</v>
+        <v>656</v>
       </c>
     </row>
     <row r="26" spans="1:11">
-      <c r="B26" t="s">
-        <v>17</v>
+      <c r="A26" t="s">
+        <v>520</v>
       </c>
       <c r="C26" t="s">
-        <v>91</v>
+        <v>211</v>
       </c>
       <c r="D26" t="s">
-        <v>799</v>
+        <v>521</v>
+      </c>
+      <c r="E26" t="s">
+        <v>3493</v>
+      </c>
+      <c r="F26" t="s">
+        <v>3492</v>
+      </c>
+      <c r="J26" t="s">
+        <v>3494</v>
       </c>
       <c r="K26" t="s">
-        <v>788</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11">
-      <c r="B27" t="s">
-        <v>17</v>
-      </c>
-      <c r="C27" t="s">
-        <v>91</v>
-      </c>
-      <c r="D27" t="s">
-        <v>675</v>
-      </c>
-      <c r="K27" t="s">
-        <v>599</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11">
-      <c r="B28" t="s">
-        <v>17</v>
-      </c>
-      <c r="C28" t="s">
-        <v>91</v>
-      </c>
-      <c r="D28" t="s">
-        <v>423</v>
-      </c>
-      <c r="K28" t="s">
-        <v>424</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11">
-      <c r="B29" t="s">
-        <v>17</v>
-      </c>
-      <c r="C29" t="s">
-        <v>91</v>
-      </c>
-      <c r="D29" t="s">
-        <v>425</v>
-      </c>
-      <c r="K29" t="s">
-        <v>426</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11">
-      <c r="B30" t="s">
-        <v>17</v>
-      </c>
-      <c r="C30" t="s">
-        <v>91</v>
-      </c>
-      <c r="D30" t="s">
-        <v>531</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11">
-      <c r="B31" t="s">
-        <v>17</v>
-      </c>
-      <c r="C31" t="s">
-        <v>91</v>
-      </c>
-      <c r="D31" t="s">
-        <v>542</v>
-      </c>
-      <c r="K31" t="s">
-        <v>543</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11">
-      <c r="B32" t="s">
-        <v>17</v>
-      </c>
-      <c r="C32" t="s">
-        <v>91</v>
-      </c>
-      <c r="D32" t="s">
-        <v>123</v>
-      </c>
-      <c r="K32" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="33" spans="1:11">
-      <c r="B33" t="s">
-        <v>17</v>
-      </c>
-      <c r="C33" t="s">
-        <v>91</v>
-      </c>
-      <c r="D33" t="s">
-        <v>620</v>
-      </c>
-    </row>
-    <row r="34" spans="1:11">
-      <c r="B34" t="s">
-        <v>17</v>
-      </c>
-      <c r="C34" t="s">
-        <v>91</v>
-      </c>
-      <c r="D34" t="s">
-        <v>481</v>
-      </c>
-      <c r="K34" t="s">
-        <v>482</v>
-      </c>
-    </row>
-    <row r="35" spans="1:11">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" ht="18.75">
+      <c r="A34" s="46" t="s">
+        <v>3480</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" ht="110.25">
       <c r="B35" t="s">
         <v>17</v>
       </c>
       <c r="C35" t="s">
-        <v>91</v>
+        <v>25</v>
       </c>
       <c r="D35" t="s">
-        <v>579</v>
+        <v>407</v>
+      </c>
+      <c r="E35" t="s">
+        <v>3472</v>
+      </c>
+      <c r="F35" t="s">
+        <v>3193</v>
+      </c>
+      <c r="G35" t="s">
+        <v>1908</v>
+      </c>
+      <c r="H35" s="45" t="s">
+        <v>3473</v>
+      </c>
+      <c r="I35" s="2" t="s">
+        <v>3474</v>
+      </c>
+      <c r="K35" t="s">
+        <v>408</v>
       </c>
     </row>
     <row r="36" spans="1:11">
-      <c r="A36" t="s">
-        <v>516</v>
+      <c r="B36" t="s">
+        <v>17</v>
       </c>
       <c r="C36" t="s">
-        <v>91</v>
+        <v>25</v>
       </c>
       <c r="D36" t="s">
-        <v>517</v>
+        <v>779</v>
+      </c>
+      <c r="E36" t="s">
+        <v>1908</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>1909</v>
+      </c>
+      <c r="J36" t="s">
+        <v>3475</v>
+      </c>
+      <c r="K36" t="s">
+        <v>780</v>
       </c>
     </row>
     <row r="37" spans="1:11">
+      <c r="A37" t="s">
+        <v>40</v>
+      </c>
       <c r="C37" t="s">
-        <v>91</v>
+        <v>25</v>
       </c>
       <c r="D37" t="s">
-        <v>576</v>
+        <v>41</v>
+      </c>
+      <c r="F37" t="s">
+        <v>3193</v>
+      </c>
+      <c r="I37" t="s">
+        <v>3479</v>
+      </c>
+      <c r="J37" t="s">
+        <v>3477</v>
       </c>
       <c r="K37" t="s">
-        <v>577</v>
-      </c>
-    </row>
-    <row r="38" spans="1:11">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" ht="31.5">
+      <c r="A38" t="s">
+        <v>303</v>
+      </c>
       <c r="C38" t="s">
-        <v>91</v>
+        <v>25</v>
       </c>
       <c r="D38" t="s">
-        <v>505</v>
+        <v>304</v>
+      </c>
+      <c r="E38" t="s">
+        <v>3476</v>
+      </c>
+      <c r="F38" t="s">
+        <v>3193</v>
+      </c>
+      <c r="G38" t="s">
+        <v>1908</v>
+      </c>
+      <c r="J38" s="2" t="s">
+        <v>3482</v>
       </c>
       <c r="K38" t="s">
-        <v>506</v>
+        <v>305</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" ht="78.75">
+      <c r="A39" t="s">
+        <v>488</v>
+      </c>
+      <c r="C39" t="s">
+        <v>25</v>
+      </c>
+      <c r="D39" t="s">
+        <v>489</v>
+      </c>
+      <c r="E39" t="s">
+        <v>3468</v>
+      </c>
+      <c r="F39" t="s">
+        <v>3193</v>
+      </c>
+      <c r="G39" t="s">
+        <v>1908</v>
+      </c>
+      <c r="H39" s="45" t="s">
+        <v>3469</v>
+      </c>
+      <c r="I39" s="45" t="s">
+        <v>3471</v>
+      </c>
+      <c r="J39" s="1"/>
+      <c r="K39" t="s">
+        <v>490</v>
       </c>
     </row>
     <row r="40" spans="1:11">
-      <c r="B40" t="s">
-        <v>17</v>
+      <c r="A40" t="s">
+        <v>114</v>
       </c>
       <c r="C40" t="s">
         <v>25</v>
       </c>
       <c r="D40" t="s">
-        <v>407</v>
-      </c>
+        <v>115</v>
+      </c>
+      <c r="E40" t="s">
+        <v>1945</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>1946</v>
+      </c>
+      <c r="I40" s="1"/>
+      <c r="J40" s="1"/>
       <c r="K40" t="s">
-        <v>408</v>
+        <v>116</v>
       </c>
     </row>
     <row r="41" spans="1:11">
-      <c r="B41" t="s">
-        <v>17</v>
+      <c r="A41" t="s">
+        <v>332</v>
       </c>
       <c r="C41" t="s">
         <v>25</v>
       </c>
       <c r="D41" t="s">
-        <v>779</v>
+        <v>333</v>
+      </c>
+      <c r="F41" t="s">
+        <v>3193</v>
+      </c>
+      <c r="I41" t="s">
+        <v>3478</v>
+      </c>
+      <c r="J41" t="s">
+        <v>3477</v>
       </c>
       <c r="K41" t="s">
-        <v>780</v>
-      </c>
-    </row>
-    <row r="42" spans="1:11">
-      <c r="A42" t="s">
-        <v>40</v>
-      </c>
-      <c r="C42" t="s">
-        <v>25</v>
-      </c>
-      <c r="D42" t="s">
-        <v>41</v>
-      </c>
-      <c r="K42" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="43" spans="1:11">
-      <c r="A43" t="s">
-        <v>303</v>
-      </c>
-      <c r="C43" t="s">
-        <v>25</v>
-      </c>
-      <c r="D43" t="s">
-        <v>304</v>
-      </c>
-      <c r="K43" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="44" spans="1:11">
-      <c r="A44" t="s">
-        <v>488</v>
-      </c>
-      <c r="C44" t="s">
-        <v>25</v>
-      </c>
-      <c r="D44" t="s">
-        <v>489</v>
-      </c>
-      <c r="F44" t="s">
-        <v>1837</v>
-      </c>
-      <c r="H44" s="1" t="s">
-        <v>1838</v>
-      </c>
-      <c r="I44" s="1"/>
-      <c r="J44" s="1"/>
-      <c r="K44" t="s">
-        <v>490</v>
+        <v>334</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" ht="18.75">
+      <c r="A44" s="46" t="s">
+        <v>3481</v>
       </c>
     </row>
     <row r="45" spans="1:11">
       <c r="A45" t="s">
-        <v>114</v>
+        <v>672</v>
       </c>
       <c r="C45" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="D45" t="s">
-        <v>115</v>
-      </c>
-      <c r="F45" t="s">
-        <v>1945</v>
-      </c>
-      <c r="H45" s="1" t="s">
-        <v>1946</v>
-      </c>
-      <c r="I45" s="1"/>
-      <c r="J45" s="1"/>
+        <v>673</v>
+      </c>
       <c r="K45" t="s">
-        <v>116</v>
+        <v>674</v>
       </c>
     </row>
     <row r="46" spans="1:11">
       <c r="A46" t="s">
-        <v>332</v>
+        <v>63</v>
       </c>
       <c r="C46" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="D46" t="s">
-        <v>333</v>
+        <v>64</v>
       </c>
       <c r="K46" t="s">
-        <v>334</v>
+        <v>65</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11">
+      <c r="A47" t="s">
+        <v>783</v>
+      </c>
+      <c r="C47" t="s">
+        <v>8</v>
+      </c>
+      <c r="D47" t="s">
+        <v>784</v>
+      </c>
+      <c r="K47" t="s">
+        <v>785</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11">
+      <c r="A48" t="s">
+        <v>593</v>
+      </c>
+      <c r="C48" t="s">
+        <v>8</v>
+      </c>
+      <c r="D48" t="s">
+        <v>594</v>
+      </c>
+      <c r="K48" t="s">
+        <v>595</v>
       </c>
     </row>
     <row r="49" spans="1:11">
       <c r="A49" t="s">
-        <v>3409</v>
+        <v>342</v>
+      </c>
+      <c r="C49" t="s">
+        <v>8</v>
+      </c>
+      <c r="D49" t="s">
+        <v>343</v>
+      </c>
+      <c r="K49" t="s">
+        <v>344</v>
       </c>
     </row>
     <row r="50" spans="1:11">
       <c r="A50" t="s">
-        <v>672</v>
+        <v>151</v>
       </c>
       <c r="C50" t="s">
         <v>8</v>
       </c>
       <c r="D50" t="s">
-        <v>673</v>
+        <v>152</v>
       </c>
       <c r="K50" t="s">
-        <v>674</v>
+        <v>153</v>
       </c>
     </row>
     <row r="51" spans="1:11">
       <c r="A51" t="s">
-        <v>63</v>
+        <v>647</v>
       </c>
       <c r="C51" t="s">
         <v>8</v>
       </c>
       <c r="D51" t="s">
-        <v>64</v>
+        <v>648</v>
       </c>
       <c r="K51" t="s">
-        <v>65</v>
+        <v>649</v>
       </c>
     </row>
     <row r="52" spans="1:11">
       <c r="A52" t="s">
-        <v>783</v>
+        <v>776</v>
       </c>
       <c r="C52" t="s">
         <v>8</v>
       </c>
       <c r="D52" t="s">
-        <v>784</v>
+        <v>777</v>
       </c>
       <c r="K52" t="s">
-        <v>785</v>
+        <v>778</v>
       </c>
     </row>
     <row r="53" spans="1:11">
       <c r="A53" t="s">
-        <v>593</v>
+        <v>676</v>
       </c>
       <c r="C53" t="s">
         <v>8</v>
       </c>
       <c r="D53" t="s">
-        <v>594</v>
+        <v>677</v>
       </c>
       <c r="K53" t="s">
-        <v>595</v>
+        <v>678</v>
       </c>
     </row>
     <row r="54" spans="1:11">
       <c r="A54" t="s">
-        <v>342</v>
+        <v>244</v>
       </c>
       <c r="C54" t="s">
         <v>8</v>
       </c>
       <c r="D54" t="s">
-        <v>343</v>
+        <v>245</v>
       </c>
       <c r="K54" t="s">
-        <v>344</v>
+        <v>246</v>
       </c>
     </row>
     <row r="55" spans="1:11">
       <c r="A55" t="s">
-        <v>151</v>
+        <v>277</v>
       </c>
       <c r="C55" t="s">
         <v>8</v>
       </c>
       <c r="D55" t="s">
-        <v>152</v>
+        <v>278</v>
       </c>
       <c r="K55" t="s">
-        <v>153</v>
+        <v>279</v>
       </c>
     </row>
     <row r="56" spans="1:11">
       <c r="A56" t="s">
-        <v>647</v>
+        <v>120</v>
       </c>
       <c r="C56" t="s">
         <v>8</v>
       </c>
       <c r="D56" t="s">
-        <v>648</v>
+        <v>121</v>
       </c>
       <c r="K56" t="s">
-        <v>649</v>
+        <v>122</v>
       </c>
     </row>
     <row r="57" spans="1:11">
       <c r="A57" t="s">
-        <v>776</v>
+        <v>234</v>
       </c>
       <c r="C57" t="s">
         <v>8</v>
       </c>
       <c r="D57" t="s">
-        <v>777</v>
+        <v>235</v>
       </c>
       <c r="K57" t="s">
-        <v>778</v>
-      </c>
-    </row>
-    <row r="58" spans="1:11">
-      <c r="A58" t="s">
-        <v>676</v>
-      </c>
-      <c r="C58" t="s">
-        <v>8</v>
-      </c>
-      <c r="D58" t="s">
-        <v>677</v>
-      </c>
-      <c r="K58" t="s">
-        <v>678</v>
-      </c>
-    </row>
-    <row r="59" spans="1:11">
-      <c r="A59" t="s">
-        <v>244</v>
-      </c>
-      <c r="C59" t="s">
-        <v>8</v>
-      </c>
-      <c r="D59" t="s">
-        <v>245</v>
-      </c>
-      <c r="K59" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="60" spans="1:11">
-      <c r="A60" t="s">
-        <v>277</v>
-      </c>
-      <c r="C60" t="s">
-        <v>8</v>
-      </c>
-      <c r="D60" t="s">
-        <v>278</v>
-      </c>
-      <c r="K60" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="61" spans="1:11">
-      <c r="A61" t="s">
-        <v>120</v>
-      </c>
-      <c r="C61" t="s">
-        <v>8</v>
-      </c>
-      <c r="D61" t="s">
-        <v>121</v>
-      </c>
-      <c r="K61" t="s">
-        <v>122</v>
+        <v>236</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" ht="18.75">
+      <c r="A60" s="46" t="s">
+        <v>3507</v>
+      </c>
+      <c r="E60" t="s">
+        <v>3515</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" ht="18.75">
+      <c r="A61" s="46" t="s">
+        <v>3514</v>
+      </c>
+      <c r="E61" t="s">
+        <v>3512</v>
       </c>
     </row>
     <row r="62" spans="1:11">
       <c r="A62" t="s">
-        <v>234</v>
+        <v>431</v>
       </c>
       <c r="C62" t="s">
-        <v>8</v>
+        <v>69</v>
       </c>
       <c r="D62" t="s">
-        <v>235</v>
+        <v>432</v>
+      </c>
+      <c r="E62" t="s">
+        <v>3513</v>
       </c>
       <c r="K62" t="s">
-        <v>236</v>
+        <v>433</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11">
+      <c r="A63" t="s">
+        <v>68</v>
+      </c>
+      <c r="C63" t="s">
+        <v>69</v>
+      </c>
+      <c r="D63" t="s">
+        <v>70</v>
+      </c>
+      <c r="E63" t="s">
+        <v>3510</v>
+      </c>
+      <c r="K63" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="64" spans="1:11">
-      <c r="B64" t="s">
-        <v>17</v>
+      <c r="A64" t="s">
+        <v>110</v>
       </c>
       <c r="C64" t="s">
-        <v>15</v>
+        <v>69</v>
       </c>
       <c r="D64" t="s">
-        <v>813</v>
+        <v>111</v>
       </c>
       <c r="E64" t="s">
-        <v>3403</v>
-      </c>
-      <c r="F64" s="1" t="s">
-        <v>3404</v>
+        <v>3516</v>
+      </c>
+      <c r="K64" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11">
+      <c r="A65" t="s">
+        <v>146</v>
+      </c>
+      <c r="C65" t="s">
+        <v>69</v>
+      </c>
+      <c r="D65" t="s">
+        <v>57</v>
+      </c>
+      <c r="E65" t="s">
+        <v>3509</v>
+      </c>
+      <c r="K65" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="66" spans="1:11">
+      <c r="A66" t="s">
+        <v>446</v>
+      </c>
       <c r="C66" t="s">
-        <v>15</v>
+        <v>69</v>
       </c>
       <c r="D66" t="s">
-        <v>47</v>
+        <v>447</v>
       </c>
       <c r="J66" t="s">
-        <v>3410</v>
+        <v>3511</v>
       </c>
       <c r="K66" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="67" spans="1:11">
-      <c r="C67" t="s">
-        <v>15</v>
-      </c>
-      <c r="D67" t="s">
-        <v>655</v>
-      </c>
-      <c r="K67" t="s">
-        <v>656</v>
+        <v>448</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11">
+      <c r="A68" t="s">
+        <v>764</v>
+      </c>
+      <c r="C68" t="s">
+        <v>432</v>
+      </c>
+      <c r="D68" t="s">
+        <v>765</v>
+      </c>
+      <c r="G68" t="s">
+        <v>2069</v>
+      </c>
+      <c r="J68" t="s">
+        <v>3462</v>
+      </c>
+      <c r="K68" t="s">
+        <v>766</v>
       </c>
     </row>
     <row r="69" spans="1:11">
       <c r="A69" t="s">
-        <v>520</v>
+        <v>158</v>
       </c>
       <c r="C69" t="s">
-        <v>211</v>
+        <v>70</v>
       </c>
       <c r="D69" t="s">
-        <v>521</v>
+        <v>159</v>
+      </c>
+      <c r="G69" t="s">
+        <v>2069</v>
+      </c>
+      <c r="J69" t="s">
+        <v>3462</v>
       </c>
       <c r="K69" t="s">
-        <v>522</v>
-      </c>
-    </row>
-    <row r="70" spans="1:11">
-      <c r="A70" t="s">
-        <v>633</v>
-      </c>
-      <c r="C70" t="s">
-        <v>192</v>
-      </c>
-      <c r="D70" t="s">
-        <v>182</v>
-      </c>
-      <c r="K70" t="s">
-        <v>634</v>
-      </c>
-    </row>
-    <row r="71" spans="1:11">
-      <c r="A71" t="s">
-        <v>225</v>
-      </c>
-      <c r="C71" t="s">
-        <v>192</v>
-      </c>
-      <c r="D71" t="s">
-        <v>226</v>
-      </c>
-      <c r="K71" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="72" spans="1:11">
-      <c r="A72" t="s">
-        <v>191</v>
-      </c>
-      <c r="C72" t="s">
-        <v>192</v>
-      </c>
-      <c r="D72" t="s">
-        <v>193</v>
-      </c>
-      <c r="K72" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="73" spans="1:11">
-      <c r="A73" t="s">
-        <v>553</v>
-      </c>
-      <c r="B73" t="s">
-        <v>554</v>
-      </c>
-      <c r="C73" t="s">
-        <v>186</v>
-      </c>
-      <c r="D73" t="s">
-        <v>555</v>
-      </c>
-      <c r="K73" t="s">
-        <v>556</v>
-      </c>
-    </row>
-    <row r="74" spans="1:11">
-      <c r="A74" t="s">
-        <v>309</v>
-      </c>
-      <c r="C74" t="s">
-        <v>186</v>
-      </c>
-      <c r="D74" t="s">
-        <v>310</v>
-      </c>
-      <c r="K74" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="75" spans="1:11">
-      <c r="A75" t="s">
-        <v>185</v>
-      </c>
-      <c r="C75" t="s">
-        <v>186</v>
-      </c>
-      <c r="D75" t="s">
-        <v>187</v>
-      </c>
-      <c r="K75" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="76" spans="1:11">
-      <c r="A76" t="s">
-        <v>440</v>
-      </c>
-      <c r="C76" t="s">
-        <v>186</v>
-      </c>
-      <c r="D76" t="s">
-        <v>441</v>
-      </c>
-      <c r="K76" t="s">
-        <v>442</v>
-      </c>
-    </row>
-    <row r="77" spans="1:11">
-      <c r="A77" t="s">
-        <v>431</v>
-      </c>
-      <c r="C77" t="s">
-        <v>69</v>
-      </c>
-      <c r="D77" t="s">
-        <v>432</v>
-      </c>
-      <c r="K77" t="s">
-        <v>433</v>
-      </c>
-    </row>
-    <row r="78" spans="1:11">
-      <c r="A78" t="s">
-        <v>68</v>
-      </c>
-      <c r="C78" t="s">
-        <v>69</v>
-      </c>
-      <c r="D78" t="s">
-        <v>70</v>
-      </c>
-      <c r="K78" t="s">
-        <v>71</v>
+        <v>160</v>
       </c>
     </row>
     <row r="79" spans="1:11">
       <c r="A79" t="s">
-        <v>110</v>
+        <v>507</v>
       </c>
       <c r="C79" t="s">
-        <v>69</v>
+        <v>508</v>
       </c>
       <c r="D79" t="s">
-        <v>111</v>
+        <v>192</v>
       </c>
       <c r="K79" t="s">
-        <v>112</v>
+        <v>509</v>
       </c>
     </row>
     <row r="80" spans="1:11">
       <c r="A80" t="s">
-        <v>146</v>
+        <v>669</v>
       </c>
       <c r="C80" t="s">
-        <v>69</v>
+        <v>508</v>
       </c>
       <c r="D80" t="s">
-        <v>57</v>
+        <v>670</v>
       </c>
       <c r="K80" t="s">
-        <v>147</v>
+        <v>671</v>
       </c>
     </row>
     <row r="81" spans="1:11">
       <c r="A81" t="s">
-        <v>446</v>
+        <v>558</v>
       </c>
       <c r="C81" t="s">
-        <v>69</v>
+        <v>508</v>
       </c>
       <c r="D81" t="s">
-        <v>447</v>
+        <v>559</v>
       </c>
       <c r="K81" t="s">
-        <v>448</v>
+        <v>560</v>
       </c>
     </row>
     <row r="82" spans="1:11">
       <c r="A82" t="s">
-        <v>507</v>
+        <v>657</v>
       </c>
       <c r="C82" t="s">
         <v>508</v>
       </c>
       <c r="D82" t="s">
-        <v>192</v>
+        <v>658</v>
       </c>
       <c r="K82" t="s">
-        <v>509</v>
+        <v>659</v>
       </c>
     </row>
     <row r="83" spans="1:11">
-      <c r="A83" t="s">
-        <v>669</v>
+      <c r="B83" t="s">
+        <v>17</v>
       </c>
       <c r="C83" t="s">
-        <v>508</v>
+        <v>395</v>
       </c>
       <c r="D83" t="s">
-        <v>670</v>
-      </c>
-      <c r="K83" t="s">
-        <v>671</v>
+        <v>397</v>
       </c>
     </row>
     <row r="84" spans="1:11">
-      <c r="A84" t="s">
-        <v>558</v>
+      <c r="B84" t="s">
+        <v>17</v>
       </c>
       <c r="C84" t="s">
-        <v>508</v>
+        <v>395</v>
       </c>
       <c r="D84" t="s">
-        <v>559</v>
-      </c>
-      <c r="K84" t="s">
-        <v>560</v>
+        <v>396</v>
       </c>
     </row>
     <row r="85" spans="1:11">
-      <c r="A85" t="s">
-        <v>657</v>
+      <c r="B85" t="s">
+        <v>17</v>
       </c>
       <c r="C85" t="s">
-        <v>508</v>
+        <v>494</v>
       </c>
       <c r="D85" t="s">
-        <v>658</v>
-      </c>
-      <c r="K85" t="s">
-        <v>659</v>
+        <v>495</v>
       </c>
     </row>
     <row r="86" spans="1:11">
@@ -12340,10 +12435,10 @@
         <v>17</v>
       </c>
       <c r="C86" t="s">
-        <v>395</v>
+        <v>494</v>
       </c>
       <c r="D86" t="s">
-        <v>397</v>
+        <v>609</v>
       </c>
     </row>
     <row r="87" spans="1:11">
@@ -12351,10 +12446,10 @@
         <v>17</v>
       </c>
       <c r="C87" t="s">
-        <v>395</v>
+        <v>494</v>
       </c>
       <c r="D87" t="s">
-        <v>396</v>
+        <v>610</v>
       </c>
     </row>
     <row r="88" spans="1:11">
@@ -12365,18 +12460,21 @@
         <v>494</v>
       </c>
       <c r="D88" t="s">
-        <v>495</v>
+        <v>740</v>
       </c>
     </row>
     <row r="89" spans="1:11">
-      <c r="B89" t="s">
-        <v>17</v>
+      <c r="A89" t="s">
+        <v>377</v>
       </c>
       <c r="C89" t="s">
-        <v>494</v>
+        <v>346</v>
       </c>
       <c r="D89" t="s">
-        <v>609</v>
+        <v>378</v>
+      </c>
+      <c r="K89" t="s">
+        <v>379</v>
       </c>
     </row>
     <row r="90" spans="1:11">
@@ -12384,10 +12482,13 @@
         <v>17</v>
       </c>
       <c r="C90" t="s">
-        <v>494</v>
+        <v>60</v>
       </c>
       <c r="D90" t="s">
-        <v>610</v>
+        <v>242</v>
+      </c>
+      <c r="K90" t="s">
+        <v>243</v>
       </c>
     </row>
     <row r="91" spans="1:11">
@@ -12395,38 +12496,41 @@
         <v>17</v>
       </c>
       <c r="C91" t="s">
-        <v>494</v>
+        <v>60</v>
       </c>
       <c r="D91" t="s">
-        <v>740</v>
+        <v>288</v>
+      </c>
+      <c r="K91" t="s">
+        <v>289</v>
       </c>
     </row>
     <row r="92" spans="1:11">
-      <c r="A92" t="s">
-        <v>377</v>
+      <c r="B92" t="s">
+        <v>17</v>
       </c>
       <c r="C92" t="s">
-        <v>346</v>
+        <v>60</v>
       </c>
       <c r="D92" t="s">
-        <v>378</v>
+        <v>61</v>
       </c>
       <c r="K92" t="s">
-        <v>379</v>
+        <v>62</v>
       </c>
     </row>
     <row r="93" spans="1:11">
-      <c r="B93" t="s">
-        <v>17</v>
+      <c r="A93" t="s">
+        <v>148</v>
       </c>
       <c r="C93" t="s">
         <v>60</v>
       </c>
       <c r="D93" t="s">
-        <v>242</v>
+        <v>149</v>
       </c>
       <c r="K93" t="s">
-        <v>243</v>
+        <v>150</v>
       </c>
     </row>
     <row r="94" spans="1:11">
@@ -12434,41 +12538,38 @@
         <v>17</v>
       </c>
       <c r="C94" t="s">
-        <v>60</v>
+        <v>196</v>
       </c>
       <c r="D94" t="s">
-        <v>288</v>
-      </c>
-      <c r="K94" t="s">
-        <v>289</v>
+        <v>751</v>
       </c>
     </row>
     <row r="95" spans="1:11">
-      <c r="B95" t="s">
+      <c r="A95" t="s">
+        <v>719</v>
+      </c>
+      <c r="C95" t="s">
+        <v>196</v>
+      </c>
+      <c r="D95" t="s">
+        <v>720</v>
+      </c>
+      <c r="K95" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="96" spans="1:11">
+      <c r="B96" t="s">
         <v>17</v>
       </c>
-      <c r="C95" t="s">
-        <v>60</v>
-      </c>
-      <c r="D95" t="s">
-        <v>61</v>
-      </c>
-      <c r="K95" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="96" spans="1:11">
-      <c r="A96" t="s">
-        <v>148</v>
-      </c>
       <c r="C96" t="s">
-        <v>60</v>
+        <v>198</v>
       </c>
       <c r="D96" t="s">
-        <v>149</v>
+        <v>199</v>
       </c>
       <c r="K96" t="s">
-        <v>150</v>
+        <v>200</v>
       </c>
     </row>
     <row r="97" spans="1:11">
@@ -12476,82 +12577,70 @@
         <v>17</v>
       </c>
       <c r="C97" t="s">
-        <v>196</v>
+        <v>32</v>
       </c>
       <c r="D97" t="s">
-        <v>751</v>
+        <v>113</v>
       </c>
     </row>
     <row r="98" spans="1:11">
       <c r="A98" t="s">
-        <v>719</v>
+        <v>811</v>
       </c>
       <c r="C98" t="s">
-        <v>196</v>
+        <v>32</v>
       </c>
       <c r="D98" t="s">
-        <v>720</v>
-      </c>
-      <c r="K98" t="s">
-        <v>721</v>
+        <v>812</v>
       </c>
     </row>
     <row r="99" spans="1:11">
-      <c r="B99" t="s">
-        <v>17</v>
+      <c r="A99" t="s">
+        <v>218</v>
       </c>
       <c r="C99" t="s">
-        <v>198</v>
+        <v>32</v>
       </c>
       <c r="D99" t="s">
-        <v>199</v>
-      </c>
-      <c r="K99" t="s">
-        <v>200</v>
+        <v>219</v>
       </c>
     </row>
     <row r="100" spans="1:11">
-      <c r="B100" t="s">
-        <v>17</v>
+      <c r="A100" t="s">
+        <v>132</v>
       </c>
       <c r="C100" t="s">
         <v>32</v>
       </c>
       <c r="D100" t="s">
-        <v>113</v>
+        <v>133</v>
       </c>
     </row>
     <row r="101" spans="1:11">
-      <c r="A101" t="s">
-        <v>811</v>
-      </c>
       <c r="C101" t="s">
         <v>32</v>
       </c>
       <c r="D101" t="s">
-        <v>812</v>
+        <v>368</v>
       </c>
     </row>
     <row r="102" spans="1:11">
       <c r="A102" t="s">
-        <v>218</v>
+        <v>536</v>
       </c>
       <c r="C102" t="s">
         <v>32</v>
       </c>
       <c r="D102" t="s">
-        <v>219</v>
+        <v>537</v>
       </c>
     </row>
     <row r="103" spans="1:11">
-      <c r="A103" t="s">
-        <v>132</v>
-      </c>
       <c r="C103" t="s">
         <v>32</v>
       </c>
       <c r="D103" t="s">
-        <v>133</v>
+        <v>580</v>
       </c>
     </row>
     <row r="104" spans="1:11">
@@ -12559,18 +12648,15 @@
         <v>32</v>
       </c>
       <c r="D104" t="s">
-        <v>368</v>
+        <v>385</v>
       </c>
     </row>
     <row r="105" spans="1:11">
-      <c r="A105" t="s">
-        <v>536</v>
-      </c>
       <c r="C105" t="s">
         <v>32</v>
       </c>
       <c r="D105" t="s">
-        <v>537</v>
+        <v>635</v>
       </c>
     </row>
     <row r="106" spans="1:11">
@@ -12578,7 +12664,7 @@
         <v>32</v>
       </c>
       <c r="D106" t="s">
-        <v>580</v>
+        <v>473</v>
       </c>
     </row>
     <row r="107" spans="1:11">
@@ -12586,7 +12672,7 @@
         <v>32</v>
       </c>
       <c r="D107" t="s">
-        <v>385</v>
+        <v>117</v>
       </c>
     </row>
     <row r="108" spans="1:11">
@@ -12594,151 +12680,169 @@
         <v>32</v>
       </c>
       <c r="D108" t="s">
-        <v>635</v>
+        <v>650</v>
       </c>
     </row>
     <row r="109" spans="1:11">
+      <c r="A109" t="s">
+        <v>254</v>
+      </c>
       <c r="C109" t="s">
         <v>32</v>
       </c>
       <c r="D109" t="s">
-        <v>473</v>
+        <v>255</v>
       </c>
     </row>
     <row r="110" spans="1:11">
+      <c r="A110" t="s">
+        <v>796</v>
+      </c>
       <c r="C110" t="s">
         <v>32</v>
       </c>
       <c r="D110" t="s">
-        <v>117</v>
+        <v>797</v>
       </c>
     </row>
     <row r="111" spans="1:11">
+      <c r="A111" t="s">
+        <v>264</v>
+      </c>
       <c r="C111" t="s">
-        <v>32</v>
+        <v>265</v>
       </c>
       <c r="D111" t="s">
-        <v>650</v>
+        <v>266</v>
+      </c>
+      <c r="K111" t="s">
+        <v>267</v>
       </c>
     </row>
     <row r="112" spans="1:11">
       <c r="A112" t="s">
-        <v>254</v>
+        <v>23</v>
       </c>
       <c r="C112" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="D112" t="s">
-        <v>255</v>
+        <v>25</v>
+      </c>
+      <c r="K112" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="113" spans="1:11">
       <c r="A113" t="s">
-        <v>796</v>
+        <v>189</v>
       </c>
       <c r="C113" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="D113" t="s">
-        <v>797</v>
+        <v>186</v>
+      </c>
+      <c r="K113" t="s">
+        <v>190</v>
       </c>
     </row>
     <row r="114" spans="1:11">
       <c r="A114" t="s">
-        <v>264</v>
+        <v>144</v>
       </c>
       <c r="C114" t="s">
-        <v>265</v>
+        <v>24</v>
       </c>
       <c r="D114" t="s">
-        <v>266</v>
+        <v>60</v>
       </c>
       <c r="K114" t="s">
-        <v>267</v>
+        <v>145</v>
       </c>
     </row>
     <row r="115" spans="1:11">
       <c r="A115" t="s">
-        <v>23</v>
+        <v>630</v>
       </c>
       <c r="C115" t="s">
-        <v>24</v>
+        <v>108</v>
       </c>
       <c r="D115" t="s">
-        <v>25</v>
+        <v>631</v>
       </c>
       <c r="K115" t="s">
-        <v>26</v>
+        <v>632</v>
       </c>
     </row>
     <row r="116" spans="1:11">
       <c r="A116" t="s">
-        <v>189</v>
+        <v>205</v>
       </c>
       <c r="C116" t="s">
-        <v>24</v>
+        <v>108</v>
       </c>
       <c r="D116" t="s">
-        <v>186</v>
+        <v>206</v>
       </c>
       <c r="K116" t="s">
-        <v>190</v>
+        <v>207</v>
       </c>
     </row>
     <row r="117" spans="1:11">
       <c r="A117" t="s">
-        <v>144</v>
+        <v>362</v>
       </c>
       <c r="C117" t="s">
-        <v>24</v>
+        <v>108</v>
       </c>
       <c r="D117" t="s">
-        <v>60</v>
+        <v>363</v>
       </c>
       <c r="K117" t="s">
-        <v>145</v>
+        <v>364</v>
       </c>
     </row>
     <row r="118" spans="1:11">
-      <c r="A118" t="s">
-        <v>630</v>
+      <c r="B118" t="s">
+        <v>17</v>
       </c>
       <c r="C118" t="s">
-        <v>108</v>
+        <v>12</v>
       </c>
       <c r="D118" t="s">
-        <v>631</v>
+        <v>350</v>
       </c>
       <c r="K118" t="s">
-        <v>632</v>
+        <v>351</v>
       </c>
     </row>
     <row r="119" spans="1:11">
-      <c r="A119" t="s">
-        <v>205</v>
+      <c r="B119" t="s">
+        <v>17</v>
       </c>
       <c r="C119" t="s">
-        <v>108</v>
+        <v>12</v>
       </c>
       <c r="D119" t="s">
-        <v>206</v>
+        <v>388</v>
       </c>
       <c r="K119" t="s">
-        <v>207</v>
+        <v>389</v>
       </c>
     </row>
     <row r="120" spans="1:11">
-      <c r="A120" t="s">
-        <v>362</v>
+      <c r="B120" t="s">
+        <v>17</v>
       </c>
       <c r="C120" t="s">
-        <v>108</v>
+        <v>12</v>
       </c>
       <c r="D120" t="s">
-        <v>363</v>
+        <v>762</v>
       </c>
       <c r="K120" t="s">
-        <v>364</v>
+        <v>763</v>
       </c>
     </row>
     <row r="121" spans="1:11">
@@ -12749,13 +12853,16 @@
         <v>12</v>
       </c>
       <c r="D121" t="s">
-        <v>350</v>
+        <v>476</v>
       </c>
       <c r="K121" t="s">
-        <v>351</v>
+        <v>477</v>
       </c>
     </row>
     <row r="122" spans="1:11">
+      <c r="A122" t="s">
+        <v>644</v>
+      </c>
       <c r="B122" t="s">
         <v>17</v>
       </c>
@@ -12763,13 +12870,13 @@
         <v>12</v>
       </c>
       <c r="D122" t="s">
-        <v>388</v>
-      </c>
-      <c r="K122" t="s">
-        <v>389</v>
+        <v>645</v>
       </c>
     </row>
     <row r="123" spans="1:11">
+      <c r="A123" t="s">
+        <v>268</v>
+      </c>
       <c r="B123" t="s">
         <v>17</v>
       </c>
@@ -12777,13 +12884,13 @@
         <v>12</v>
       </c>
       <c r="D123" t="s">
-        <v>762</v>
-      </c>
-      <c r="K123" t="s">
-        <v>763</v>
+        <v>269</v>
       </c>
     </row>
     <row r="124" spans="1:11">
+      <c r="A124" t="s">
+        <v>268</v>
+      </c>
       <c r="B124" t="s">
         <v>17</v>
       </c>
@@ -12791,16 +12898,10 @@
         <v>12</v>
       </c>
       <c r="D124" t="s">
-        <v>476</v>
-      </c>
-      <c r="K124" t="s">
-        <v>477</v>
+        <v>590</v>
       </c>
     </row>
     <row r="125" spans="1:11">
-      <c r="A125" t="s">
-        <v>644</v>
-      </c>
       <c r="B125" t="s">
         <v>17</v>
       </c>
@@ -12808,13 +12909,13 @@
         <v>12</v>
       </c>
       <c r="D125" t="s">
-        <v>645</v>
+        <v>357</v>
+      </c>
+      <c r="K125" t="s">
+        <v>358</v>
       </c>
     </row>
     <row r="126" spans="1:11">
-      <c r="A126" t="s">
-        <v>268</v>
-      </c>
       <c r="B126" t="s">
         <v>17</v>
       </c>
@@ -12822,13 +12923,13 @@
         <v>12</v>
       </c>
       <c r="D126" t="s">
-        <v>269</v>
+        <v>390</v>
+      </c>
+      <c r="K126" t="s">
+        <v>391</v>
       </c>
     </row>
     <row r="127" spans="1:11">
-      <c r="A127" t="s">
-        <v>268</v>
-      </c>
       <c r="B127" t="s">
         <v>17</v>
       </c>
@@ -12836,7 +12937,10 @@
         <v>12</v>
       </c>
       <c r="D127" t="s">
-        <v>590</v>
+        <v>679</v>
+      </c>
+      <c r="K127" t="s">
+        <v>307</v>
       </c>
     </row>
     <row r="128" spans="1:11">
@@ -12847,10 +12951,10 @@
         <v>12</v>
       </c>
       <c r="D128" t="s">
-        <v>357</v>
+        <v>646</v>
       </c>
       <c r="K128" t="s">
-        <v>358</v>
+        <v>307</v>
       </c>
     </row>
     <row r="129" spans="1:11">
@@ -12861,10 +12965,10 @@
         <v>12</v>
       </c>
       <c r="D129" t="s">
-        <v>390</v>
+        <v>306</v>
       </c>
       <c r="K129" t="s">
-        <v>391</v>
+        <v>307</v>
       </c>
     </row>
     <row r="130" spans="1:11">
@@ -12875,7 +12979,7 @@
         <v>12</v>
       </c>
       <c r="D130" t="s">
-        <v>679</v>
+        <v>381</v>
       </c>
       <c r="K130" t="s">
         <v>307</v>
@@ -12889,10 +12993,7 @@
         <v>12</v>
       </c>
       <c r="D131" t="s">
-        <v>646</v>
-      </c>
-      <c r="K131" t="s">
-        <v>307</v>
+        <v>467</v>
       </c>
     </row>
     <row r="132" spans="1:11">
@@ -12903,10 +13004,7 @@
         <v>12</v>
       </c>
       <c r="D132" t="s">
-        <v>306</v>
-      </c>
-      <c r="K132" t="s">
-        <v>307</v>
+        <v>380</v>
       </c>
     </row>
     <row r="133" spans="1:11">
@@ -12917,10 +13015,10 @@
         <v>12</v>
       </c>
       <c r="D133" t="s">
-        <v>381</v>
+        <v>538</v>
       </c>
       <c r="K133" t="s">
-        <v>307</v>
+        <v>539</v>
       </c>
     </row>
     <row r="134" spans="1:11">
@@ -12931,7 +13029,10 @@
         <v>12</v>
       </c>
       <c r="D134" t="s">
-        <v>467</v>
+        <v>461</v>
+      </c>
+      <c r="K134" t="s">
+        <v>462</v>
       </c>
     </row>
     <row r="135" spans="1:11">
@@ -12942,270 +13043,241 @@
         <v>12</v>
       </c>
       <c r="D135" t="s">
-        <v>380</v>
+        <v>247</v>
+      </c>
+      <c r="K135" t="s">
+        <v>248</v>
       </c>
     </row>
     <row r="136" spans="1:11">
-      <c r="B136" t="s">
-        <v>17</v>
+      <c r="A136" t="s">
+        <v>49</v>
       </c>
       <c r="C136" t="s">
         <v>12</v>
       </c>
       <c r="D136" t="s">
-        <v>538</v>
+        <v>50</v>
       </c>
       <c r="K136" t="s">
-        <v>539</v>
+        <v>51</v>
       </c>
     </row>
     <row r="137" spans="1:11">
-      <c r="B137" t="s">
-        <v>17</v>
+      <c r="A137" t="s">
+        <v>567</v>
       </c>
       <c r="C137" t="s">
         <v>12</v>
       </c>
       <c r="D137" t="s">
-        <v>461</v>
+        <v>568</v>
       </c>
       <c r="K137" t="s">
-        <v>462</v>
+        <v>569</v>
       </c>
     </row>
     <row r="138" spans="1:11">
-      <c r="B138" t="s">
-        <v>17</v>
+      <c r="A138" t="s">
+        <v>717</v>
       </c>
       <c r="C138" t="s">
         <v>12</v>
       </c>
       <c r="D138" t="s">
-        <v>247</v>
-      </c>
-      <c r="K138" t="s">
-        <v>248</v>
+        <v>718</v>
       </c>
     </row>
     <row r="139" spans="1:11">
       <c r="A139" t="s">
-        <v>49</v>
+        <v>755</v>
       </c>
       <c r="C139" t="s">
         <v>12</v>
       </c>
       <c r="D139" t="s">
-        <v>50</v>
+        <v>756</v>
       </c>
       <c r="K139" t="s">
-        <v>51</v>
+        <v>757</v>
       </c>
     </row>
     <row r="140" spans="1:11">
       <c r="A140" t="s">
-        <v>567</v>
+        <v>11</v>
       </c>
       <c r="C140" t="s">
         <v>12</v>
       </c>
       <c r="D140" t="s">
-        <v>568</v>
+        <v>13</v>
       </c>
       <c r="K140" t="s">
-        <v>569</v>
+        <v>14</v>
       </c>
     </row>
     <row r="141" spans="1:11">
       <c r="A141" t="s">
-        <v>717</v>
+        <v>547</v>
       </c>
       <c r="C141" t="s">
         <v>12</v>
       </c>
       <c r="D141" t="s">
-        <v>718</v>
+        <v>548</v>
+      </c>
+      <c r="K141" t="s">
+        <v>549</v>
       </c>
     </row>
     <row r="142" spans="1:11">
-      <c r="A142" t="s">
-        <v>755</v>
-      </c>
       <c r="C142" t="s">
         <v>12</v>
       </c>
       <c r="D142" t="s">
-        <v>756</v>
+        <v>636</v>
       </c>
       <c r="K142" t="s">
-        <v>757</v>
+        <v>636</v>
       </c>
     </row>
     <row r="143" spans="1:11">
       <c r="A143" t="s">
-        <v>11</v>
+        <v>82</v>
       </c>
       <c r="C143" t="s">
         <v>12</v>
       </c>
       <c r="D143" t="s">
-        <v>13</v>
+        <v>83</v>
       </c>
       <c r="K143" t="s">
-        <v>14</v>
+        <v>84</v>
       </c>
     </row>
     <row r="144" spans="1:11">
-      <c r="A144" t="s">
-        <v>547</v>
-      </c>
       <c r="C144" t="s">
         <v>12</v>
       </c>
       <c r="D144" t="s">
-        <v>548</v>
+        <v>319</v>
       </c>
       <c r="K144" t="s">
-        <v>549</v>
+        <v>320</v>
       </c>
     </row>
     <row r="145" spans="1:12">
+      <c r="A145" t="s">
+        <v>705</v>
+      </c>
       <c r="C145" t="s">
         <v>12</v>
       </c>
       <c r="D145" t="s">
-        <v>636</v>
+        <v>706</v>
       </c>
       <c r="K145" t="s">
-        <v>636</v>
+        <v>707</v>
       </c>
     </row>
     <row r="146" spans="1:12">
-      <c r="A146" t="s">
-        <v>82</v>
+      <c r="B146" t="s">
+        <v>17</v>
       </c>
       <c r="C146" t="s">
-        <v>12</v>
+        <v>165</v>
       </c>
       <c r="D146" t="s">
-        <v>83</v>
+        <v>529</v>
       </c>
       <c r="K146" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="147" spans="1:12">
-      <c r="C147" t="s">
-        <v>12</v>
-      </c>
-      <c r="D147" t="s">
-        <v>319</v>
-      </c>
-      <c r="K147" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="148" spans="1:12">
-      <c r="A148" t="s">
-        <v>705</v>
-      </c>
-      <c r="C148" t="s">
-        <v>12</v>
-      </c>
-      <c r="D148" t="s">
-        <v>706</v>
-      </c>
-      <c r="K148" t="s">
-        <v>707</v>
-      </c>
-    </row>
-    <row r="149" spans="1:12">
-      <c r="B149" t="s">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="150" spans="1:12">
+      <c r="A150" t="s">
+        <v>7</v>
+      </c>
+      <c r="C150" t="s">
+        <v>8</v>
+      </c>
+      <c r="D150" t="s">
+        <v>9</v>
+      </c>
+      <c r="F150" t="s">
+        <v>9</v>
+      </c>
+      <c r="H150" t="s">
+        <v>859</v>
+      </c>
+      <c r="K150" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="151" spans="1:12">
+      <c r="B151" t="s">
         <v>17</v>
       </c>
-      <c r="C149" t="s">
-        <v>165</v>
-      </c>
-      <c r="D149" t="s">
-        <v>529</v>
-      </c>
-      <c r="K149" t="s">
-        <v>530</v>
-      </c>
-    </row>
-    <row r="153" spans="1:12">
-      <c r="A153" t="s">
-        <v>7</v>
-      </c>
-      <c r="C153" t="s">
-        <v>8</v>
-      </c>
-      <c r="D153" t="s">
-        <v>9</v>
-      </c>
-      <c r="F153" t="s">
-        <v>9</v>
-      </c>
-      <c r="H153" t="s">
-        <v>859</v>
-      </c>
-      <c r="K153" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="154" spans="1:12">
-      <c r="B154" t="s">
-        <v>17</v>
-      </c>
-      <c r="C154" t="s">
+      <c r="C151" t="s">
         <v>60</v>
       </c>
-      <c r="D154" t="s">
+      <c r="D151" t="s">
         <v>386</v>
       </c>
-      <c r="F154" t="s">
+      <c r="F151" t="s">
         <v>891</v>
       </c>
-      <c r="H154" s="1" t="s">
+      <c r="H151" s="1" t="s">
         <v>889</v>
       </c>
-      <c r="I154" s="1"/>
-      <c r="J154" s="1"/>
-      <c r="K154" t="s">
+      <c r="I151" s="1"/>
+      <c r="J151" s="1"/>
+      <c r="K151" t="s">
         <v>387</v>
       </c>
-      <c r="L154" t="s">
+      <c r="L151" t="s">
         <v>890</v>
       </c>
     </row>
+    <row r="156" spans="1:12">
+      <c r="A156" t="s">
+        <v>2069</v>
+      </c>
+      <c r="B156" t="s">
+        <v>3352</v>
+      </c>
+      <c r="C156" t="s">
+        <v>3291</v>
+      </c>
+    </row>
+    <row r="157" spans="1:12">
+      <c r="B157" t="s">
+        <v>1218</v>
+      </c>
+      <c r="C157" t="s">
+        <v>3353</v>
+      </c>
+    </row>
+    <row r="158" spans="1:12">
+      <c r="B158" t="s">
+        <v>3354</v>
+      </c>
+      <c r="C158" t="s">
+        <v>3355</v>
+      </c>
+    </row>
     <row r="159" spans="1:12">
-      <c r="A159" t="s">
-        <v>2069</v>
-      </c>
-      <c r="B159" t="s">
-        <v>3354</v>
-      </c>
       <c r="C159" t="s">
-        <v>3291</v>
+        <v>3356</v>
       </c>
     </row>
     <row r="160" spans="1:12">
       <c r="B160" t="s">
-        <v>1218</v>
-      </c>
-      <c r="C160" t="s">
-        <v>3355</v>
-      </c>
-    </row>
-    <row r="161" spans="1:11">
-      <c r="B161" t="s">
-        <v>3356</v>
-      </c>
-      <c r="C161" t="s">
         <v>3357</v>
       </c>
     </row>
     <row r="162" spans="1:11">
-      <c r="C162" t="s">
+      <c r="A162" t="s">
         <v>3358</v>
       </c>
     </row>
@@ -13214,184 +13286,216 @@
         <v>3359</v>
       </c>
     </row>
-    <row r="165" spans="1:11">
-      <c r="A165" t="s">
+    <row r="164" spans="1:11">
+      <c r="C164" t="s">
         <v>3360</v>
       </c>
     </row>
-    <row r="166" spans="1:11">
-      <c r="B166" t="s">
-        <v>3361</v>
-      </c>
-    </row>
-    <row r="167" spans="1:11">
-      <c r="C167" t="s">
-        <v>3362</v>
+    <row r="168" spans="1:11">
+      <c r="A168" t="s">
+        <v>3376</v>
+      </c>
+    </row>
+    <row r="169" spans="1:11">
+      <c r="A169" t="s">
+        <v>285</v>
+      </c>
+      <c r="C169" t="s">
+        <v>100</v>
+      </c>
+      <c r="D169" t="s">
+        <v>94</v>
+      </c>
+      <c r="J169" t="s">
+        <v>3345</v>
+      </c>
+      <c r="K169" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="170" spans="1:11">
+      <c r="A170" t="s">
+        <v>771</v>
+      </c>
+      <c r="C170" t="s">
+        <v>664</v>
+      </c>
+      <c r="D170" t="s">
+        <v>772</v>
+      </c>
+      <c r="E170" t="s">
+        <v>3336</v>
+      </c>
+      <c r="F170" s="1" t="s">
+        <v>3337</v>
+      </c>
+      <c r="I170" t="s">
+        <v>3338</v>
+      </c>
+      <c r="J170" t="s">
+        <v>3339</v>
+      </c>
+      <c r="K170" t="s">
+        <v>773</v>
       </c>
     </row>
     <row r="171" spans="1:11">
       <c r="A171" t="s">
-        <v>3379</v>
+        <v>43</v>
+      </c>
+      <c r="C171" t="s">
+        <v>44</v>
+      </c>
+      <c r="D171" t="s">
+        <v>45</v>
+      </c>
+      <c r="E171" t="s">
+        <v>3371</v>
+      </c>
+      <c r="F171" t="s">
+        <v>3370</v>
+      </c>
+      <c r="J171" t="s">
+        <v>3372</v>
+      </c>
+      <c r="K171" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="172" spans="1:11">
       <c r="A172" t="s">
-        <v>285</v>
+        <v>258</v>
       </c>
       <c r="C172" t="s">
-        <v>100</v>
+        <v>259</v>
       </c>
       <c r="D172" t="s">
-        <v>94</v>
-      </c>
-      <c r="J172" t="s">
-        <v>3346</v>
+        <v>260</v>
       </c>
       <c r="K172" t="s">
-        <v>286</v>
+        <v>261</v>
       </c>
     </row>
     <row r="173" spans="1:11">
       <c r="A173" t="s">
-        <v>771</v>
+        <v>316</v>
       </c>
       <c r="C173" t="s">
-        <v>664</v>
+        <v>259</v>
       </c>
       <c r="D173" t="s">
-        <v>772</v>
-      </c>
-      <c r="E173" t="s">
-        <v>3336</v>
-      </c>
-      <c r="F173" s="1" t="s">
-        <v>3337</v>
-      </c>
-      <c r="I173" t="s">
-        <v>3338</v>
-      </c>
-      <c r="J173" t="s">
-        <v>3339</v>
+        <v>317</v>
       </c>
       <c r="K173" t="s">
-        <v>773</v>
+        <v>318</v>
       </c>
     </row>
     <row r="174" spans="1:11">
       <c r="A174" t="s">
-        <v>43</v>
+        <v>392</v>
       </c>
       <c r="C174" t="s">
-        <v>44</v>
+        <v>260</v>
       </c>
       <c r="D174" t="s">
-        <v>45</v>
-      </c>
-      <c r="E174" t="s">
-        <v>3374</v>
-      </c>
-      <c r="F174" t="s">
+        <v>393</v>
+      </c>
+      <c r="G174" t="s">
+        <v>3375</v>
+      </c>
+      <c r="J174" t="s">
         <v>3373</v>
       </c>
-      <c r="J174" t="s">
-        <v>3375</v>
-      </c>
       <c r="K174" t="s">
-        <v>46</v>
+        <v>394</v>
       </c>
     </row>
     <row r="175" spans="1:11">
       <c r="A175" t="s">
-        <v>258</v>
+        <v>468</v>
       </c>
       <c r="C175" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="D175" t="s">
-        <v>260</v>
+        <v>469</v>
+      </c>
+      <c r="G175" t="s">
+        <v>954</v>
+      </c>
+      <c r="J175" t="s">
+        <v>3374</v>
       </c>
       <c r="K175" t="s">
-        <v>261</v>
+        <v>470</v>
       </c>
     </row>
     <row r="176" spans="1:11">
       <c r="A176" t="s">
-        <v>316</v>
+        <v>611</v>
       </c>
       <c r="C176" t="s">
-        <v>259</v>
+        <v>155</v>
       </c>
       <c r="D176" t="s">
-        <v>317</v>
+        <v>612</v>
       </c>
       <c r="K176" t="s">
-        <v>318</v>
+        <v>613</v>
       </c>
     </row>
     <row r="177" spans="1:11">
       <c r="A177" t="s">
-        <v>392</v>
+        <v>633</v>
       </c>
       <c r="C177" t="s">
-        <v>260</v>
+        <v>192</v>
       </c>
       <c r="D177" t="s">
-        <v>393</v>
-      </c>
-      <c r="G177" t="s">
-        <v>3378</v>
-      </c>
-      <c r="J177" t="s">
-        <v>3376</v>
+        <v>182</v>
       </c>
       <c r="K177" t="s">
-        <v>394</v>
+        <v>634</v>
       </c>
     </row>
     <row r="178" spans="1:11">
       <c r="A178" t="s">
-        <v>468</v>
+        <v>225</v>
       </c>
       <c r="C178" t="s">
-        <v>260</v>
+        <v>192</v>
       </c>
       <c r="D178" t="s">
-        <v>469</v>
-      </c>
-      <c r="G178" t="s">
-        <v>954</v>
-      </c>
-      <c r="J178" t="s">
-        <v>3377</v>
+        <v>226</v>
       </c>
       <c r="K178" t="s">
-        <v>470</v>
+        <v>227</v>
       </c>
     </row>
     <row r="179" spans="1:11">
       <c r="A179" t="s">
-        <v>611</v>
+        <v>191</v>
       </c>
       <c r="C179" t="s">
-        <v>155</v>
+        <v>192</v>
       </c>
       <c r="D179" t="s">
-        <v>612</v>
+        <v>193</v>
       </c>
       <c r="K179" t="s">
-        <v>613</v>
+        <v>194</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="H154" r:id="rId1"/>
-    <hyperlink ref="H44" r:id="rId2"/>
-    <hyperlink ref="H45" r:id="rId3"/>
-    <hyperlink ref="F173" r:id="rId4"/>
-    <hyperlink ref="F14" r:id="rId5"/>
-    <hyperlink ref="F18" r:id="rId6"/>
-    <hyperlink ref="F19" r:id="rId7"/>
-    <hyperlink ref="F64" r:id="rId8"/>
+    <hyperlink ref="H151" r:id="rId1"/>
+    <hyperlink ref="F40" r:id="rId2"/>
+    <hyperlink ref="F170" r:id="rId3"/>
+    <hyperlink ref="F17" r:id="rId4"/>
+    <hyperlink ref="F21" r:id="rId5"/>
+    <hyperlink ref="F22" r:id="rId6"/>
+    <hyperlink ref="F23" r:id="rId7"/>
+    <hyperlink ref="F36" r:id="rId8"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" r:id="rId9"/>
@@ -13403,7 +13507,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E54"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
+    <sheetView topLeftCell="A25" workbookViewId="0">
       <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
@@ -13983,11 +14087,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:M69"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="U2" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="4" ySplit="1" topLeftCell="E14" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A17" sqref="A17:XFD19"/>
+      <selection pane="bottomRight" activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -14011,31 +14115,31 @@
         <v>3199</v>
       </c>
       <c r="C1" s="12" t="s">
-        <v>3398</v>
+        <v>3395</v>
       </c>
       <c r="D1" s="12" t="s">
         <v>3331</v>
       </c>
       <c r="E1" s="12" t="s">
+        <v>3385</v>
+      </c>
+      <c r="F1" s="12" t="s">
+        <v>3379</v>
+      </c>
+      <c r="G1" s="12" t="s">
+        <v>3380</v>
+      </c>
+      <c r="H1" s="12" t="s">
+        <v>3381</v>
+      </c>
+      <c r="J1" s="12" t="s">
+        <v>3411</v>
+      </c>
+      <c r="K1" s="12" t="s">
+        <v>3387</v>
+      </c>
+      <c r="L1" s="12" t="s">
         <v>3388</v>
-      </c>
-      <c r="F1" s="12" t="s">
-        <v>3382</v>
-      </c>
-      <c r="G1" s="12" t="s">
-        <v>3383</v>
-      </c>
-      <c r="H1" s="12" t="s">
-        <v>3384</v>
-      </c>
-      <c r="J1" s="12" t="s">
-        <v>3417</v>
-      </c>
-      <c r="K1" s="12" t="s">
-        <v>3390</v>
-      </c>
-      <c r="L1" s="12" t="s">
-        <v>3391</v>
       </c>
       <c r="M1" s="12" t="s">
         <v>818</v>
@@ -14043,26 +14147,26 @@
     </row>
     <row r="2" spans="1:13">
       <c r="A2" s="12" t="s">
-        <v>3448</v>
+        <v>3442</v>
       </c>
       <c r="B2" t="s">
-        <v>3387</v>
+        <v>3384</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" t="s">
-        <v>3448</v>
+        <v>3442</v>
       </c>
       <c r="E2" t="s">
-        <v>3389</v>
+        <v>3386</v>
       </c>
       <c r="H2" t="s">
         <v>2441</v>
       </c>
       <c r="K2" t="s">
-        <v>3450</v>
+        <v>3444</v>
       </c>
       <c r="M2" t="s">
-        <v>3449</v>
+        <v>3443</v>
       </c>
     </row>
     <row r="3" spans="1:13">
@@ -14070,46 +14174,46 @@
         <v>879</v>
       </c>
       <c r="B3" t="s">
-        <v>3387</v>
+        <v>3384</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" t="s">
         <v>879</v>
       </c>
       <c r="E3" t="s">
-        <v>3389</v>
+        <v>3386</v>
       </c>
       <c r="H3" t="s">
         <v>2290</v>
       </c>
       <c r="K3" t="s">
-        <v>3451</v>
+        <v>3445</v>
       </c>
       <c r="M3" t="s">
-        <v>3449</v>
+        <v>3443</v>
       </c>
     </row>
     <row r="4" spans="1:13">
       <c r="A4" s="12" t="s">
-        <v>3424</v>
+        <v>3418</v>
       </c>
       <c r="B4" t="s">
-        <v>3387</v>
+        <v>3384</v>
       </c>
       <c r="D4" t="s">
-        <v>3424</v>
+        <v>3418</v>
       </c>
       <c r="E4" t="s">
         <v>993</v>
       </c>
       <c r="F4" t="s">
-        <v>3380</v>
+        <v>3377</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>3381</v>
+        <v>3378</v>
       </c>
       <c r="K4" t="s">
-        <v>3425</v>
+        <v>3419</v>
       </c>
     </row>
     <row r="5" spans="1:13">
@@ -14117,29 +14221,29 @@
         <v>19</v>
       </c>
       <c r="B5" t="s">
-        <v>3387</v>
+        <v>3384</v>
       </c>
       <c r="D5" t="s">
-        <v>3423</v>
+        <v>3417</v>
       </c>
       <c r="E5" t="s">
-        <v>3389</v>
+        <v>3386</v>
       </c>
       <c r="F5" t="s">
-        <v>3380</v>
+        <v>3377</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>3381</v>
+        <v>3378</v>
       </c>
       <c r="H5" t="s">
-        <v>3386</v>
+        <v>3383</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>3385</v>
+        <v>3382</v>
       </c>
       <c r="J5" s="1"/>
       <c r="K5" t="s">
-        <v>3392</v>
+        <v>3389</v>
       </c>
       <c r="L5" t="s">
         <v>20</v>
@@ -14150,19 +14254,19 @@
         <v>702</v>
       </c>
       <c r="B6" t="s">
-        <v>3387</v>
+        <v>3384</v>
       </c>
       <c r="D6" t="s">
-        <v>3429</v>
+        <v>3423</v>
       </c>
       <c r="E6" t="s">
-        <v>3428</v>
+        <v>3422</v>
       </c>
       <c r="F6" t="s">
-        <v>3380</v>
+        <v>3377</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>3381</v>
+        <v>3378</v>
       </c>
       <c r="H6" t="s">
         <v>2335</v>
@@ -14172,7 +14276,7 @@
       </c>
       <c r="J6" s="1"/>
       <c r="K6" t="s">
-        <v>3436</v>
+        <v>3430</v>
       </c>
     </row>
     <row r="7" spans="1:13">
@@ -14180,54 +14284,54 @@
         <v>216</v>
       </c>
       <c r="B7" t="s">
-        <v>3387</v>
+        <v>3384</v>
       </c>
       <c r="D7" t="s">
-        <v>3427</v>
+        <v>3421</v>
       </c>
       <c r="E7" t="s">
-        <v>3438</v>
+        <v>3432</v>
       </c>
       <c r="F7" t="s">
-        <v>3380</v>
+        <v>3377</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>3381</v>
+        <v>3378</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>3412</v>
+        <v>3406</v>
       </c>
       <c r="J7" s="1"/>
       <c r="K7" t="s">
-        <v>3437</v>
+        <v>3431</v>
       </c>
       <c r="M7" t="s">
-        <v>3422</v>
+        <v>3416</v>
       </c>
     </row>
     <row r="8" spans="1:13">
       <c r="A8" s="12" t="s">
-        <v>3438</v>
+        <v>3432</v>
       </c>
       <c r="B8" t="s">
-        <v>3387</v>
+        <v>3384</v>
       </c>
       <c r="D8" t="s">
-        <v>3438</v>
+        <v>3432</v>
       </c>
       <c r="E8" t="s">
-        <v>3411</v>
+        <v>3405</v>
       </c>
       <c r="G8" s="1"/>
       <c r="H8" t="s">
-        <v>3413</v>
+        <v>3407</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>3412</v>
+        <v>3406</v>
       </c>
       <c r="J8" s="1"/>
       <c r="K8" t="s">
-        <v>3439</v>
+        <v>3433</v>
       </c>
     </row>
     <row r="9" spans="1:13">
@@ -14235,44 +14339,44 @@
         <v>66</v>
       </c>
       <c r="B9" t="s">
-        <v>3387</v>
+        <v>3384</v>
       </c>
       <c r="D9" t="s">
-        <v>3442</v>
+        <v>3436</v>
       </c>
       <c r="E9" t="s">
         <v>1023</v>
       </c>
       <c r="F9" t="s">
-        <v>3394</v>
+        <v>3391</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>3395</v>
+        <v>3392</v>
       </c>
       <c r="H9" t="s">
-        <v>3441</v>
+        <v>3435</v>
       </c>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
       <c r="K9" t="s">
-        <v>3393</v>
+        <v>3390</v>
       </c>
       <c r="L9" t="s">
         <v>67</v>
       </c>
       <c r="M9" t="s">
-        <v>3396</v>
+        <v>3393</v>
       </c>
     </row>
     <row r="10" spans="1:13">
       <c r="A10" s="12" t="s">
-        <v>3441</v>
+        <v>3435</v>
       </c>
       <c r="B10" t="s">
-        <v>3387</v>
+        <v>3384</v>
       </c>
       <c r="D10" t="s">
-        <v>3441</v>
+        <v>3435</v>
       </c>
       <c r="E10" t="s">
         <v>2290</v>
@@ -14281,10 +14385,10 @@
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
       <c r="K10" t="s">
-        <v>3440</v>
+        <v>3434</v>
       </c>
       <c r="M10" t="s">
-        <v>3443</v>
+        <v>3437</v>
       </c>
     </row>
     <row r="11" spans="1:13">
@@ -14292,19 +14396,19 @@
         <v>72</v>
       </c>
       <c r="B11" t="s">
-        <v>3387</v>
+        <v>3384</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>3397</v>
+        <v>3394</v>
       </c>
       <c r="D11" t="s">
-        <v>3426</v>
+        <v>3420</v>
       </c>
       <c r="E11" t="s">
-        <v>3389</v>
+        <v>3386</v>
       </c>
       <c r="K11" t="s">
-        <v>3444</v>
+        <v>3438</v>
       </c>
       <c r="L11" t="s">
         <v>73</v>
@@ -14315,20 +14419,20 @@
         <v>551</v>
       </c>
       <c r="B12" t="s">
-        <v>3461</v>
+        <v>3455</v>
       </c>
       <c r="C12" s="1"/>
       <c r="D12" t="s">
-        <v>3460</v>
+        <v>3454</v>
       </c>
       <c r="E12" t="s">
-        <v>3464</v>
+        <v>3458</v>
       </c>
       <c r="J12" t="s">
-        <v>3462</v>
+        <v>3456</v>
       </c>
       <c r="K12" t="s">
-        <v>3463</v>
+        <v>3457</v>
       </c>
       <c r="L12" t="s">
         <v>552</v>
@@ -14345,27 +14449,27 @@
         <v>76</v>
       </c>
       <c r="B17" t="s">
-        <v>3399</v>
+        <v>3396</v>
       </c>
       <c r="D17" t="s">
-        <v>3418</v>
+        <v>3412</v>
       </c>
       <c r="E17" t="s">
         <v>993</v>
       </c>
       <c r="J17" t="s">
-        <v>3416</v>
+        <v>3410</v>
       </c>
       <c r="L17" t="s">
-        <v>3400</v>
+        <v>3397</v>
       </c>
       <c r="M17" t="s">
-        <v>3401</v>
+        <v>3398</v>
       </c>
     </row>
     <row r="18" spans="1:13">
       <c r="D18" t="s">
-        <v>3419</v>
+        <v>3413</v>
       </c>
     </row>
     <row r="19" spans="1:13">
@@ -14373,7 +14477,7 @@
         <v>98</v>
       </c>
       <c r="M19" t="s">
-        <v>3402</v>
+        <v>3399</v>
       </c>
     </row>
     <row r="25" spans="1:13">
@@ -14453,10 +14557,10 @@
         <v>256</v>
       </c>
       <c r="F35" t="s">
-        <v>3414</v>
+        <v>3408</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>3415</v>
+        <v>3409</v>
       </c>
       <c r="K35" t="s">
         <v>257</v>
@@ -14723,13 +14827,13 @@
     </row>
     <row r="57" spans="1:11">
       <c r="D57" t="s">
-        <v>3420</v>
+        <v>3414</v>
       </c>
       <c r="E57">
         <v>9033</v>
       </c>
       <c r="F57" t="s">
-        <v>3421</v>
+        <v>3415</v>
       </c>
     </row>
     <row r="58" spans="1:11">
@@ -14742,37 +14846,37 @@
     </row>
     <row r="62" spans="1:11">
       <c r="A62" t="s">
-        <v>3430</v>
+        <v>3424</v>
       </c>
     </row>
     <row r="63" spans="1:11">
       <c r="A63" t="s">
-        <v>3433</v>
+        <v>3427</v>
       </c>
     </row>
     <row r="64" spans="1:11">
       <c r="B64" t="s">
-        <v>3431</v>
+        <v>3425</v>
       </c>
     </row>
     <row r="65" spans="1:2">
       <c r="B65" t="s">
-        <v>3432</v>
+        <v>3426</v>
       </c>
     </row>
     <row r="66" spans="1:2">
       <c r="A66" t="s">
-        <v>3435</v>
+        <v>3429</v>
       </c>
     </row>
     <row r="67" spans="1:2">
       <c r="A67" t="s">
-        <v>3434</v>
+        <v>3428</v>
       </c>
     </row>
     <row r="69" spans="1:2">
       <c r="A69" t="s">
-        <v>3467</v>
+        <v>3461</v>
       </c>
     </row>
   </sheetData>
@@ -14800,13 +14904,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N12"/>
+  <dimension ref="A1:N42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="J2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B23" sqref="B23"/>
+      <selection pane="bottomRight" activeCell="B45" sqref="B45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -14825,7 +14929,7 @@
   <sheetData>
     <row r="1" spans="1:14" s="12" customFormat="1">
       <c r="B1" s="12" t="s">
-        <v>3445</v>
+        <v>3439</v>
       </c>
       <c r="C1" s="12" t="s">
         <v>3199</v>
@@ -14834,25 +14938,25 @@
         <v>3331</v>
       </c>
       <c r="E1" s="12" t="s">
-        <v>3388</v>
+        <v>3385</v>
       </c>
       <c r="F1" s="12" t="s">
         <v>1895</v>
       </c>
       <c r="G1" s="12" t="s">
-        <v>3382</v>
+        <v>3379</v>
       </c>
       <c r="H1" s="12" t="s">
+        <v>3441</v>
+      </c>
+      <c r="I1" s="12" t="s">
         <v>3447</v>
       </c>
-      <c r="I1" s="12" t="s">
-        <v>3453</v>
-      </c>
       <c r="J1" s="12" t="s">
-        <v>3390</v>
+        <v>3387</v>
       </c>
       <c r="K1" s="12" t="s">
-        <v>3391</v>
+        <v>3388</v>
       </c>
       <c r="L1" s="12" t="s">
         <v>818</v>
@@ -14869,13 +14973,13 @@
         <v>3253</v>
       </c>
       <c r="E2" t="s">
-        <v>3465</v>
+        <v>3459</v>
       </c>
       <c r="F2" t="s">
+        <v>3440</v>
+      </c>
+      <c r="H2" t="s">
         <v>3446</v>
-      </c>
-      <c r="H2" t="s">
-        <v>3452</v>
       </c>
       <c r="K2" t="s">
         <v>229</v>
@@ -14889,25 +14993,25 @@
         <v>774</v>
       </c>
       <c r="C3" t="s">
-        <v>3387</v>
+        <v>3384</v>
       </c>
       <c r="D3" t="s">
-        <v>3456</v>
+        <v>3450</v>
       </c>
       <c r="E3" t="s">
-        <v>3455</v>
+        <v>3449</v>
       </c>
       <c r="F3" t="s">
+        <v>3440</v>
+      </c>
+      <c r="G3" t="s">
+        <v>3377</v>
+      </c>
+      <c r="H3" t="s">
         <v>3446</v>
       </c>
-      <c r="G3" t="s">
-        <v>3380</v>
-      </c>
-      <c r="H3" t="s">
-        <v>3452</v>
-      </c>
       <c r="I3" s="1" t="s">
-        <v>3454</v>
+        <v>3448</v>
       </c>
       <c r="K3" t="s">
         <v>775</v>
@@ -14921,19 +15025,19 @@
         <v>312</v>
       </c>
       <c r="C4" t="s">
-        <v>3387</v>
+        <v>3384</v>
       </c>
       <c r="D4" t="s">
-        <v>3458</v>
+        <v>3452</v>
       </c>
       <c r="I4" t="s">
-        <v>3459</v>
+        <v>3453</v>
       </c>
       <c r="K4" t="s">
         <v>313</v>
       </c>
       <c r="L4" t="s">
-        <v>3457</v>
+        <v>3451</v>
       </c>
     </row>
     <row r="5" spans="1:14">
@@ -14963,7 +15067,7 @@
         <v>798</v>
       </c>
       <c r="L7" t="s">
-        <v>3466</v>
+        <v>3460</v>
       </c>
     </row>
     <row r="8" spans="1:14">
@@ -14990,27 +15094,27 @@
         <v>76</v>
       </c>
       <c r="C10" t="s">
-        <v>3399</v>
+        <v>3396</v>
       </c>
       <c r="E10" t="s">
-        <v>3418</v>
+        <v>3412</v>
       </c>
       <c r="F10" t="s">
         <v>993</v>
       </c>
       <c r="K10" t="s">
-        <v>3416</v>
+        <v>3410</v>
       </c>
       <c r="M10" t="s">
-        <v>3400</v>
+        <v>3397</v>
       </c>
       <c r="N10" t="s">
-        <v>3401</v>
+        <v>3398</v>
       </c>
     </row>
     <row r="11" spans="1:14">
       <c r="E11" t="s">
-        <v>3419</v>
+        <v>3413</v>
       </c>
     </row>
     <row r="12" spans="1:14">
@@ -15021,7 +15125,227 @@
         <v>98</v>
       </c>
       <c r="N12" t="s">
-        <v>3402</v>
+        <v>3399</v>
+      </c>
+    </row>
+    <row r="26" spans="2:11">
+      <c r="B26" t="s">
+        <v>17</v>
+      </c>
+      <c r="C26" t="s">
+        <v>91</v>
+      </c>
+      <c r="D26" t="s">
+        <v>786</v>
+      </c>
+      <c r="K26" t="s">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="27" spans="2:11">
+      <c r="B27" t="s">
+        <v>17</v>
+      </c>
+      <c r="C27" t="s">
+        <v>91</v>
+      </c>
+      <c r="D27" t="s">
+        <v>787</v>
+      </c>
+      <c r="K27" t="s">
+        <v>788</v>
+      </c>
+    </row>
+    <row r="28" spans="2:11">
+      <c r="B28" t="s">
+        <v>17</v>
+      </c>
+      <c r="C28" t="s">
+        <v>91</v>
+      </c>
+      <c r="D28" t="s">
+        <v>570</v>
+      </c>
+      <c r="K28" t="s">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="29" spans="2:11">
+      <c r="B29" t="s">
+        <v>17</v>
+      </c>
+      <c r="C29" t="s">
+        <v>91</v>
+      </c>
+      <c r="D29" t="s">
+        <v>598</v>
+      </c>
+      <c r="K29" t="s">
+        <v>599</v>
+      </c>
+    </row>
+    <row r="30" spans="2:11">
+      <c r="B30" t="s">
+        <v>17</v>
+      </c>
+      <c r="C30" t="s">
+        <v>91</v>
+      </c>
+      <c r="D30" t="s">
+        <v>799</v>
+      </c>
+      <c r="K30" t="s">
+        <v>788</v>
+      </c>
+    </row>
+    <row r="31" spans="2:11">
+      <c r="B31" t="s">
+        <v>17</v>
+      </c>
+      <c r="C31" t="s">
+        <v>91</v>
+      </c>
+      <c r="D31" t="s">
+        <v>675</v>
+      </c>
+      <c r="K31" t="s">
+        <v>599</v>
+      </c>
+    </row>
+    <row r="32" spans="2:11">
+      <c r="B32" t="s">
+        <v>17</v>
+      </c>
+      <c r="C32" t="s">
+        <v>91</v>
+      </c>
+      <c r="D32" t="s">
+        <v>423</v>
+      </c>
+      <c r="K32" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11">
+      <c r="B33" t="s">
+        <v>17</v>
+      </c>
+      <c r="C33" t="s">
+        <v>91</v>
+      </c>
+      <c r="D33" t="s">
+        <v>425</v>
+      </c>
+      <c r="K33" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11">
+      <c r="B34" t="s">
+        <v>17</v>
+      </c>
+      <c r="C34" t="s">
+        <v>91</v>
+      </c>
+      <c r="D34" t="s">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11">
+      <c r="B35" t="s">
+        <v>17</v>
+      </c>
+      <c r="C35" t="s">
+        <v>91</v>
+      </c>
+      <c r="D35" t="s">
+        <v>542</v>
+      </c>
+      <c r="K35" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11">
+      <c r="B36" t="s">
+        <v>17</v>
+      </c>
+      <c r="C36" t="s">
+        <v>91</v>
+      </c>
+      <c r="D36" t="s">
+        <v>123</v>
+      </c>
+      <c r="K36" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11">
+      <c r="B37" t="s">
+        <v>17</v>
+      </c>
+      <c r="C37" t="s">
+        <v>91</v>
+      </c>
+      <c r="D37" t="s">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11">
+      <c r="B38" t="s">
+        <v>17</v>
+      </c>
+      <c r="C38" t="s">
+        <v>91</v>
+      </c>
+      <c r="D38" t="s">
+        <v>481</v>
+      </c>
+      <c r="K38" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11">
+      <c r="B39" t="s">
+        <v>17</v>
+      </c>
+      <c r="C39" t="s">
+        <v>91</v>
+      </c>
+      <c r="D39" t="s">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11">
+      <c r="A40" t="s">
+        <v>516</v>
+      </c>
+      <c r="C40" t="s">
+        <v>91</v>
+      </c>
+      <c r="D40" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11">
+      <c r="C41" t="s">
+        <v>91</v>
+      </c>
+      <c r="D41" t="s">
+        <v>576</v>
+      </c>
+      <c r="K41" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11">
+      <c r="C42" t="s">
+        <v>91</v>
+      </c>
+      <c r="D42" t="s">
+        <v>505</v>
+      </c>
+      <c r="K42" t="s">
+        <v>506</v>
       </c>
     </row>
   </sheetData>
@@ -15034,9 +15358,133 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:H5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75"/>
+  <cols>
+    <col min="1" max="1" width="13.5" customWidth="1"/>
+    <col min="2" max="2" width="9.875" customWidth="1"/>
+    <col min="3" max="3" width="23.75" customWidth="1"/>
+    <col min="4" max="4" width="16.5" customWidth="1"/>
+    <col min="5" max="5" width="24.75" customWidth="1"/>
+    <col min="6" max="6" width="42.125" customWidth="1"/>
+    <col min="7" max="7" width="18.25" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" s="3" customFormat="1" ht="18.75">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>3483</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>818</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="B2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" t="s">
+        <v>3484</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>3487</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="B3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" t="s">
+        <v>557</v>
+      </c>
+      <c r="E3" t="s">
+        <v>3485</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>3488</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="B4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" t="s">
+        <v>789</v>
+      </c>
+      <c r="E4" t="s">
+        <v>3486</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>3489</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="B5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" t="s">
+        <v>813</v>
+      </c>
+      <c r="E5" t="s">
+        <v>3490</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>3400</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F5" r:id="rId1"/>
+    <hyperlink ref="F2" r:id="rId2"/>
+    <hyperlink ref="F3" r:id="rId3"/>
+    <hyperlink ref="F4" r:id="rId4"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G92"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C76" sqref="C76"/>
     </sheetView>
   </sheetViews>
@@ -16314,13 +16762,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K672"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A49" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D85" sqref="D85"/>
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E81" sqref="E81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -29234,10 +29682,10 @@
         <v>626</v>
       </c>
       <c r="E672" t="s">
-        <v>3408</v>
+        <v>3404</v>
       </c>
       <c r="F672" s="1" t="s">
-        <v>3407</v>
+        <v>3403</v>
       </c>
       <c r="K672" t="s">
         <v>627</v>
@@ -29317,13 +29765,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H188"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D42" sqref="D42"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A86" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D100" sqref="D100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -31845,77 +32293,6 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="0" r:id="rId5"/>
   <headerFooter alignWithMargins="0"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
-  <cols>
-    <col min="1" max="1" width="13.5" customWidth="1"/>
-    <col min="2" max="2" width="9.875" customWidth="1"/>
-    <col min="3" max="3" width="23.75" customWidth="1"/>
-    <col min="4" max="4" width="16.5" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" s="3" customFormat="1" ht="18.75">
-      <c r="A1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>818</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8">
-      <c r="C2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
-      <c r="C3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3" t="s">
-        <v>557</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8">
-      <c r="C4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4" t="s">
-        <v>789</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
worked on mouse strain terms and added some mouse strain in the ontology
</commit_message>
<xml_diff>
--- a/doc/mapping results/termsMapping.xlsx
+++ b/doc/mapping results/termsMapping.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr date1904="1"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="-15" windowWidth="12615" windowHeight="11760" tabRatio="852" activeTab="4"/>
+    <workbookView xWindow="-15" yWindow="-15" windowWidth="12615" windowHeight="11760" tabRatio="852" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="terms2add" sheetId="9" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6307" uniqueCount="3524">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6320" uniqueCount="3535">
   <si>
     <t>MO URI</t>
   </si>
@@ -10616,6 +10616,39 @@
   </si>
   <si>
     <t>scanning software</t>
+  </si>
+  <si>
+    <t>we may need to add following planned process in OBI</t>
+  </si>
+  <si>
+    <t>inbreeding</t>
+  </si>
+  <si>
+    <t>outbreeding</t>
+  </si>
+  <si>
+    <t>crossing</t>
+  </si>
+  <si>
+    <t>C57BL/6J mouse strain</t>
+  </si>
+  <si>
+    <t>http://purl.oblibrary.org/obo/bcgo/BCGO_0000013</t>
+  </si>
+  <si>
+    <t>mouse strain</t>
+  </si>
+  <si>
+    <t>129X1/SvJ mouse strain</t>
+  </si>
+  <si>
+    <t>http://purl.oblibrary.org/obo/bcgo/BCGO_0000028</t>
+  </si>
+  <si>
+    <t>C3H mouse strain</t>
+  </si>
+  <si>
+    <t>http://purl.oblibrary.org/obo/bcgo/BCGO_0000030</t>
   </si>
 </sst>
 </file>
@@ -13057,8 +13090,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -16583,13 +16616,20 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K29"/>
+  <dimension ref="A1:K52"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView topLeftCell="A13" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
+  <cols>
+    <col min="2" max="2" width="21.125" customWidth="1"/>
+    <col min="3" max="3" width="30.25" customWidth="1"/>
+    <col min="4" max="4" width="36.625" customWidth="1"/>
+    <col min="5" max="5" width="19" customWidth="1"/>
+    <col min="6" max="6" width="42.125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:11" s="3" customFormat="1" ht="18.75">
       <c r="A1" s="3" t="s">
@@ -16627,45 +16667,72 @@
       </c>
     </row>
     <row r="2" spans="1:11">
-      <c r="B2" t="s">
-        <v>17</v>
+      <c r="A2" t="s">
+        <v>547</v>
       </c>
       <c r="C2" t="s">
         <v>12</v>
       </c>
       <c r="D2" t="s">
-        <v>350</v>
+        <v>548</v>
+      </c>
+      <c r="E2" t="s">
+        <v>3528</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>3529</v>
+      </c>
+      <c r="G2" t="s">
+        <v>3530</v>
       </c>
       <c r="K2" t="s">
-        <v>351</v>
+        <v>549</v>
       </c>
     </row>
     <row r="3" spans="1:11">
-      <c r="B3" t="s">
-        <v>17</v>
+      <c r="A3" t="s">
+        <v>49</v>
       </c>
       <c r="C3" t="s">
         <v>12</v>
       </c>
       <c r="D3" t="s">
-        <v>388</v>
+        <v>50</v>
+      </c>
+      <c r="E3" t="s">
+        <v>3531</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>3532</v>
+      </c>
+      <c r="G3" t="s">
+        <v>3530</v>
       </c>
       <c r="K3" t="s">
-        <v>389</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:11">
-      <c r="B4" t="s">
-        <v>17</v>
+      <c r="A4" t="s">
+        <v>11</v>
       </c>
       <c r="C4" t="s">
         <v>12</v>
       </c>
       <c r="D4" t="s">
-        <v>762</v>
+        <v>13</v>
+      </c>
+      <c r="E4" t="s">
+        <v>3533</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>3534</v>
+      </c>
+      <c r="G4" t="s">
+        <v>3530</v>
       </c>
       <c r="K4" t="s">
-        <v>763</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:11">
@@ -16676,10 +16743,10 @@
         <v>12</v>
       </c>
       <c r="D5" t="s">
-        <v>476</v>
+        <v>388</v>
       </c>
       <c r="K5" t="s">
-        <v>477</v>
+        <v>389</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -16697,9 +16764,6 @@
       </c>
     </row>
     <row r="7" spans="1:11">
-      <c r="A7" t="s">
-        <v>268</v>
-      </c>
       <c r="B7" t="s">
         <v>17</v>
       </c>
@@ -16707,13 +16771,13 @@
         <v>12</v>
       </c>
       <c r="D7" t="s">
-        <v>269</v>
+        <v>538</v>
+      </c>
+      <c r="K7" t="s">
+        <v>539</v>
       </c>
     </row>
     <row r="8" spans="1:11">
-      <c r="A8" t="s">
-        <v>268</v>
-      </c>
       <c r="B8" t="s">
         <v>17</v>
       </c>
@@ -16721,49 +16785,10 @@
         <v>12</v>
       </c>
       <c r="D8" t="s">
-        <v>590</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11">
-      <c r="B9" t="s">
-        <v>17</v>
-      </c>
-      <c r="C9" t="s">
-        <v>12</v>
-      </c>
-      <c r="D9" t="s">
         <v>357</v>
       </c>
-      <c r="K9" t="s">
+      <c r="K8" t="s">
         <v>358</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11">
-      <c r="B10" t="s">
-        <v>17</v>
-      </c>
-      <c r="C10" t="s">
-        <v>12</v>
-      </c>
-      <c r="D10" t="s">
-        <v>390</v>
-      </c>
-      <c r="K10" t="s">
-        <v>391</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11">
-      <c r="B11" t="s">
-        <v>17</v>
-      </c>
-      <c r="C11" t="s">
-        <v>12</v>
-      </c>
-      <c r="D11" t="s">
-        <v>679</v>
-      </c>
-      <c r="K11" t="s">
-        <v>307</v>
       </c>
     </row>
     <row r="12" spans="1:11">
@@ -16774,10 +16799,10 @@
         <v>12</v>
       </c>
       <c r="D12" t="s">
-        <v>646</v>
+        <v>762</v>
       </c>
       <c r="K12" t="s">
-        <v>307</v>
+        <v>763</v>
       </c>
     </row>
     <row r="13" spans="1:11">
@@ -16788,10 +16813,10 @@
         <v>12</v>
       </c>
       <c r="D13" t="s">
-        <v>306</v>
+        <v>476</v>
       </c>
       <c r="K13" t="s">
-        <v>307</v>
+        <v>477</v>
       </c>
     </row>
     <row r="14" spans="1:11">
@@ -16802,60 +16827,57 @@
         <v>12</v>
       </c>
       <c r="D14" t="s">
-        <v>381</v>
-      </c>
-      <c r="K14" t="s">
-        <v>307</v>
+        <v>380</v>
       </c>
     </row>
     <row r="15" spans="1:11">
-      <c r="B15" t="s">
-        <v>17</v>
+      <c r="A15" t="s">
+        <v>567</v>
       </c>
       <c r="C15" t="s">
         <v>12</v>
       </c>
       <c r="D15" t="s">
-        <v>467</v>
+        <v>568</v>
+      </c>
+      <c r="K15" t="s">
+        <v>569</v>
       </c>
     </row>
     <row r="16" spans="1:11">
-      <c r="B16" t="s">
-        <v>17</v>
+      <c r="A16" t="s">
+        <v>717</v>
       </c>
       <c r="C16" t="s">
         <v>12</v>
       </c>
       <c r="D16" t="s">
-        <v>380</v>
+        <v>718</v>
       </c>
     </row>
     <row r="17" spans="1:11">
-      <c r="B17" t="s">
-        <v>17</v>
+      <c r="A17" t="s">
+        <v>755</v>
       </c>
       <c r="C17" t="s">
         <v>12</v>
       </c>
       <c r="D17" t="s">
-        <v>538</v>
+        <v>756</v>
       </c>
       <c r="K17" t="s">
-        <v>539</v>
+        <v>757</v>
       </c>
     </row>
     <row r="18" spans="1:11">
-      <c r="B18" t="s">
-        <v>17</v>
-      </c>
       <c r="C18" t="s">
         <v>12</v>
       </c>
       <c r="D18" t="s">
-        <v>461</v>
+        <v>636</v>
       </c>
       <c r="K18" t="s">
-        <v>462</v>
+        <v>636</v>
       </c>
     </row>
     <row r="19" spans="1:11">
@@ -16866,144 +16888,214 @@
         <v>12</v>
       </c>
       <c r="D19" t="s">
-        <v>247</v>
+        <v>350</v>
       </c>
       <c r="K19" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11">
-      <c r="A20" t="s">
-        <v>49</v>
-      </c>
-      <c r="C20" t="s">
-        <v>12</v>
-      </c>
-      <c r="D20" t="s">
-        <v>50</v>
-      </c>
-      <c r="K20" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11">
-      <c r="A21" t="s">
-        <v>567</v>
-      </c>
-      <c r="C21" t="s">
-        <v>12</v>
-      </c>
-      <c r="D21" t="s">
-        <v>568</v>
-      </c>
-      <c r="K21" t="s">
-        <v>569</v>
+        <v>351</v>
       </c>
     </row>
     <row r="22" spans="1:11">
       <c r="A22" t="s">
-        <v>717</v>
+        <v>268</v>
+      </c>
+      <c r="B22" t="s">
+        <v>17</v>
       </c>
       <c r="C22" t="s">
         <v>12</v>
       </c>
       <c r="D22" t="s">
-        <v>718</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11">
-      <c r="A23" t="s">
-        <v>755</v>
-      </c>
-      <c r="C23" t="s">
-        <v>12</v>
-      </c>
-      <c r="D23" t="s">
-        <v>756</v>
-      </c>
-      <c r="K23" t="s">
-        <v>757</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11">
-      <c r="A24" t="s">
-        <v>11</v>
-      </c>
-      <c r="C24" t="s">
-        <v>12</v>
-      </c>
-      <c r="D24" t="s">
-        <v>13</v>
-      </c>
-      <c r="K24" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11">
-      <c r="A25" t="s">
-        <v>547</v>
-      </c>
-      <c r="C25" t="s">
-        <v>12</v>
-      </c>
-      <c r="D25" t="s">
-        <v>548</v>
-      </c>
-      <c r="K25" t="s">
-        <v>549</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11">
-      <c r="C26" t="s">
-        <v>12</v>
-      </c>
-      <c r="D26" t="s">
-        <v>636</v>
-      </c>
-      <c r="K26" t="s">
-        <v>636</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11">
-      <c r="A27" t="s">
-        <v>82</v>
-      </c>
-      <c r="C27" t="s">
-        <v>12</v>
-      </c>
-      <c r="D27" t="s">
-        <v>83</v>
-      </c>
-      <c r="K27" t="s">
-        <v>84</v>
+        <v>269</v>
       </c>
     </row>
     <row r="28" spans="1:11">
+      <c r="B28" t="s">
+        <v>17</v>
+      </c>
       <c r="C28" t="s">
         <v>12</v>
       </c>
       <c r="D28" t="s">
-        <v>319</v>
+        <v>306</v>
       </c>
       <c r="K28" t="s">
-        <v>320</v>
+        <v>307</v>
       </c>
     </row>
     <row r="29" spans="1:11">
-      <c r="A29" t="s">
-        <v>705</v>
+      <c r="B29" t="s">
+        <v>17</v>
       </c>
       <c r="C29" t="s">
         <v>12</v>
       </c>
       <c r="D29" t="s">
+        <v>381</v>
+      </c>
+      <c r="K29" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11">
+      <c r="B30" t="s">
+        <v>17</v>
+      </c>
+      <c r="C30" t="s">
+        <v>12</v>
+      </c>
+      <c r="D30" t="s">
+        <v>679</v>
+      </c>
+      <c r="K30" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11">
+      <c r="B31" t="s">
+        <v>17</v>
+      </c>
+      <c r="C31" t="s">
+        <v>12</v>
+      </c>
+      <c r="D31" t="s">
+        <v>646</v>
+      </c>
+      <c r="K31" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11">
+      <c r="B33" t="s">
+        <v>17</v>
+      </c>
+      <c r="C33" t="s">
+        <v>12</v>
+      </c>
+      <c r="D33" t="s">
+        <v>461</v>
+      </c>
+      <c r="K33" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11">
+      <c r="B34" t="s">
+        <v>17</v>
+      </c>
+      <c r="C34" t="s">
+        <v>12</v>
+      </c>
+      <c r="D34" t="s">
+        <v>247</v>
+      </c>
+      <c r="K34" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11">
+      <c r="B35" t="s">
+        <v>17</v>
+      </c>
+      <c r="C35" t="s">
+        <v>12</v>
+      </c>
+      <c r="D35" t="s">
+        <v>390</v>
+      </c>
+      <c r="K35" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11">
+      <c r="A42" t="s">
+        <v>82</v>
+      </c>
+      <c r="C42" t="s">
+        <v>12</v>
+      </c>
+      <c r="D42" t="s">
+        <v>83</v>
+      </c>
+      <c r="K42" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11">
+      <c r="C43" t="s">
+        <v>12</v>
+      </c>
+      <c r="D43" t="s">
+        <v>319</v>
+      </c>
+      <c r="K43" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11">
+      <c r="A44" t="s">
+        <v>705</v>
+      </c>
+      <c r="C44" t="s">
+        <v>12</v>
+      </c>
+      <c r="D44" t="s">
         <v>706</v>
       </c>
-      <c r="K29" t="s">
+      <c r="K44" t="s">
         <v>707</v>
       </c>
     </row>
+    <row r="46" spans="1:11">
+      <c r="B46" t="s">
+        <v>17</v>
+      </c>
+      <c r="C46" t="s">
+        <v>12</v>
+      </c>
+      <c r="D46" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11">
+      <c r="A47" t="s">
+        <v>268</v>
+      </c>
+      <c r="B47" t="s">
+        <v>17</v>
+      </c>
+      <c r="C47" t="s">
+        <v>12</v>
+      </c>
+      <c r="D47" t="s">
+        <v>590</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2">
+      <c r="A49" t="s">
+        <v>3524</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2">
+      <c r="B50" t="s">
+        <v>3525</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2">
+      <c r="B51" t="s">
+        <v>3526</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2">
+      <c r="B52" t="s">
+        <v>3527</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F2" r:id="rId1"/>
+    <hyperlink ref="F3" r:id="rId2"/>
+    <hyperlink ref="F4" r:id="rId3"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -17012,8 +17104,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>

</xml_diff>